<commit_message>
f/mmcdaniel-RASS: Resolve morphine gen error, reorganize sub data
Morphine error in previous commit was caused by replacing ";" with ",".
Re-ordered PD data on CDM so that effect site rate constant and shape
parameter are first, followed by all PD modifiers in alpha order.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -2166,9 +2166,6 @@
     <t>2.4 mL/min kg</t>
   </si>
   <si>
-    <t>6.4;9.5</t>
-  </si>
-  <si>
     <t>Zwitterion</t>
   </si>
   <si>
@@ -2376,238 +2373,241 @@
     <t>4.5 mL/min kg</t>
   </si>
   <si>
-    <t>[-0.25, 0.075 ug/mL]</t>
-  </si>
-  <si>
     <t>[0, 0.7649 ug/mL]</t>
   </si>
   <si>
-    <t>http://link.springer.com/article/10.1007%2FBF00453496?LI=true;https://www.ncbi.nlm.nih.gov/pubmed/3281377?dopt=Abstract</t>
-  </si>
-  <si>
-    <t>[0.3;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>Table on p779 shows bronchi dilate when sympathetically stimulated;baldwin1994comparison shows epi has similar effects to albuterol when inhaled;chose .3 for moderate dilation when in plasma</t>
-  </si>
-  <si>
-    <t>[0;0.0 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0;0.0 ug/L]</t>
-  </si>
-  <si>
-    <t>[1;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.8;0.5 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.25;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.45;100 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.05;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.25;0.0558 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.15;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.45;8 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.25;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.2;0.5549 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.1;0.5 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.15;0.5811 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1;0.3 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.1;5.17 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.45;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.3;0.031 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.4;100 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.01;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.2;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.3;0.0558 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.06;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.15;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.2;0.5549 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.05;0.5811 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.597;60.0 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1.0;0.5549 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1;0.5811 ug/mL]</t>
-  </si>
-  <si>
-    <t>https://www-ncbi-nlm-nih-gov.prox.lib.ncsu.edu/pmc/articles/PMC1357052/pdf/jphysiol01306-0176.pdf;https://www-ncbi-nlm-nih-gov.prox.lib.ncsu.edu/pmc/articles/PMC2466988/pdf/postmedj00350-0007.pdf</t>
-  </si>
-  <si>
-    <t>[0;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.5;0.031 ug/L]</t>
-  </si>
-  <si>
-    <t>This source is a case study;so may not be representative of normal patients</t>
-  </si>
-  <si>
-    <t>[-0.5;4 ug/L]</t>
-  </si>
-  <si>
-    <t>https://www.ncbi.nlm.nih.gov/pubmed/2875674;http://anesthesiology.pubs.asahq.org/article.aspx?articleid=1936490</t>
-  </si>
-  <si>
-    <t>[-0.5;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.5;0.0588 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>Often used to reverse opioid effects;and since opioids affect pupil diameter;it's hard to distinguish naloxone effects</t>
-  </si>
-  <si>
-    <t>[0.5;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1;0.5 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.34;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>guyton2006medical;https://www.ncbi.nlm.nih.gov/pubmed/9715439</t>
-  </si>
-  <si>
-    <t>[0.5;0.031 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.33;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[0;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0;0.0588 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.2;0.031 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.3;100 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.95;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[-1;0.0558 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.5;0.5 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1;0.0558 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.5;0.9 ug/L]</t>
-  </si>
-  <si>
-    <t>[-0.5;100 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.1;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.25;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.5;0.0558 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.1;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.55;0.7649 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.85;100 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.8;0.4462 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1;0.3 ug/L]</t>
-  </si>
-  <si>
-    <t>[1.0;4 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.75;0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.85;0.075 ug/mL]</t>
-  </si>
-  <si>
-    <t>[1.0;0.5 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.0;0.0 ug/L]</t>
-  </si>
-  <si>
-    <t>[0.05;5.17 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.5;0.4 ug/L]</t>
+    <t>[-0.25; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.1007%2FBF00453496?LI=true; https://www.ncbi.nlm.nih.gov/pubmed/3281377?dopt=Abstract</t>
+  </si>
+  <si>
+    <t>6.4; 9.5</t>
+  </si>
+  <si>
+    <t>[0.3; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>Table on p779 shows bronchi dilate when sympathetically stimulated; baldwin1994comparison shows epi has similar effects to albuterol when inhaled; chose .3 for moderate dilation when in plasma</t>
+  </si>
+  <si>
+    <t>[0; 0.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 0.0 ug/L]</t>
+  </si>
+  <si>
+    <t>[1; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.8; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.25; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.45; 100 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.05; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.25; 0.0558 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.15; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.45; 8 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.25; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.2; 0.5549 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.1; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.15; 0.5811 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.3 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.1; 5.17 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.45; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.3; 0.031 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.4; 100 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.01; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.2; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.3; 0.0558 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.06; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.15; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.2; 0.5549 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.05; 0.5811 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.597; 60.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1.0; 0.5549 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.5811 ug/mL]</t>
+  </si>
+  <si>
+    <t>https://www-ncbi-nlm-nih-gov.prox.lib.ncsu.edu/pmc/articles/PMC1357052/pdf/jphysiol01306-0176.pdf; https://www-ncbi-nlm-nih-gov.prox.lib.ncsu.edu/pmc/articles/PMC2466988/pdf/postmedj00350-0007.pdf</t>
+  </si>
+  <si>
+    <t>[0; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.031 ug/L]</t>
+  </si>
+  <si>
+    <t>This source is a case study; so may not be representative of normal patients</t>
+  </si>
+  <si>
+    <t>[-0.5; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/2875674; http://anesthesiology.pubs.asahq.org/article.aspx?articleid=1936490</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.0588 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>Often used to reverse opioid effects; and since opioids affect pupil diameter; it's hard to distinguish naloxone effects</t>
+  </si>
+  <si>
+    <t>[0.5; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.34; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>guyton2006medical; https://www.ncbi.nlm.nih.gov/pubmed/9715439</t>
+  </si>
+  <si>
+    <t>[0.5; 0.031 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.33; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[0; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 0.0588 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.2; 0.031 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.3; 100 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.95; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[-1; 0.0558 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.0558 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.5; 0.9 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.5; 100 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.1; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.25; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.0558 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.1; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.55; 0.7649 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.85; 100 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.8; 0.4462 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 0.3 ug/L]</t>
+  </si>
+  <si>
+    <t>[1.0; 4 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.75; 0.4319 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.85; 0.075 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1.0; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.0; 0.0 ug/L]</t>
+  </si>
+  <si>
+    <t>[0.05; 5.17 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.5; 0.4 ug/L]</t>
   </si>
 </sst>
 </file>
@@ -5558,10 +5558,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="V32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V34" sqref="V34"/>
+      <selection pane="bottomRight" activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6528,7 +6528,7 @@
         <v>165</v>
       </c>
       <c r="BZ2" s="96" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="CA2" s="257" t="s">
         <v>190</v>
@@ -6879,64 +6879,64 @@
         <v>563</v>
       </c>
       <c r="GM2" s="101" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="GN2" s="101" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="GO2" s="101" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="GP2" s="101" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="GQ2" s="101" t="s">
+        <v>739</v>
+      </c>
+      <c r="GR2" s="101" t="s">
+        <v>739</v>
+      </c>
+      <c r="GS2" s="101" t="s">
+        <v>739</v>
+      </c>
+      <c r="GT2" s="101" t="s">
+        <v>739</v>
+      </c>
+      <c r="GU2" s="101" t="s">
+        <v>742</v>
+      </c>
+      <c r="GV2" s="101" t="s">
+        <v>742</v>
+      </c>
+      <c r="GW2" s="101" t="s">
+        <v>742</v>
+      </c>
+      <c r="GX2" s="101" t="s">
+        <v>742</v>
+      </c>
+      <c r="GY2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="GZ2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="HA2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="HB2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="HC2" s="101" t="s">
         <v>740</v>
       </c>
-      <c r="GR2" s="101" t="s">
+      <c r="HD2" s="101" t="s">
         <v>740</v>
       </c>
-      <c r="GS2" s="101" t="s">
+      <c r="HE2" s="101" t="s">
         <v>740</v>
       </c>
-      <c r="GT2" s="101" t="s">
+      <c r="HF2" s="101" t="s">
         <v>740</v>
-      </c>
-      <c r="GU2" s="101" t="s">
-        <v>743</v>
-      </c>
-      <c r="GV2" s="101" t="s">
-        <v>743</v>
-      </c>
-      <c r="GW2" s="101" t="s">
-        <v>743</v>
-      </c>
-      <c r="GX2" s="101" t="s">
-        <v>743</v>
-      </c>
-      <c r="GY2" s="101" t="s">
-        <v>736</v>
-      </c>
-      <c r="GZ2" s="101" t="s">
-        <v>736</v>
-      </c>
-      <c r="HA2" s="101" t="s">
-        <v>736</v>
-      </c>
-      <c r="HB2" s="101" t="s">
-        <v>736</v>
-      </c>
-      <c r="HC2" s="101" t="s">
-        <v>741</v>
-      </c>
-      <c r="HD2" s="101" t="s">
-        <v>741</v>
-      </c>
-      <c r="HE2" s="101" t="s">
-        <v>741</v>
-      </c>
-      <c r="HF2" s="101" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="3" spans="1:214" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -7993,31 +7993,31 @@
       <c r="GK5" s="178"/>
       <c r="GL5" s="178"/>
       <c r="GM5" s="245" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="GN5" s="246"/>
       <c r="GO5" s="246"/>
       <c r="GP5" s="246"/>
       <c r="GQ5" s="245" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="GR5" s="246"/>
       <c r="GS5" s="246"/>
       <c r="GT5" s="246"/>
       <c r="GU5" s="245" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="GV5" s="246"/>
       <c r="GW5" s="246"/>
       <c r="GX5" s="246"/>
       <c r="GY5" s="245" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="GZ5" s="246"/>
       <c r="HA5" s="246"/>
       <c r="HB5" s="246"/>
       <c r="HC5" s="245" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="HD5" s="221"/>
       <c r="HE5" s="221"/>
@@ -8116,7 +8116,7 @@
       <c r="BX6" s="167"/>
       <c r="BY6" s="252"/>
       <c r="BZ6" s="107" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="CA6" s="258" t="s">
         <v>124</v>
@@ -8249,19 +8249,19 @@
       <c r="GS6" s="246"/>
       <c r="GT6" s="246"/>
       <c r="GU6" s="249" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="GV6" s="246"/>
       <c r="GW6" s="246"/>
       <c r="GX6" s="246"/>
       <c r="GY6" s="249" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="GZ6" s="246"/>
       <c r="HA6" s="246"/>
       <c r="HB6" s="246"/>
       <c r="HC6" s="249" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="HD6" s="221"/>
       <c r="HE6" s="221"/>
@@ -9060,7 +9060,7 @@
       <c r="BX10" s="167"/>
       <c r="BY10" s="252"/>
       <c r="BZ10" s="107" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="CA10" s="258" t="s">
         <v>312</v>
@@ -9237,31 +9237,31 @@
       <c r="GK10" s="178"/>
       <c r="GL10" s="178"/>
       <c r="GM10" s="245" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="GN10" s="246"/>
       <c r="GO10" s="246"/>
       <c r="GP10" s="246"/>
       <c r="GQ10" s="245" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="GR10" s="246"/>
       <c r="GS10" s="246"/>
       <c r="GT10" s="246"/>
       <c r="GU10" s="245" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="GV10" s="246"/>
       <c r="GW10" s="246"/>
       <c r="GX10" s="246"/>
       <c r="GY10" s="245" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="GZ10" s="246"/>
       <c r="HA10" s="246"/>
       <c r="HB10" s="246"/>
       <c r="HC10" s="245" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="HD10" s="221"/>
       <c r="HE10" s="221"/>
@@ -12059,7 +12059,7 @@
       <c r="CK20" s="107"/>
       <c r="CL20" s="107"/>
       <c r="CM20" s="107" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="CN20" s="107"/>
       <c r="CO20" s="107"/>
@@ -12071,13 +12071,13 @@
       <c r="CS20" s="107"/>
       <c r="CT20" s="107"/>
       <c r="CU20" s="107" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="CV20" s="107"/>
       <c r="CW20" s="107"/>
       <c r="CX20" s="107"/>
       <c r="CY20" s="107" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="CZ20" s="107"/>
       <c r="DA20" s="107"/>
@@ -12095,7 +12095,7 @@
       <c r="DI20" s="107"/>
       <c r="DJ20" s="107"/>
       <c r="DK20" s="107" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="DL20" s="107"/>
       <c r="DM20" s="107"/>
@@ -12125,13 +12125,13 @@
       <c r="EC20" s="107"/>
       <c r="ED20" s="107"/>
       <c r="EE20" s="107" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="EF20" s="107"/>
       <c r="EG20" s="107"/>
       <c r="EH20" s="107"/>
       <c r="EI20" s="107" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="EJ20" s="107"/>
       <c r="EK20" s="107"/>
@@ -12149,7 +12149,7 @@
       <c r="ES20" s="107"/>
       <c r="ET20" s="107"/>
       <c r="EU20" s="107" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="EV20" s="107"/>
       <c r="EW20" s="107"/>
@@ -12161,7 +12161,7 @@
       <c r="FA20" s="107"/>
       <c r="FB20" s="107"/>
       <c r="FC20" s="107" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="FD20" s="107"/>
       <c r="FE20" s="107"/>
@@ -12312,7 +12312,7 @@
       <c r="BX21" s="167"/>
       <c r="BY21" s="252"/>
       <c r="BZ21" s="107" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="CA21" s="258" t="s">
         <v>528</v>
@@ -12351,7 +12351,7 @@
       <c r="CW21" s="107"/>
       <c r="CX21" s="107"/>
       <c r="CY21" s="107" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="CZ21" s="107"/>
       <c r="DA21" s="107"/>
@@ -12437,7 +12437,7 @@
         <v>656</v>
       </c>
       <c r="EY21" s="107" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="EZ21" s="107"/>
       <c r="FA21" s="107"/>
@@ -12572,7 +12572,7 @@
         <v>591</v>
       </c>
       <c r="AV22" s="162" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="AW22" s="162"/>
       <c r="AX22" s="167"/>
@@ -12627,7 +12627,7 @@
       <c r="CK22" s="107"/>
       <c r="CL22" s="107"/>
       <c r="CM22" s="107" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="CN22" s="107"/>
       <c r="CO22" s="107"/>
@@ -12639,7 +12639,7 @@
       <c r="CS22" s="107"/>
       <c r="CT22" s="107"/>
       <c r="CU22" s="107" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="CV22" s="107"/>
       <c r="CW22" s="107"/>
@@ -12663,13 +12663,13 @@
       <c r="DI22" s="107"/>
       <c r="DJ22" s="107"/>
       <c r="DK22" s="107" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="DL22" s="107"/>
       <c r="DM22" s="107"/>
       <c r="DN22" s="107"/>
       <c r="DO22" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="DP22" s="107"/>
       <c r="DQ22" s="107" t="s">
@@ -12699,13 +12699,13 @@
       <c r="EC22" s="107"/>
       <c r="ED22" s="107"/>
       <c r="EE22" s="107" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="EF22" s="107"/>
       <c r="EG22" s="107"/>
       <c r="EH22" s="107"/>
       <c r="EI22" s="107" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="EJ22" s="107"/>
       <c r="EK22" s="107"/>
@@ -12717,7 +12717,7 @@
       <c r="EO22" s="107"/>
       <c r="EP22" s="107"/>
       <c r="EQ22" s="107" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="ER22" s="107"/>
       <c r="ES22" s="107"/>
@@ -12733,13 +12733,13 @@
         <v>656</v>
       </c>
       <c r="EY22" s="107" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="EZ22" s="107"/>
       <c r="FA22" s="107"/>
       <c r="FB22" s="107"/>
       <c r="FC22" s="107" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="FD22" s="107"/>
       <c r="FE22" s="107"/>
@@ -13372,7 +13372,7 @@
       <c r="BX24" s="167"/>
       <c r="BY24" s="252"/>
       <c r="BZ24" s="107" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="CA24" s="258" t="str">
         <f>CA21</f>
@@ -13607,7 +13607,7 @@
         <v>656</v>
       </c>
       <c r="EY24" s="107" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="EZ24" s="107"/>
       <c r="FA24" s="107"/>
@@ -15201,7 +15201,7 @@
     </row>
     <row r="30" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="79" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B30" s="222"/>
       <c r="C30" s="223" t="s">
@@ -15691,7 +15691,7 @@
     </row>
     <row r="31" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="80" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B31" s="99"/>
       <c r="C31" s="99"/>
@@ -15887,31 +15887,31 @@
       <c r="GK31" s="177"/>
       <c r="GL31" s="177"/>
       <c r="GM31" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GN31" s="245"/>
       <c r="GO31" s="245"/>
       <c r="GP31" s="245"/>
       <c r="GQ31" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GR31" s="245"/>
       <c r="GS31" s="245"/>
       <c r="GT31" s="245"/>
       <c r="GU31" s="245" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="GV31" s="245"/>
       <c r="GW31" s="245"/>
       <c r="GX31" s="245"/>
       <c r="GY31" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GZ31" s="245"/>
       <c r="HA31" s="245"/>
       <c r="HB31" s="245"/>
       <c r="HC31" s="245" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="HD31" s="220"/>
       <c r="HE31" s="220"/>
@@ -15919,7 +15919,7 @@
     </row>
     <row r="32" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="80" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B32" s="99"/>
       <c r="C32" s="99"/>
@@ -16115,31 +16115,31 @@
       <c r="GK32" s="177"/>
       <c r="GL32" s="177"/>
       <c r="GM32" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GN32" s="245"/>
       <c r="GO32" s="245"/>
       <c r="GP32" s="245"/>
       <c r="GQ32" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GR32" s="245"/>
       <c r="GS32" s="245"/>
       <c r="GT32" s="245"/>
       <c r="GU32" s="245" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="GV32" s="245"/>
       <c r="GW32" s="245"/>
       <c r="GX32" s="245"/>
       <c r="GY32" s="245" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="GZ32" s="245"/>
       <c r="HA32" s="245"/>
       <c r="HB32" s="245"/>
       <c r="HC32" s="245" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="HD32" s="220"/>
       <c r="HE32" s="220"/>
@@ -16765,7 +16765,7 @@
       <c r="DE34" s="107"/>
       <c r="DF34" s="107"/>
       <c r="DG34" s="107" t="s">
-        <v>710</v>
+        <v>782</v>
       </c>
       <c r="DH34" s="107"/>
       <c r="DI34" s="107"/>
@@ -17912,7 +17912,7 @@
       <c r="DE38" s="107"/>
       <c r="DF38" s="107"/>
       <c r="DG38" s="107" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DH38" s="107"/>
       <c r="DI38" s="107"/>
@@ -19410,7 +19410,7 @@
       <c r="CK43" s="111"/>
       <c r="CL43" s="111"/>
       <c r="CM43" s="111" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="CN43" s="111"/>
       <c r="CO43" s="111"/>
@@ -19831,8 +19831,8 @@
       <c r="HF44" s="218"/>
     </row>
     <row r="45" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="62" t="s">
-        <v>251</v>
+      <c r="A45" s="157" t="s">
+        <v>704</v>
       </c>
       <c r="B45" s="110"/>
       <c r="C45" s="110"/>
@@ -19847,9 +19847,9 @@
       <c r="L45" s="110"/>
       <c r="M45" s="110"/>
       <c r="N45" s="110"/>
-      <c r="O45" s="110"/>
-      <c r="P45" s="110"/>
-      <c r="Q45" s="110"/>
+      <c r="O45" s="103"/>
+      <c r="P45" s="103"/>
+      <c r="Q45" s="103"/>
       <c r="R45" s="89"/>
       <c r="S45" s="89"/>
       <c r="T45" s="89"/>
@@ -19866,28 +19866,24 @@
       <c r="AE45" s="89"/>
       <c r="AF45" s="89"/>
       <c r="AG45" s="89"/>
-      <c r="AH45" s="89"/>
-      <c r="AI45" s="89"/>
-      <c r="AJ45" s="89"/>
-      <c r="AK45" s="89"/>
+      <c r="AH45" s="90"/>
+      <c r="AI45" s="92"/>
+      <c r="AJ45" s="92"/>
+      <c r="AK45" s="92"/>
       <c r="AL45" s="165" t="s">
-        <v>783</v>
+        <v>711</v>
       </c>
       <c r="AM45" s="162"/>
-      <c r="AN45" s="162" t="s">
-        <v>285</v>
-      </c>
-      <c r="AO45" s="162" t="s">
-        <v>784</v>
-      </c>
+      <c r="AN45" s="162"/>
+      <c r="AO45" s="162"/>
       <c r="AP45" s="162"/>
       <c r="AQ45" s="162"/>
       <c r="AR45" s="162"/>
       <c r="AS45" s="162"/>
       <c r="AT45" s="162"/>
-      <c r="AU45" s="162"/>
-      <c r="AV45" s="162"/>
-      <c r="AW45" s="162"/>
+      <c r="AU45" s="161"/>
+      <c r="AV45" s="161"/>
+      <c r="AW45" s="161"/>
       <c r="AX45" s="167"/>
       <c r="AY45" s="167"/>
       <c r="AZ45" s="167"/>
@@ -19913,136 +19909,136 @@
       <c r="BT45" s="167"/>
       <c r="BU45" s="167"/>
       <c r="BV45" s="167"/>
-      <c r="BW45" s="167"/>
-      <c r="BX45" s="167"/>
-      <c r="BY45" s="252"/>
+      <c r="BW45" s="166"/>
+      <c r="BX45" s="166"/>
+      <c r="BY45" s="250"/>
       <c r="BZ45" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="CA45" s="111" t="s">
-        <v>786</v>
+        <v>711</v>
+      </c>
+      <c r="CA45" s="208" t="s">
+        <v>711</v>
       </c>
       <c r="CB45" s="111"/>
       <c r="CC45" s="111"/>
       <c r="CD45" s="111"/>
       <c r="CE45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="CF45" s="111"/>
       <c r="CG45" s="111"/>
       <c r="CH45" s="111"/>
       <c r="CI45" s="111" t="s">
-        <v>785</v>
+        <v>712</v>
       </c>
       <c r="CJ45" s="111"/>
       <c r="CK45" s="111"/>
       <c r="CL45" s="111"/>
       <c r="CM45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="CN45" s="111"/>
       <c r="CO45" s="111"/>
       <c r="CP45" s="111"/>
       <c r="CQ45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="CR45" s="111"/>
       <c r="CS45" s="111"/>
       <c r="CT45" s="111"/>
       <c r="CU45" s="111" t="s">
-        <v>787</v>
+        <v>711</v>
       </c>
       <c r="CV45" s="111"/>
       <c r="CW45" s="111"/>
       <c r="CX45" s="111"/>
       <c r="CY45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="CZ45" s="111"/>
       <c r="DA45" s="111"/>
       <c r="DB45" s="111"/>
       <c r="DC45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="DD45" s="111"/>
       <c r="DE45" s="111"/>
       <c r="DF45" s="111"/>
       <c r="DG45" s="111" t="s">
-        <v>785</v>
+        <v>712</v>
       </c>
       <c r="DH45" s="111"/>
       <c r="DI45" s="111"/>
       <c r="DJ45" s="111"/>
       <c r="DK45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="DL45" s="111"/>
       <c r="DM45" s="111"/>
       <c r="DN45" s="111"/>
       <c r="DO45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="DP45" s="111"/>
       <c r="DQ45" s="111"/>
       <c r="DR45" s="111"/>
       <c r="DS45" s="111" t="s">
-        <v>785</v>
+        <v>712</v>
       </c>
       <c r="DT45" s="111"/>
       <c r="DU45" s="111"/>
       <c r="DV45" s="111"/>
       <c r="DW45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="DX45" s="111"/>
       <c r="DY45" s="111"/>
       <c r="DZ45" s="111"/>
       <c r="EA45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="EB45" s="111"/>
       <c r="EC45" s="111"/>
       <c r="ED45" s="111"/>
       <c r="EE45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="EF45" s="111"/>
       <c r="EG45" s="111"/>
       <c r="EH45" s="111"/>
       <c r="EI45" s="111" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
       <c r="EJ45" s="111"/>
       <c r="EK45" s="111"/>
       <c r="EL45" s="111"/>
       <c r="EM45" s="111" t="s">
-        <v>788</v>
+        <v>711</v>
       </c>
       <c r="EN45" s="111"/>
       <c r="EO45" s="111"/>
       <c r="EP45" s="111"/>
       <c r="EQ45" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="ER45" s="111"/>
-      <c r="ES45" s="111"/>
-      <c r="ET45" s="111"/>
-      <c r="EU45" s="111"/>
-      <c r="EV45" s="111"/>
-      <c r="EW45" s="111"/>
-      <c r="EX45" s="111"/>
+        <v>711</v>
+      </c>
+      <c r="ER45" s="185"/>
+      <c r="ES45" s="185"/>
+      <c r="ET45" s="185"/>
+      <c r="EU45" s="185"/>
+      <c r="EV45" s="185"/>
+      <c r="EW45" s="185"/>
+      <c r="EX45" s="185"/>
       <c r="EY45" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="EZ45" s="111"/>
-      <c r="FA45" s="111"/>
-      <c r="FB45" s="111"/>
+        <v>711</v>
+      </c>
+      <c r="EZ45" s="185"/>
+      <c r="FA45" s="185"/>
+      <c r="FB45" s="185"/>
       <c r="FC45" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="FD45" s="111"/>
-      <c r="FE45" s="111"/>
-      <c r="FF45" s="111"/>
+        <v>711</v>
+      </c>
+      <c r="FD45" s="185"/>
+      <c r="FE45" s="185"/>
+      <c r="FF45" s="185"/>
       <c r="FG45" s="177"/>
       <c r="FH45" s="177"/>
       <c r="FI45" s="177"/>
@@ -20098,7 +20094,7 @@
     </row>
     <row r="46" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B46" s="110"/>
       <c r="C46" s="110"/>
@@ -20137,11 +20133,15 @@
       <c r="AJ46" s="89"/>
       <c r="AK46" s="89"/>
       <c r="AL46" s="165" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="AM46" s="162"/>
-      <c r="AN46" s="162"/>
-      <c r="AO46" s="162"/>
+      <c r="AN46" s="162" t="s">
+        <v>285</v>
+      </c>
+      <c r="AO46" s="162" t="s">
+        <v>784</v>
+      </c>
       <c r="AP46" s="162"/>
       <c r="AQ46" s="162"/>
       <c r="AR46" s="162"/>
@@ -20188,7 +20188,7 @@
       <c r="CC46" s="111"/>
       <c r="CD46" s="111"/>
       <c r="CE46" s="111" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="CF46" s="111"/>
       <c r="CG46" s="111"/>
@@ -20200,7 +20200,7 @@
       <c r="CK46" s="111"/>
       <c r="CL46" s="111"/>
       <c r="CM46" s="111" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="CN46" s="111"/>
       <c r="CO46" s="111"/>
@@ -20212,19 +20212,19 @@
       <c r="CS46" s="111"/>
       <c r="CT46" s="111"/>
       <c r="CU46" s="111" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="CV46" s="111"/>
       <c r="CW46" s="111"/>
       <c r="CX46" s="111"/>
       <c r="CY46" s="111" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="CZ46" s="111"/>
       <c r="DA46" s="111"/>
       <c r="DB46" s="111"/>
       <c r="DC46" s="111" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="DD46" s="111"/>
       <c r="DE46" s="111"/>
@@ -20242,7 +20242,7 @@
       <c r="DM46" s="111"/>
       <c r="DN46" s="111"/>
       <c r="DO46" s="111" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="DP46" s="111"/>
       <c r="DQ46" s="111"/>
@@ -20266,25 +20266,25 @@
       <c r="EC46" s="111"/>
       <c r="ED46" s="111"/>
       <c r="EE46" s="111" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="EF46" s="111"/>
       <c r="EG46" s="111"/>
       <c r="EH46" s="111"/>
       <c r="EI46" s="111" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
       <c r="EJ46" s="111"/>
       <c r="EK46" s="111"/>
       <c r="EL46" s="111"/>
       <c r="EM46" s="111" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="EN46" s="111"/>
       <c r="EO46" s="111"/>
       <c r="EP46" s="111"/>
       <c r="EQ46" s="111" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="ER46" s="111"/>
       <c r="ES46" s="111"/>
@@ -20300,7 +20300,7 @@
       <c r="FA46" s="111"/>
       <c r="FB46" s="111"/>
       <c r="FC46" s="111" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="FD46" s="111"/>
       <c r="FE46" s="111"/>
@@ -20360,7 +20360,7 @@
     </row>
     <row r="47" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="62" t="s">
-        <v>774</v>
+        <v>571</v>
       </c>
       <c r="B47" s="110"/>
       <c r="C47" s="110"/>
@@ -20375,9 +20375,15 @@
       <c r="L47" s="110"/>
       <c r="M47" s="110"/>
       <c r="N47" s="110"/>
-      <c r="O47" s="110"/>
-      <c r="P47" s="110"/>
-      <c r="Q47" s="110"/>
+      <c r="O47" s="103" t="s">
+        <v>281</v>
+      </c>
+      <c r="P47" s="103" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q47" s="103" t="s">
+        <v>283</v>
+      </c>
       <c r="R47" s="89"/>
       <c r="S47" s="89"/>
       <c r="T47" s="89"/>
@@ -20394,10 +20400,16 @@
       <c r="AE47" s="89"/>
       <c r="AF47" s="89"/>
       <c r="AG47" s="89"/>
-      <c r="AH47" s="89"/>
-      <c r="AI47" s="89"/>
-      <c r="AJ47" s="89"/>
-      <c r="AK47" s="89"/>
+      <c r="AH47" s="90"/>
+      <c r="AI47" s="92" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ47" s="92" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK47" s="92" t="s">
+        <v>283</v>
+      </c>
       <c r="AL47" s="165" t="s">
         <v>786</v>
       </c>
@@ -20409,39 +20421,87 @@
       <c r="AR47" s="162"/>
       <c r="AS47" s="162"/>
       <c r="AT47" s="162"/>
-      <c r="AU47" s="162"/>
-      <c r="AV47" s="162"/>
-      <c r="AW47" s="162"/>
+      <c r="AU47" s="161" t="s">
+        <v>281</v>
+      </c>
+      <c r="AV47" s="161" t="s">
+        <v>282</v>
+      </c>
+      <c r="AW47" s="161" t="s">
+        <v>283</v>
+      </c>
       <c r="AX47" s="167"/>
-      <c r="AY47" s="167"/>
-      <c r="AZ47" s="167"/>
-      <c r="BA47" s="167"/>
+      <c r="AY47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="AZ47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BA47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BB47" s="167"/>
-      <c r="BC47" s="167"/>
-      <c r="BD47" s="167"/>
-      <c r="BE47" s="167"/>
+      <c r="BC47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BD47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BE47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BF47" s="167"/>
-      <c r="BG47" s="167"/>
-      <c r="BH47" s="167"/>
-      <c r="BI47" s="167"/>
+      <c r="BG47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BH47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BI47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BJ47" s="167"/>
-      <c r="BK47" s="167"/>
-      <c r="BL47" s="167"/>
-      <c r="BM47" s="167"/>
+      <c r="BK47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BL47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BM47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BN47" s="167"/>
-      <c r="BO47" s="167"/>
-      <c r="BP47" s="167"/>
-      <c r="BQ47" s="167"/>
+      <c r="BO47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BP47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BQ47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BR47" s="167"/>
-      <c r="BS47" s="167"/>
-      <c r="BT47" s="167"/>
-      <c r="BU47" s="167"/>
+      <c r="BS47" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT47" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BU47" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BV47" s="167"/>
-      <c r="BW47" s="167"/>
-      <c r="BX47" s="167"/>
-      <c r="BY47" s="252"/>
+      <c r="BW47" s="166" t="s">
+        <v>281</v>
+      </c>
+      <c r="BX47" s="166" t="s">
+        <v>282</v>
+      </c>
+      <c r="BY47" s="250" t="s">
+        <v>283</v>
+      </c>
       <c r="BZ47" s="111" t="s">
-        <v>800</v>
+        <v>785</v>
       </c>
       <c r="CA47" s="111" t="s">
         <v>786</v>
@@ -20462,7 +20522,7 @@
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>785</v>
+        <v>851</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
@@ -20474,7 +20534,7 @@
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>785</v>
+        <v>852</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
@@ -20486,7 +20546,7 @@
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>785</v>
+        <v>853</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
@@ -20540,7 +20600,7 @@
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>785</v>
+        <v>854</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
@@ -20622,7 +20682,7 @@
     </row>
     <row r="48" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62" t="s">
-        <v>3</v>
+        <v>252</v>
       </c>
       <c r="B48" s="110"/>
       <c r="C48" s="110"/>
@@ -20661,7 +20721,7 @@
       <c r="AJ48" s="89"/>
       <c r="AK48" s="89"/>
       <c r="AL48" s="165" t="s">
-        <v>801</v>
+        <v>789</v>
       </c>
       <c r="AM48" s="162"/>
       <c r="AN48" s="162"/>
@@ -20705,14 +20765,14 @@
       <c r="BZ48" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA48" s="208" t="s">
-        <v>802</v>
+      <c r="CA48" s="111" t="s">
+        <v>786</v>
       </c>
       <c r="CB48" s="111"/>
       <c r="CC48" s="111"/>
       <c r="CD48" s="111"/>
       <c r="CE48" s="111" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
       <c r="CF48" s="111"/>
       <c r="CG48" s="111"/>
@@ -20724,7 +20784,7 @@
       <c r="CK48" s="111"/>
       <c r="CL48" s="111"/>
       <c r="CM48" s="111" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
       <c r="CN48" s="111"/>
       <c r="CO48" s="111"/>
@@ -20736,19 +20796,19 @@
       <c r="CS48" s="111"/>
       <c r="CT48" s="111"/>
       <c r="CU48" s="111" t="s">
-        <v>805</v>
+        <v>785</v>
       </c>
       <c r="CV48" s="111"/>
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>806</v>
+        <v>792</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>807</v>
+        <v>793</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
@@ -20766,7 +20826,7 @@
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
@@ -20790,13 +20850,13 @@
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>808</v>
+        <v>795</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>809</v>
+        <v>796</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
@@ -20808,7 +20868,7 @@
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>810</v>
+        <v>798</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20816,15 +20876,15 @@
       <c r="EU48" s="111"/>
       <c r="EV48" s="111"/>
       <c r="EW48" s="111"/>
-      <c r="EX48" s="207"/>
+      <c r="EX48" s="111"/>
       <c r="EY48" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="EZ48" s="208"/>
-      <c r="FA48" s="208"/>
-      <c r="FB48" s="208"/>
+      <c r="EZ48" s="111"/>
+      <c r="FA48" s="111"/>
+      <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>785</v>
+        <v>799</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -20884,7 +20944,7 @@
     </row>
     <row r="49" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="62" t="s">
-        <v>696</v>
+        <v>773</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="110"/>
@@ -20965,7 +21025,7 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>785</v>
+        <v>800</v>
       </c>
       <c r="CA49" s="111" t="s">
         <v>786</v>
@@ -21080,7 +21140,7 @@
       <c r="EW49" s="111"/>
       <c r="EX49" s="207"/>
       <c r="EY49" s="111" t="s">
-        <v>811</v>
+        <v>785</v>
       </c>
       <c r="EZ49" s="208"/>
       <c r="FA49" s="208"/>
@@ -21146,7 +21206,7 @@
     </row>
     <row r="50" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="62" t="s">
-        <v>253</v>
+        <v>3</v>
       </c>
       <c r="B50" s="110"/>
       <c r="C50" s="110"/>
@@ -21185,7 +21245,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>786</v>
+        <v>801</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21229,14 +21289,14 @@
       <c r="BZ50" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA50" s="111" t="s">
-        <v>786</v>
+      <c r="CA50" s="208" t="s">
+        <v>802</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>785</v>
+        <v>803</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
@@ -21248,7 +21308,7 @@
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>785</v>
+        <v>804</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
@@ -21260,19 +21320,19 @@
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>785</v>
+        <v>805</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>785</v>
+        <v>806</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>785</v>
+        <v>807</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
@@ -21314,25 +21374,25 @@
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21408,7 +21468,7 @@
     </row>
     <row r="51" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="62" t="s">
-        <v>543</v>
+        <v>696</v>
       </c>
       <c r="B51" s="110"/>
       <c r="C51" s="110"/>
@@ -21416,12 +21476,8 @@
       <c r="E51" s="110"/>
       <c r="F51" s="110"/>
       <c r="G51" s="110"/>
-      <c r="H51" s="110" t="s">
-        <v>814</v>
-      </c>
-      <c r="I51" s="110" t="s">
-        <v>545</v>
-      </c>
+      <c r="H51" s="110"/>
+      <c r="I51" s="110"/>
       <c r="J51" s="110"/>
       <c r="K51" s="110"/>
       <c r="L51" s="110"/>
@@ -21451,7 +21507,7 @@
       <c r="AJ51" s="89"/>
       <c r="AK51" s="89"/>
       <c r="AL51" s="165" t="s">
-        <v>815</v>
+        <v>786</v>
       </c>
       <c r="AM51" s="162"/>
       <c r="AN51" s="162"/>
@@ -21495,16 +21551,12 @@
       <c r="BZ51" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA51" s="208" t="s">
-        <v>816</v>
+      <c r="CA51" s="111" t="s">
+        <v>786</v>
       </c>
       <c r="CB51" s="111"/>
-      <c r="CC51" s="111" t="s">
-        <v>552</v>
-      </c>
-      <c r="CD51" s="111" t="s">
-        <v>817</v>
-      </c>
+      <c r="CC51" s="111"/>
+      <c r="CD51" s="111"/>
       <c r="CE51" s="111" t="s">
         <v>785</v>
       </c>
@@ -21518,12 +21570,10 @@
       <c r="CK51" s="111"/>
       <c r="CL51" s="111"/>
       <c r="CM51" s="111" t="s">
-        <v>818</v>
+        <v>785</v>
       </c>
       <c r="CN51" s="111"/>
-      <c r="CO51" s="111" t="s">
-        <v>819</v>
-      </c>
+      <c r="CO51" s="111"/>
       <c r="CP51" s="111"/>
       <c r="CQ51" s="111" t="s">
         <v>785</v>
@@ -21532,29 +21582,21 @@
       <c r="CS51" s="111"/>
       <c r="CT51" s="111"/>
       <c r="CU51" s="111" t="s">
-        <v>820</v>
+        <v>785</v>
       </c>
       <c r="CV51" s="111"/>
-      <c r="CW51" s="111" t="s">
-        <v>551</v>
-      </c>
+      <c r="CW51" s="111"/>
       <c r="CX51" s="111"/>
       <c r="CY51" s="111" t="s">
-        <v>821</v>
-      </c>
-      <c r="CZ51" s="111" t="s">
-        <v>547</v>
-      </c>
-      <c r="DA51" s="111" t="s">
-        <v>548</v>
-      </c>
+        <v>785</v>
+      </c>
+      <c r="CZ51" s="111"/>
+      <c r="DA51" s="111"/>
       <c r="DB51" s="111"/>
       <c r="DC51" s="111" t="s">
-        <v>822</v>
-      </c>
-      <c r="DD51" s="111" t="s">
-        <v>546</v>
-      </c>
+        <v>785</v>
+      </c>
+      <c r="DD51" s="111"/>
       <c r="DE51" s="111"/>
       <c r="DF51" s="111"/>
       <c r="DG51" s="111" t="s">
@@ -21567,12 +21609,8 @@
         <v>785</v>
       </c>
       <c r="DL51" s="111"/>
-      <c r="DM51" s="111" t="s">
-        <v>549</v>
-      </c>
-      <c r="DN51" s="111" t="s">
-        <v>823</v>
-      </c>
+      <c r="DM51" s="111"/>
+      <c r="DN51" s="111"/>
       <c r="DO51" s="111" t="s">
         <v>785</v>
       </c>
@@ -21598,23 +21636,19 @@
       <c r="EC51" s="111"/>
       <c r="ED51" s="111"/>
       <c r="EE51" s="111" t="s">
-        <v>824</v>
+        <v>785</v>
       </c>
       <c r="EF51" s="111"/>
-      <c r="EG51" s="111" t="s">
-        <v>602</v>
-      </c>
+      <c r="EG51" s="111"/>
       <c r="EH51" s="111"/>
       <c r="EI51" s="111" t="s">
         <v>785</v>
       </c>
       <c r="EJ51" s="111"/>
-      <c r="EK51" s="111" t="s">
-        <v>550</v>
-      </c>
+      <c r="EK51" s="111"/>
       <c r="EL51" s="111"/>
       <c r="EM51" s="111" t="s">
-        <v>825</v>
+        <v>785</v>
       </c>
       <c r="EN51" s="111"/>
       <c r="EO51" s="111"/>
@@ -21623,16 +21657,14 @@
         <v>785</v>
       </c>
       <c r="ER51" s="111"/>
-      <c r="ES51" s="111" t="s">
-        <v>550</v>
-      </c>
+      <c r="ES51" s="111"/>
       <c r="ET51" s="111"/>
       <c r="EU51" s="111"/>
       <c r="EV51" s="111"/>
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>785</v>
+        <v>811</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
@@ -21698,7 +21730,7 @@
     </row>
     <row r="52" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="62" t="s">
-        <v>542</v>
+        <v>253</v>
       </c>
       <c r="B52" s="110"/>
       <c r="C52" s="110"/>
@@ -21706,12 +21738,8 @@
       <c r="E52" s="110"/>
       <c r="F52" s="110"/>
       <c r="G52" s="110"/>
-      <c r="H52" s="110" t="s">
-        <v>814</v>
-      </c>
-      <c r="I52" s="110" t="s">
-        <v>545</v>
-      </c>
+      <c r="H52" s="110"/>
+      <c r="I52" s="110"/>
       <c r="J52" s="110"/>
       <c r="K52" s="110"/>
       <c r="L52" s="110"/>
@@ -21741,12 +21769,10 @@
       <c r="AJ52" s="89"/>
       <c r="AK52" s="89"/>
       <c r="AL52" s="165" t="s">
-        <v>826</v>
+        <v>786</v>
       </c>
       <c r="AM52" s="162"/>
-      <c r="AN52" s="162" t="s">
-        <v>827</v>
-      </c>
+      <c r="AN52" s="162"/>
       <c r="AO52" s="162"/>
       <c r="AP52" s="162"/>
       <c r="AQ52" s="162"/>
@@ -21787,16 +21813,12 @@
       <c r="BZ52" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA52" s="208" t="s">
-        <v>828</v>
+      <c r="CA52" s="111" t="s">
+        <v>786</v>
       </c>
       <c r="CB52" s="111"/>
-      <c r="CC52" s="111" t="s">
-        <v>552</v>
-      </c>
-      <c r="CD52" s="111" t="s">
-        <v>817</v>
-      </c>
+      <c r="CC52" s="111"/>
+      <c r="CD52" s="111"/>
       <c r="CE52" s="111" t="s">
         <v>785</v>
       </c>
@@ -21810,12 +21832,10 @@
       <c r="CK52" s="111"/>
       <c r="CL52" s="111"/>
       <c r="CM52" s="111" t="s">
-        <v>829</v>
+        <v>785</v>
       </c>
       <c r="CN52" s="111"/>
-      <c r="CO52" s="111" t="s">
-        <v>819</v>
-      </c>
+      <c r="CO52" s="111"/>
       <c r="CP52" s="111"/>
       <c r="CQ52" s="111" t="s">
         <v>785</v>
@@ -21824,25 +21844,21 @@
       <c r="CS52" s="111"/>
       <c r="CT52" s="111"/>
       <c r="CU52" s="111" t="s">
-        <v>830</v>
+        <v>785</v>
       </c>
       <c r="CV52" s="111"/>
-      <c r="CW52" s="111" t="s">
-        <v>551</v>
-      </c>
+      <c r="CW52" s="111"/>
       <c r="CX52" s="111"/>
       <c r="CY52" s="111" t="s">
-        <v>831</v>
+        <v>785</v>
       </c>
       <c r="CZ52" s="111"/>
       <c r="DA52" s="111"/>
       <c r="DB52" s="111"/>
       <c r="DC52" s="111" t="s">
-        <v>780</v>
-      </c>
-      <c r="DD52" s="111" t="s">
-        <v>546</v>
-      </c>
+        <v>785</v>
+      </c>
+      <c r="DD52" s="111"/>
       <c r="DE52" s="111"/>
       <c r="DF52" s="111"/>
       <c r="DG52" s="111" t="s">
@@ -21855,12 +21871,8 @@
         <v>785</v>
       </c>
       <c r="DL52" s="111"/>
-      <c r="DM52" s="111" t="s">
-        <v>549</v>
-      </c>
-      <c r="DN52" s="111" t="s">
-        <v>823</v>
-      </c>
+      <c r="DM52" s="111"/>
+      <c r="DN52" s="111"/>
       <c r="DO52" s="111" t="s">
         <v>785</v>
       </c>
@@ -21886,25 +21898,25 @@
       <c r="EC52" s="111"/>
       <c r="ED52" s="111"/>
       <c r="EE52" s="111" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="EF52" s="111"/>
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>785</v>
+        <v>812</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
       <c r="EL52" s="111"/>
       <c r="EM52" s="111" t="s">
-        <v>825</v>
+        <v>785</v>
       </c>
       <c r="EN52" s="111"/>
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>785</v>
+        <v>813</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -21980,7 +21992,7 @@
     </row>
     <row r="53" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>4</v>
+        <v>774</v>
       </c>
       <c r="B53" s="110"/>
       <c r="C53" s="110"/>
@@ -21995,9 +22007,15 @@
       <c r="L53" s="110"/>
       <c r="M53" s="110"/>
       <c r="N53" s="110"/>
-      <c r="O53" s="110"/>
-      <c r="P53" s="110"/>
-      <c r="Q53" s="110"/>
+      <c r="O53" s="103" t="s">
+        <v>281</v>
+      </c>
+      <c r="P53" s="103" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q53" s="103" t="s">
+        <v>283</v>
+      </c>
       <c r="R53" s="89"/>
       <c r="S53" s="89"/>
       <c r="T53" s="89"/>
@@ -22014,12 +22032,18 @@
       <c r="AE53" s="89"/>
       <c r="AF53" s="89"/>
       <c r="AG53" s="89"/>
-      <c r="AH53" s="89"/>
-      <c r="AI53" s="89"/>
-      <c r="AJ53" s="89"/>
-      <c r="AK53" s="89"/>
+      <c r="AH53" s="90"/>
+      <c r="AI53" s="92" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ53" s="92" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK53" s="92" t="s">
+        <v>283</v>
+      </c>
       <c r="AL53" s="165" t="s">
-        <v>786</v>
+        <v>855</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22029,48 +22053,96 @@
       <c r="AR53" s="162"/>
       <c r="AS53" s="162"/>
       <c r="AT53" s="162"/>
-      <c r="AU53" s="162"/>
-      <c r="AV53" s="162"/>
-      <c r="AW53" s="162"/>
+      <c r="AU53" s="161" t="s">
+        <v>281</v>
+      </c>
+      <c r="AV53" s="161" t="s">
+        <v>282</v>
+      </c>
+      <c r="AW53" s="161" t="s">
+        <v>283</v>
+      </c>
       <c r="AX53" s="167"/>
-      <c r="AY53" s="167"/>
-      <c r="AZ53" s="167"/>
-      <c r="BA53" s="167"/>
+      <c r="AY53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="AZ53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BA53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BB53" s="167"/>
-      <c r="BC53" s="167"/>
-      <c r="BD53" s="167"/>
-      <c r="BE53" s="167"/>
+      <c r="BC53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BD53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BE53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BF53" s="167"/>
-      <c r="BG53" s="167"/>
-      <c r="BH53" s="167"/>
-      <c r="BI53" s="167"/>
+      <c r="BG53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BH53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BI53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BJ53" s="167"/>
-      <c r="BK53" s="167"/>
-      <c r="BL53" s="167"/>
-      <c r="BM53" s="167"/>
+      <c r="BK53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BL53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BM53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BN53" s="167"/>
-      <c r="BO53" s="167"/>
-      <c r="BP53" s="167"/>
-      <c r="BQ53" s="167"/>
+      <c r="BO53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BP53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BQ53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BR53" s="167"/>
-      <c r="BS53" s="167"/>
-      <c r="BT53" s="167"/>
-      <c r="BU53" s="167"/>
+      <c r="BS53" s="167" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT53" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="BU53" s="167" t="s">
+        <v>283</v>
+      </c>
       <c r="BV53" s="167"/>
-      <c r="BW53" s="167"/>
-      <c r="BX53" s="167"/>
-      <c r="BY53" s="252"/>
+      <c r="BW53" s="166" t="s">
+        <v>281</v>
+      </c>
+      <c r="BX53" s="166" t="s">
+        <v>282</v>
+      </c>
+      <c r="BY53" s="250" t="s">
+        <v>283</v>
+      </c>
       <c r="BZ53" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="CA53" s="208" t="s">
-        <v>832</v>
+        <v>856</v>
+      </c>
+      <c r="CA53" s="111" t="s">
+        <v>786</v>
       </c>
       <c r="CB53" s="111"/>
       <c r="CC53" s="111"/>
       <c r="CD53" s="111"/>
       <c r="CE53" s="111" t="s">
-        <v>833</v>
+        <v>785</v>
       </c>
       <c r="CF53" s="111"/>
       <c r="CG53" s="111"/>
@@ -22082,7 +22154,7 @@
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>834</v>
+        <v>857</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
@@ -22094,19 +22166,19 @@
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>785</v>
+        <v>852</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
       <c r="CX53" s="111"/>
       <c r="CY53" s="111" t="s">
-        <v>835</v>
+        <v>785</v>
       </c>
       <c r="CZ53" s="111"/>
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>836</v>
+        <v>853</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
@@ -22148,7 +22220,7 @@
       <c r="EC53" s="111"/>
       <c r="ED53" s="111"/>
       <c r="EE53" s="111" t="s">
-        <v>837</v>
+        <v>785</v>
       </c>
       <c r="EF53" s="111"/>
       <c r="EG53" s="111"/>
@@ -22160,7 +22232,7 @@
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>838</v>
+        <v>854</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
@@ -22242,7 +22314,7 @@
     </row>
     <row r="54" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="62" t="s">
-        <v>254</v>
+        <v>543</v>
       </c>
       <c r="B54" s="110"/>
       <c r="C54" s="110"/>
@@ -22250,8 +22322,12 @@
       <c r="E54" s="110"/>
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
-      <c r="H54" s="110"/>
-      <c r="I54" s="110"/>
+      <c r="H54" s="110" t="s">
+        <v>814</v>
+      </c>
+      <c r="I54" s="110" t="s">
+        <v>545</v>
+      </c>
       <c r="J54" s="110"/>
       <c r="K54" s="110"/>
       <c r="L54" s="110"/>
@@ -22281,7 +22357,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>786</v>
+        <v>815</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22325,12 +22401,16 @@
       <c r="BZ54" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA54" s="111" t="s">
-        <v>786</v>
+      <c r="CA54" s="208" t="s">
+        <v>816</v>
       </c>
       <c r="CB54" s="111"/>
-      <c r="CC54" s="111"/>
-      <c r="CD54" s="111"/>
+      <c r="CC54" s="111" t="s">
+        <v>552</v>
+      </c>
+      <c r="CD54" s="111" t="s">
+        <v>817</v>
+      </c>
       <c r="CE54" s="111" t="s">
         <v>785</v>
       </c>
@@ -22344,10 +22424,12 @@
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>785</v>
+        <v>818</v>
       </c>
       <c r="CN54" s="111"/>
-      <c r="CO54" s="111"/>
+      <c r="CO54" s="111" t="s">
+        <v>819</v>
+      </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
         <v>785</v>
@@ -22356,21 +22438,29 @@
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>787</v>
+        <v>820</v>
       </c>
       <c r="CV54" s="111"/>
-      <c r="CW54" s="111"/>
+      <c r="CW54" s="111" t="s">
+        <v>551</v>
+      </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>839</v>
-      </c>
-      <c r="CZ54" s="111"/>
-      <c r="DA54" s="111"/>
+        <v>821</v>
+      </c>
+      <c r="CZ54" s="111" t="s">
+        <v>547</v>
+      </c>
+      <c r="DA54" s="111" t="s">
+        <v>548</v>
+      </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>785</v>
-      </c>
-      <c r="DD54" s="111"/>
+        <v>822</v>
+      </c>
+      <c r="DD54" s="111" t="s">
+        <v>546</v>
+      </c>
       <c r="DE54" s="111"/>
       <c r="DF54" s="111"/>
       <c r="DG54" s="111" t="s">
@@ -22383,8 +22473,12 @@
         <v>785</v>
       </c>
       <c r="DL54" s="111"/>
-      <c r="DM54" s="111"/>
-      <c r="DN54" s="111"/>
+      <c r="DM54" s="111" t="s">
+        <v>549</v>
+      </c>
+      <c r="DN54" s="111" t="s">
+        <v>823</v>
+      </c>
       <c r="DO54" s="111" t="s">
         <v>785</v>
       </c>
@@ -22410,19 +22504,23 @@
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>840</v>
+        <v>824</v>
       </c>
       <c r="EF54" s="111"/>
-      <c r="EG54" s="111"/>
+      <c r="EG54" s="111" t="s">
+        <v>602</v>
+      </c>
       <c r="EH54" s="111"/>
       <c r="EI54" s="111" t="s">
         <v>785</v>
       </c>
       <c r="EJ54" s="111"/>
-      <c r="EK54" s="111"/>
+      <c r="EK54" s="111" t="s">
+        <v>550</v>
+      </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>785</v>
+        <v>825</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
@@ -22431,7 +22529,9 @@
         <v>785</v>
       </c>
       <c r="ER54" s="111"/>
-      <c r="ES54" s="111"/>
+      <c r="ES54" s="111" t="s">
+        <v>550</v>
+      </c>
       <c r="ET54" s="111"/>
       <c r="EU54" s="111"/>
       <c r="EV54" s="111"/>
@@ -22504,7 +22604,7 @@
     </row>
     <row r="55" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="62" t="s">
-        <v>255</v>
+        <v>542</v>
       </c>
       <c r="B55" s="110"/>
       <c r="C55" s="110"/>
@@ -22512,8 +22612,12 @@
       <c r="E55" s="110"/>
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
-      <c r="H55" s="110"/>
-      <c r="I55" s="110"/>
+      <c r="H55" s="110" t="s">
+        <v>814</v>
+      </c>
+      <c r="I55" s="110" t="s">
+        <v>545</v>
+      </c>
       <c r="J55" s="110"/>
       <c r="K55" s="110"/>
       <c r="L55" s="110"/>
@@ -22538,15 +22642,17 @@
       <c r="AE55" s="89"/>
       <c r="AF55" s="89"/>
       <c r="AG55" s="89"/>
-      <c r="AH55" s="88"/>
-      <c r="AI55" s="90"/>
-      <c r="AJ55" s="90"/>
-      <c r="AK55" s="88"/>
+      <c r="AH55" s="89"/>
+      <c r="AI55" s="89"/>
+      <c r="AJ55" s="89"/>
+      <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>841</v>
+        <v>826</v>
       </c>
       <c r="AM55" s="162"/>
-      <c r="AN55" s="162"/>
+      <c r="AN55" s="162" t="s">
+        <v>827</v>
+      </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
       <c r="AQ55" s="162"/>
@@ -22587,14 +22693,18 @@
       <c r="BZ55" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA55" s="111" t="s">
-        <v>786</v>
+      <c r="CA55" s="208" t="s">
+        <v>828</v>
       </c>
       <c r="CB55" s="111"/>
-      <c r="CC55" s="111"/>
-      <c r="CD55" s="111"/>
+      <c r="CC55" s="111" t="s">
+        <v>552</v>
+      </c>
+      <c r="CD55" s="111" t="s">
+        <v>817</v>
+      </c>
       <c r="CE55" s="111" t="s">
-        <v>842</v>
+        <v>785</v>
       </c>
       <c r="CF55" s="111"/>
       <c r="CG55" s="111"/>
@@ -22606,10 +22716,12 @@
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>843</v>
+        <v>829</v>
       </c>
       <c r="CN55" s="111"/>
-      <c r="CO55" s="111"/>
+      <c r="CO55" s="111" t="s">
+        <v>819</v>
+      </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
         <v>785</v>
@@ -22618,21 +22730,25 @@
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>844</v>
+        <v>830</v>
       </c>
       <c r="CV55" s="111"/>
-      <c r="CW55" s="111"/>
+      <c r="CW55" s="111" t="s">
+        <v>551</v>
+      </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>845</v>
+        <v>831</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
       <c r="DB55" s="111"/>
       <c r="DC55" s="111" t="s">
-        <v>846</v>
-      </c>
-      <c r="DD55" s="111"/>
+        <v>780</v>
+      </c>
+      <c r="DD55" s="111" t="s">
+        <v>546</v>
+      </c>
       <c r="DE55" s="111"/>
       <c r="DF55" s="111"/>
       <c r="DG55" s="111" t="s">
@@ -22645,10 +22761,14 @@
         <v>785</v>
       </c>
       <c r="DL55" s="111"/>
-      <c r="DM55" s="111"/>
-      <c r="DN55" s="111"/>
+      <c r="DM55" s="111" t="s">
+        <v>549</v>
+      </c>
+      <c r="DN55" s="111" t="s">
+        <v>823</v>
+      </c>
       <c r="DO55" s="111" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="DP55" s="111"/>
       <c r="DQ55" s="111"/>
@@ -22672,25 +22792,25 @@
       <c r="EC55" s="111"/>
       <c r="ED55" s="111"/>
       <c r="EE55" s="111" t="s">
-        <v>847</v>
+        <v>779</v>
       </c>
       <c r="EF55" s="111"/>
       <c r="EG55" s="111"/>
       <c r="EH55" s="111"/>
       <c r="EI55" s="111" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
       <c r="EJ55" s="111"/>
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>797</v>
+        <v>825</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
       <c r="EP55" s="111"/>
       <c r="EQ55" s="111" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="ER55" s="111"/>
       <c r="ES55" s="111"/>
@@ -22705,8 +22825,8 @@
       <c r="EZ55" s="208"/>
       <c r="FA55" s="208"/>
       <c r="FB55" s="208"/>
-      <c r="FC55" s="208" t="s">
-        <v>799</v>
+      <c r="FC55" s="111" t="s">
+        <v>785</v>
       </c>
       <c r="FD55" s="111"/>
       <c r="FE55" s="111"/>
@@ -22766,7 +22886,7 @@
     </row>
     <row r="56" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="62" t="s">
-        <v>256</v>
+        <v>4</v>
       </c>
       <c r="B56" s="110"/>
       <c r="C56" s="110"/>
@@ -22800,10 +22920,10 @@
       <c r="AE56" s="89"/>
       <c r="AF56" s="89"/>
       <c r="AG56" s="89"/>
-      <c r="AH56" s="90"/>
-      <c r="AI56" s="90"/>
-      <c r="AJ56" s="90"/>
-      <c r="AK56" s="90"/>
+      <c r="AH56" s="89"/>
+      <c r="AI56" s="89"/>
+      <c r="AJ56" s="89"/>
+      <c r="AK56" s="89"/>
       <c r="AL56" s="165" t="s">
         <v>786</v>
       </c>
@@ -22849,14 +22969,14 @@
       <c r="BZ56" s="111" t="s">
         <v>785</v>
       </c>
-      <c r="CA56" s="111" t="s">
-        <v>786</v>
+      <c r="CA56" s="208" t="s">
+        <v>832</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>848</v>
+        <v>833</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
@@ -22868,7 +22988,7 @@
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>785</v>
+        <v>834</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
@@ -22892,7 +23012,7 @@
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>785</v>
+        <v>836</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
@@ -22946,7 +23066,7 @@
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>785</v>
+        <v>838</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
@@ -23028,7 +23148,7 @@
     </row>
     <row r="57" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="62" t="s">
-        <v>540</v>
+        <v>254</v>
       </c>
       <c r="B57" s="110"/>
       <c r="C57" s="110"/>
@@ -23062,10 +23182,10 @@
       <c r="AE57" s="89"/>
       <c r="AF57" s="89"/>
       <c r="AG57" s="89"/>
-      <c r="AH57" s="90"/>
-      <c r="AI57" s="90"/>
-      <c r="AJ57" s="90"/>
-      <c r="AK57" s="90"/>
+      <c r="AH57" s="89"/>
+      <c r="AI57" s="89"/>
+      <c r="AJ57" s="89"/>
+      <c r="AK57" s="89"/>
       <c r="AL57" s="165" t="s">
         <v>786</v>
       </c>
@@ -23136,19 +23256,19 @@
       <c r="CO57" s="111"/>
       <c r="CP57" s="111"/>
       <c r="CQ57" s="111" t="s">
-        <v>849</v>
+        <v>785</v>
       </c>
       <c r="CR57" s="111"/>
       <c r="CS57" s="111"/>
       <c r="CT57" s="111"/>
       <c r="CU57" s="111" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="CV57" s="111"/>
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>785</v>
+        <v>839</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
@@ -23196,7 +23316,7 @@
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>785</v>
+        <v>840</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
@@ -23229,8 +23349,8 @@
       <c r="EZ57" s="208"/>
       <c r="FA57" s="208"/>
       <c r="FB57" s="208"/>
-      <c r="FC57" s="208" t="s">
-        <v>850</v>
+      <c r="FC57" s="111" t="s">
+        <v>785</v>
       </c>
       <c r="FD57" s="111"/>
       <c r="FE57" s="111"/>
@@ -23290,7 +23410,7 @@
     </row>
     <row r="58" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="62" t="s">
-        <v>571</v>
+        <v>255</v>
       </c>
       <c r="B58" s="110"/>
       <c r="C58" s="110"/>
@@ -23305,15 +23425,9 @@
       <c r="L58" s="110"/>
       <c r="M58" s="110"/>
       <c r="N58" s="110"/>
-      <c r="O58" s="103" t="s">
-        <v>281</v>
-      </c>
-      <c r="P58" s="103" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q58" s="103" t="s">
-        <v>283</v>
-      </c>
+      <c r="O58" s="110"/>
+      <c r="P58" s="110"/>
+      <c r="Q58" s="110"/>
       <c r="R58" s="89"/>
       <c r="S58" s="89"/>
       <c r="T58" s="89"/>
@@ -23330,18 +23444,12 @@
       <c r="AE58" s="89"/>
       <c r="AF58" s="89"/>
       <c r="AG58" s="89"/>
-      <c r="AH58" s="90"/>
-      <c r="AI58" s="92" t="s">
-        <v>281</v>
-      </c>
-      <c r="AJ58" s="92" t="s">
-        <v>282</v>
-      </c>
-      <c r="AK58" s="92" t="s">
-        <v>283</v>
-      </c>
+      <c r="AH58" s="88"/>
+      <c r="AI58" s="90"/>
+      <c r="AJ58" s="90"/>
+      <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>786</v>
+        <v>841</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23351,85 +23459,37 @@
       <c r="AR58" s="162"/>
       <c r="AS58" s="162"/>
       <c r="AT58" s="162"/>
-      <c r="AU58" s="161" t="s">
-        <v>281</v>
-      </c>
-      <c r="AV58" s="161" t="s">
-        <v>282</v>
-      </c>
-      <c r="AW58" s="161" t="s">
-        <v>283</v>
-      </c>
+      <c r="AU58" s="162"/>
+      <c r="AV58" s="162"/>
+      <c r="AW58" s="162"/>
       <c r="AX58" s="167"/>
-      <c r="AY58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="AZ58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BA58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="AY58" s="167"/>
+      <c r="AZ58" s="167"/>
+      <c r="BA58" s="167"/>
       <c r="BB58" s="167"/>
-      <c r="BC58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BD58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BE58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BC58" s="167"/>
+      <c r="BD58" s="167"/>
+      <c r="BE58" s="167"/>
       <c r="BF58" s="167"/>
-      <c r="BG58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BH58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BI58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BG58" s="167"/>
+      <c r="BH58" s="167"/>
+      <c r="BI58" s="167"/>
       <c r="BJ58" s="167"/>
-      <c r="BK58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BL58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BM58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BK58" s="167"/>
+      <c r="BL58" s="167"/>
+      <c r="BM58" s="167"/>
       <c r="BN58" s="167"/>
-      <c r="BO58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BP58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BQ58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BO58" s="167"/>
+      <c r="BP58" s="167"/>
+      <c r="BQ58" s="167"/>
       <c r="BR58" s="167"/>
-      <c r="BS58" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT58" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BU58" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BS58" s="167"/>
+      <c r="BT58" s="167"/>
+      <c r="BU58" s="167"/>
       <c r="BV58" s="167"/>
-      <c r="BW58" s="166" t="s">
-        <v>281</v>
-      </c>
-      <c r="BX58" s="166" t="s">
-        <v>282</v>
-      </c>
-      <c r="BY58" s="250" t="s">
-        <v>283</v>
-      </c>
+      <c r="BW58" s="167"/>
+      <c r="BX58" s="167"/>
+      <c r="BY58" s="252"/>
       <c r="BZ58" s="111" t="s">
         <v>785</v>
       </c>
@@ -23440,7 +23500,7 @@
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>785</v>
+        <v>842</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
@@ -23452,7 +23512,7 @@
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
@@ -23464,19 +23524,19 @@
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>785</v>
+        <v>845</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
@@ -23494,7 +23554,7 @@
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
@@ -23518,25 +23578,25 @@
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>785</v>
+        <v>847</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>785</v>
+        <v>796</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>854</v>
+        <v>797</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>785</v>
+        <v>798</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23551,8 +23611,8 @@
       <c r="EZ58" s="208"/>
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
-      <c r="FC58" s="111" t="s">
-        <v>785</v>
+      <c r="FC58" s="208" t="s">
+        <v>799</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23612,7 +23672,7 @@
     </row>
     <row r="59" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="62" t="s">
-        <v>775</v>
+        <v>256</v>
       </c>
       <c r="B59" s="110"/>
       <c r="C59" s="110"/>
@@ -23627,15 +23687,9 @@
       <c r="L59" s="110"/>
       <c r="M59" s="110"/>
       <c r="N59" s="110"/>
-      <c r="O59" s="103" t="s">
-        <v>281</v>
-      </c>
-      <c r="P59" s="103" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q59" s="103" t="s">
-        <v>283</v>
-      </c>
+      <c r="O59" s="110"/>
+      <c r="P59" s="110"/>
+      <c r="Q59" s="110"/>
       <c r="R59" s="89"/>
       <c r="S59" s="89"/>
       <c r="T59" s="89"/>
@@ -23653,17 +23707,11 @@
       <c r="AF59" s="89"/>
       <c r="AG59" s="89"/>
       <c r="AH59" s="90"/>
-      <c r="AI59" s="92" t="s">
-        <v>281</v>
-      </c>
-      <c r="AJ59" s="92" t="s">
-        <v>282</v>
-      </c>
-      <c r="AK59" s="92" t="s">
-        <v>283</v>
-      </c>
+      <c r="AI59" s="90"/>
+      <c r="AJ59" s="90"/>
+      <c r="AK59" s="90"/>
       <c r="AL59" s="165" t="s">
-        <v>855</v>
+        <v>786</v>
       </c>
       <c r="AM59" s="162"/>
       <c r="AN59" s="162"/>
@@ -23673,87 +23721,39 @@
       <c r="AR59" s="162"/>
       <c r="AS59" s="162"/>
       <c r="AT59" s="162"/>
-      <c r="AU59" s="161" t="s">
-        <v>281</v>
-      </c>
-      <c r="AV59" s="161" t="s">
-        <v>282</v>
-      </c>
-      <c r="AW59" s="161" t="s">
-        <v>283</v>
-      </c>
+      <c r="AU59" s="162"/>
+      <c r="AV59" s="162"/>
+      <c r="AW59" s="162"/>
       <c r="AX59" s="167"/>
-      <c r="AY59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="AZ59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BA59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="AY59" s="167"/>
+      <c r="AZ59" s="167"/>
+      <c r="BA59" s="167"/>
       <c r="BB59" s="167"/>
-      <c r="BC59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BD59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BE59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BC59" s="167"/>
+      <c r="BD59" s="167"/>
+      <c r="BE59" s="167"/>
       <c r="BF59" s="167"/>
-      <c r="BG59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BH59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BI59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BG59" s="167"/>
+      <c r="BH59" s="167"/>
+      <c r="BI59" s="167"/>
       <c r="BJ59" s="167"/>
-      <c r="BK59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BL59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BM59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BK59" s="167"/>
+      <c r="BL59" s="167"/>
+      <c r="BM59" s="167"/>
       <c r="BN59" s="167"/>
-      <c r="BO59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BP59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BQ59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BO59" s="167"/>
+      <c r="BP59" s="167"/>
+      <c r="BQ59" s="167"/>
       <c r="BR59" s="167"/>
-      <c r="BS59" s="167" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT59" s="167" t="s">
-        <v>282</v>
-      </c>
-      <c r="BU59" s="167" t="s">
-        <v>283</v>
-      </c>
+      <c r="BS59" s="167"/>
+      <c r="BT59" s="167"/>
+      <c r="BU59" s="167"/>
       <c r="BV59" s="167"/>
-      <c r="BW59" s="166" t="s">
-        <v>281</v>
-      </c>
-      <c r="BX59" s="166" t="s">
-        <v>282</v>
-      </c>
-      <c r="BY59" s="250" t="s">
-        <v>283</v>
-      </c>
+      <c r="BW59" s="167"/>
+      <c r="BX59" s="167"/>
+      <c r="BY59" s="252"/>
       <c r="BZ59" s="111" t="s">
-        <v>856</v>
+        <v>785</v>
       </c>
       <c r="CA59" s="111" t="s">
         <v>786</v>
@@ -23762,7 +23762,7 @@
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>785</v>
+        <v>848</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
@@ -23774,7 +23774,7 @@
       <c r="CK59" s="111"/>
       <c r="CL59" s="111"/>
       <c r="CM59" s="111" t="s">
-        <v>857</v>
+        <v>785</v>
       </c>
       <c r="CN59" s="111"/>
       <c r="CO59" s="111"/>
@@ -23786,19 +23786,19 @@
       <c r="CS59" s="111"/>
       <c r="CT59" s="111"/>
       <c r="CU59" s="111" t="s">
-        <v>852</v>
+        <v>785</v>
       </c>
       <c r="CV59" s="111"/>
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>785</v>
+        <v>835</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
       <c r="DB59" s="111"/>
       <c r="DC59" s="111" t="s">
-        <v>853</v>
+        <v>785</v>
       </c>
       <c r="DD59" s="111"/>
       <c r="DE59" s="111"/>
@@ -23840,7 +23840,7 @@
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>785</v>
+        <v>837</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
@@ -23852,7 +23852,7 @@
       <c r="EK59" s="111"/>
       <c r="EL59" s="111"/>
       <c r="EM59" s="111" t="s">
-        <v>854</v>
+        <v>785</v>
       </c>
       <c r="EN59" s="111"/>
       <c r="EO59" s="111"/>
@@ -23933,8 +23933,8 @@
       <c r="HF59" s="218"/>
     </row>
     <row r="60" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="157" t="s">
-        <v>704</v>
+      <c r="A60" s="62" t="s">
+        <v>540</v>
       </c>
       <c r="B60" s="110"/>
       <c r="C60" s="110"/>
@@ -23949,9 +23949,9 @@
       <c r="L60" s="110"/>
       <c r="M60" s="110"/>
       <c r="N60" s="110"/>
-      <c r="O60" s="103"/>
-      <c r="P60" s="103"/>
-      <c r="Q60" s="103"/>
+      <c r="O60" s="110"/>
+      <c r="P60" s="110"/>
+      <c r="Q60" s="110"/>
       <c r="R60" s="89"/>
       <c r="S60" s="89"/>
       <c r="T60" s="89"/>
@@ -23969,11 +23969,11 @@
       <c r="AF60" s="89"/>
       <c r="AG60" s="89"/>
       <c r="AH60" s="90"/>
-      <c r="AI60" s="92"/>
-      <c r="AJ60" s="92"/>
-      <c r="AK60" s="92"/>
+      <c r="AI60" s="90"/>
+      <c r="AJ60" s="90"/>
+      <c r="AK60" s="90"/>
       <c r="AL60" s="165" t="s">
-        <v>712</v>
+        <v>786</v>
       </c>
       <c r="AM60" s="162"/>
       <c r="AN60" s="162"/>
@@ -23983,9 +23983,9 @@
       <c r="AR60" s="162"/>
       <c r="AS60" s="162"/>
       <c r="AT60" s="162"/>
-      <c r="AU60" s="161"/>
-      <c r="AV60" s="161"/>
-      <c r="AW60" s="161"/>
+      <c r="AU60" s="162"/>
+      <c r="AV60" s="162"/>
+      <c r="AW60" s="162"/>
       <c r="AX60" s="167"/>
       <c r="AY60" s="167"/>
       <c r="AZ60" s="167"/>
@@ -24011,136 +24011,136 @@
       <c r="BT60" s="167"/>
       <c r="BU60" s="167"/>
       <c r="BV60" s="167"/>
-      <c r="BW60" s="166"/>
-      <c r="BX60" s="166"/>
-      <c r="BY60" s="250"/>
+      <c r="BW60" s="167"/>
+      <c r="BX60" s="167"/>
+      <c r="BY60" s="252"/>
       <c r="BZ60" s="111" t="s">
-        <v>712</v>
-      </c>
-      <c r="CA60" s="208" t="s">
-        <v>712</v>
+        <v>785</v>
+      </c>
+      <c r="CA60" s="111" t="s">
+        <v>786</v>
       </c>
       <c r="CB60" s="111"/>
       <c r="CC60" s="111"/>
       <c r="CD60" s="111"/>
       <c r="CE60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="CF60" s="111"/>
       <c r="CG60" s="111"/>
       <c r="CH60" s="111"/>
       <c r="CI60" s="111" t="s">
-        <v>713</v>
+        <v>785</v>
       </c>
       <c r="CJ60" s="111"/>
       <c r="CK60" s="111"/>
       <c r="CL60" s="111"/>
       <c r="CM60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="CN60" s="111"/>
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>712</v>
+        <v>849</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
       <c r="CT60" s="111"/>
       <c r="CU60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="CV60" s="111"/>
       <c r="CW60" s="111"/>
       <c r="CX60" s="111"/>
       <c r="CY60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="CZ60" s="111"/>
       <c r="DA60" s="111"/>
       <c r="DB60" s="111"/>
       <c r="DC60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="DD60" s="111"/>
       <c r="DE60" s="111"/>
       <c r="DF60" s="111"/>
       <c r="DG60" s="111" t="s">
-        <v>713</v>
+        <v>785</v>
       </c>
       <c r="DH60" s="111"/>
       <c r="DI60" s="111"/>
       <c r="DJ60" s="111"/>
       <c r="DK60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="DL60" s="111"/>
       <c r="DM60" s="111"/>
       <c r="DN60" s="111"/>
       <c r="DO60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="DP60" s="111"/>
       <c r="DQ60" s="111"/>
       <c r="DR60" s="111"/>
       <c r="DS60" s="111" t="s">
-        <v>713</v>
+        <v>785</v>
       </c>
       <c r="DT60" s="111"/>
       <c r="DU60" s="111"/>
       <c r="DV60" s="111"/>
       <c r="DW60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="DX60" s="111"/>
       <c r="DY60" s="111"/>
       <c r="DZ60" s="111"/>
       <c r="EA60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="EB60" s="111"/>
       <c r="EC60" s="111"/>
       <c r="ED60" s="111"/>
       <c r="EE60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="EF60" s="111"/>
       <c r="EG60" s="111"/>
       <c r="EH60" s="111"/>
       <c r="EI60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="EJ60" s="111"/>
       <c r="EK60" s="111"/>
       <c r="EL60" s="111"/>
       <c r="EM60" s="111" t="s">
-        <v>712</v>
+        <v>785</v>
       </c>
       <c r="EN60" s="111"/>
       <c r="EO60" s="111"/>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111" t="s">
-        <v>712</v>
-      </c>
-      <c r="ER60" s="185"/>
-      <c r="ES60" s="185"/>
-      <c r="ET60" s="185"/>
-      <c r="EU60" s="185"/>
-      <c r="EV60" s="185"/>
-      <c r="EW60" s="185"/>
-      <c r="EX60" s="185"/>
+        <v>785</v>
+      </c>
+      <c r="ER60" s="111"/>
+      <c r="ES60" s="111"/>
+      <c r="ET60" s="111"/>
+      <c r="EU60" s="111"/>
+      <c r="EV60" s="111"/>
+      <c r="EW60" s="111"/>
+      <c r="EX60" s="207"/>
       <c r="EY60" s="111" t="s">
-        <v>712</v>
-      </c>
-      <c r="EZ60" s="185"/>
-      <c r="FA60" s="185"/>
-      <c r="FB60" s="185"/>
-      <c r="FC60" s="111" t="s">
-        <v>712</v>
-      </c>
-      <c r="FD60" s="185"/>
-      <c r="FE60" s="185"/>
-      <c r="FF60" s="185"/>
+        <v>785</v>
+      </c>
+      <c r="EZ60" s="208"/>
+      <c r="FA60" s="208"/>
+      <c r="FB60" s="208"/>
+      <c r="FC60" s="208" t="s">
+        <v>850</v>
+      </c>
+      <c r="FD60" s="111"/>
+      <c r="FE60" s="111"/>
+      <c r="FF60" s="111"/>
       <c r="FG60" s="177"/>
       <c r="FH60" s="177"/>
       <c r="FI60" s="177"/>
@@ -33626,7 +33626,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="214" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D3" s="189" t="s">
         <v>603</v>
@@ -33635,31 +33635,31 @@
         <v>663</v>
       </c>
       <c r="F3" s="214" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G3" s="214" t="s">
+        <v>744</v>
+      </c>
+      <c r="H3" s="214" t="s">
         <v>745</v>
       </c>
-      <c r="H3" s="214" t="s">
+      <c r="I3" s="214" t="s">
         <v>746</v>
       </c>
-      <c r="I3" s="214" t="s">
+      <c r="J3" s="214" t="s">
         <v>747</v>
       </c>
-      <c r="J3" s="214" t="s">
+      <c r="K3" s="214" t="s">
         <v>748</v>
       </c>
-      <c r="K3" s="214" t="s">
+      <c r="L3" s="214" t="s">
         <v>749</v>
       </c>
-      <c r="L3" s="214" t="s">
+      <c r="M3" s="214" t="s">
         <v>750</v>
       </c>
-      <c r="M3" s="214" t="s">
+      <c r="N3" s="214" t="s">
         <v>751</v>
-      </c>
-      <c r="N3" s="214" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -33671,62 +33671,62 @@
       <c r="D4" s="216"/>
       <c r="E4" s="216"/>
       <c r="F4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="L4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="M4" s="216" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="N4" s="216"/>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="215" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B5" s="216"/>
       <c r="C5" s="216"/>
       <c r="D5" s="216"/>
       <c r="E5" s="216"/>
       <c r="F5" s="248" t="s">
+        <v>764</v>
+      </c>
+      <c r="G5" s="248" t="s">
         <v>765</v>
       </c>
-      <c r="G5" s="248" t="s">
-        <v>766</v>
-      </c>
       <c r="H5" s="248" t="s">
+        <v>764</v>
+      </c>
+      <c r="I5" s="248" t="s">
         <v>765</v>
       </c>
-      <c r="I5" s="248" t="s">
-        <v>766</v>
-      </c>
       <c r="J5" s="248" t="s">
+        <v>764</v>
+      </c>
+      <c r="K5" s="248" t="s">
         <v>765</v>
       </c>
-      <c r="K5" s="248" t="s">
-        <v>766</v>
-      </c>
       <c r="L5" s="248" t="s">
+        <v>764</v>
+      </c>
+      <c r="M5" s="248" t="s">
         <v>765</v>
-      </c>
-      <c r="M5" s="248" t="s">
-        <v>766</v>
       </c>
       <c r="N5" s="216"/>
     </row>
@@ -35319,28 +35319,28 @@
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
       <c r="F46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="M46" s="72" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="N46" s="72"/>
     </row>
@@ -35353,28 +35353,28 @@
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
       <c r="F47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="K47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M47" s="72" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="N47" s="72"/>
     </row>
@@ -35429,28 +35429,28 @@
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
       <c r="F49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="K49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="L49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="N49" s="72"/>
     </row>
@@ -35463,28 +35463,28 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="L50" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="N50" s="72"/>
     </row>
@@ -35539,28 +35539,28 @@
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
       <c r="F52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="K52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="M52" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N52" s="72"/>
     </row>
@@ -35573,28 +35573,28 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H53" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I53" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J53" s="72" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="K53" s="72" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L53" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="M53" s="72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="N53" s="72"/>
     </row>
@@ -35649,28 +35649,28 @@
       <c r="D55" s="72"/>
       <c r="E55" s="72"/>
       <c r="F55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="K55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="L55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="M55" s="72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="N55" s="72"/>
     </row>
@@ -35683,28 +35683,28 @@
       <c r="D56" s="72"/>
       <c r="E56" s="72"/>
       <c r="F56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="H56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="L56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="M56" s="72" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="N56" s="72"/>
     </row>
@@ -35759,28 +35759,28 @@
       <c r="D58" s="72"/>
       <c r="E58" s="72"/>
       <c r="F58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="K58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="L58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="M58" s="72" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="N58" s="72"/>
     </row>
@@ -35793,28 +35793,28 @@
       <c r="D59" s="72"/>
       <c r="E59" s="72"/>
       <c r="F59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="K59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="L59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="M59" s="72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="N59" s="72"/>
     </row>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Resolve propofol merge conflicts.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="857">
   <si>
     <t>Name</t>
   </si>
@@ -2373,9 +2373,6 @@
     <t>4.5 mL/min kg</t>
   </si>
   <si>
-    <t>[0, 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.25; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2421,9 +2418,6 @@
     <t>[0.45; 8 ug/L]</t>
   </si>
   <si>
-    <t>[-0.25; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.2; 0.5549 ug/mL]</t>
   </si>
   <si>
@@ -2460,9 +2454,6 @@
     <t>[-0.06; 0.075 ug/mL]</t>
   </si>
   <si>
-    <t>[0.15; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.2; 0.5549 ug/mL]</t>
   </si>
   <si>
@@ -2508,9 +2499,6 @@
     <t>Often used to reverse opioid effects; and since opioids affect pupil diameter; it's hard to distinguish naloxone effects</t>
   </si>
   <si>
-    <t>[0.5; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[-1; 0.5 ug/mL]</t>
   </si>
   <si>
@@ -2547,18 +2535,12 @@
     <t>[-1; 0.075 ug/mL]</t>
   </si>
   <si>
-    <t>[-1; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.5; 0.5 ug/mL]</t>
   </si>
   <si>
     <t>[1; 0.0558 ug/mL]</t>
   </si>
   <si>
-    <t>[1; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.5; 0.9 ug/L]</t>
   </si>
   <si>
@@ -2577,9 +2559,6 @@
     <t>[-0.1; 0.075 ug/mL]</t>
   </si>
   <si>
-    <t>[-0.55; 0.7649 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.85; 100 ug/mL]</t>
   </si>
   <si>
@@ -2608,6 +2587,24 @@
   </si>
   <si>
     <t>[0.5; 0.4 ug/L]</t>
+  </si>
+  <si>
+    <t>[-0.25; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.15; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.5; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.55; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.7; 1.99 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5558,10 +5555,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="V32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CI32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V54" sqref="V54"/>
+      <selection pane="bottomRight" activeCell="EE55" sqref="EE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -12572,7 +12569,7 @@
         <v>591</v>
       </c>
       <c r="AV22" s="162" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="AW22" s="162"/>
       <c r="AX22" s="167"/>
@@ -16765,7 +16762,7 @@
       <c r="DE34" s="107"/>
       <c r="DF34" s="107"/>
       <c r="DG34" s="107" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="DH34" s="107"/>
       <c r="DI34" s="107"/>
@@ -20133,14 +20130,14 @@
       <c r="AJ46" s="89"/>
       <c r="AK46" s="89"/>
       <c r="AL46" s="165" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="AM46" s="162"/>
       <c r="AN46" s="162" t="s">
         <v>285</v>
       </c>
       <c r="AO46" s="162" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="AP46" s="162"/>
       <c r="AQ46" s="162"/>
@@ -20179,112 +20176,112 @@
       <c r="BX46" s="167"/>
       <c r="BY46" s="252"/>
       <c r="BZ46" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA46" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA46" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB46" s="111"/>
       <c r="CC46" s="111"/>
       <c r="CD46" s="111"/>
       <c r="CE46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF46" s="111"/>
       <c r="CG46" s="111"/>
       <c r="CH46" s="111"/>
       <c r="CI46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ46" s="111"/>
       <c r="CK46" s="111"/>
       <c r="CL46" s="111"/>
       <c r="CM46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN46" s="111"/>
       <c r="CO46" s="111"/>
       <c r="CP46" s="111"/>
       <c r="CQ46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR46" s="111"/>
       <c r="CS46" s="111"/>
       <c r="CT46" s="111"/>
       <c r="CU46" s="111" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="CV46" s="111"/>
       <c r="CW46" s="111"/>
       <c r="CX46" s="111"/>
       <c r="CY46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ46" s="111"/>
       <c r="DA46" s="111"/>
       <c r="DB46" s="111"/>
       <c r="DC46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD46" s="111"/>
       <c r="DE46" s="111"/>
       <c r="DF46" s="111"/>
       <c r="DG46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH46" s="111"/>
       <c r="DI46" s="111"/>
       <c r="DJ46" s="111"/>
       <c r="DK46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL46" s="111"/>
       <c r="DM46" s="111"/>
       <c r="DN46" s="111"/>
       <c r="DO46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP46" s="111"/>
       <c r="DQ46" s="111"/>
       <c r="DR46" s="111"/>
       <c r="DS46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT46" s="111"/>
       <c r="DU46" s="111"/>
       <c r="DV46" s="111"/>
       <c r="DW46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX46" s="111"/>
       <c r="DY46" s="111"/>
       <c r="DZ46" s="111"/>
       <c r="EA46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB46" s="111"/>
       <c r="EC46" s="111"/>
       <c r="ED46" s="111"/>
       <c r="EE46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF46" s="111"/>
       <c r="EG46" s="111"/>
       <c r="EH46" s="111"/>
       <c r="EI46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ46" s="111"/>
       <c r="EK46" s="111"/>
       <c r="EL46" s="111"/>
       <c r="EM46" s="111" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="EN46" s="111"/>
       <c r="EO46" s="111"/>
       <c r="EP46" s="111"/>
       <c r="EQ46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER46" s="111"/>
       <c r="ES46" s="111"/>
@@ -20294,13 +20291,13 @@
       <c r="EW46" s="111"/>
       <c r="EX46" s="111"/>
       <c r="EY46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ46" s="111"/>
       <c r="FA46" s="111"/>
       <c r="FB46" s="111"/>
       <c r="FC46" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD46" s="111"/>
       <c r="FE46" s="111"/>
@@ -20411,7 +20408,7 @@
         <v>283</v>
       </c>
       <c r="AL47" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM47" s="162"/>
       <c r="AN47" s="162"/>
@@ -20501,112 +20498,112 @@
         <v>283</v>
       </c>
       <c r="BZ47" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA47" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA47" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB47" s="111"/>
       <c r="CC47" s="111"/>
       <c r="CD47" s="111"/>
       <c r="CE47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF47" s="111"/>
       <c r="CG47" s="111"/>
       <c r="CH47" s="111"/>
       <c r="CI47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ47" s="111"/>
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
       <c r="CP47" s="111"/>
       <c r="CQ47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR47" s="111"/>
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
       <c r="CX47" s="111"/>
       <c r="CY47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ47" s="111"/>
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
       <c r="DF47" s="111"/>
       <c r="DG47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH47" s="111"/>
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>
       <c r="DN47" s="111"/>
       <c r="DO47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP47" s="111"/>
       <c r="DQ47" s="111"/>
       <c r="DR47" s="111"/>
       <c r="DS47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT47" s="111"/>
       <c r="DU47" s="111"/>
       <c r="DV47" s="111"/>
       <c r="DW47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX47" s="111"/>
       <c r="DY47" s="111"/>
       <c r="DZ47" s="111"/>
       <c r="EA47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB47" s="111"/>
       <c r="EC47" s="111"/>
       <c r="ED47" s="111"/>
       <c r="EE47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF47" s="111"/>
       <c r="EG47" s="111"/>
       <c r="EH47" s="111"/>
       <c r="EI47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ47" s="111"/>
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
       <c r="EP47" s="111"/>
       <c r="EQ47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER47" s="111"/>
       <c r="ES47" s="111"/>
@@ -20616,13 +20613,13 @@
       <c r="EW47" s="111"/>
       <c r="EX47" s="207"/>
       <c r="EY47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ47" s="208"/>
       <c r="FA47" s="208"/>
       <c r="FB47" s="208"/>
       <c r="FC47" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD47" s="111"/>
       <c r="FE47" s="111"/>
@@ -20721,7 +20718,7 @@
       <c r="AJ48" s="89"/>
       <c r="AK48" s="89"/>
       <c r="AL48" s="165" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="AM48" s="162"/>
       <c r="AN48" s="162"/>
@@ -20763,112 +20760,112 @@
       <c r="BX48" s="167"/>
       <c r="BY48" s="252"/>
       <c r="BZ48" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA48" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA48" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB48" s="111"/>
       <c r="CC48" s="111"/>
       <c r="CD48" s="111"/>
       <c r="CE48" s="111" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="CF48" s="111"/>
       <c r="CG48" s="111"/>
       <c r="CH48" s="111"/>
       <c r="CI48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ48" s="111"/>
       <c r="CK48" s="111"/>
       <c r="CL48" s="111"/>
       <c r="CM48" s="111" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="CN48" s="111"/>
       <c r="CO48" s="111"/>
       <c r="CP48" s="111"/>
       <c r="CQ48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR48" s="111"/>
       <c r="CS48" s="111"/>
       <c r="CT48" s="111"/>
       <c r="CU48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV48" s="111"/>
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
       <c r="DF48" s="111"/>
       <c r="DG48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH48" s="111"/>
       <c r="DI48" s="111"/>
       <c r="DJ48" s="111"/>
       <c r="DK48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL48" s="111"/>
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
       <c r="DR48" s="111"/>
       <c r="DS48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT48" s="111"/>
       <c r="DU48" s="111"/>
       <c r="DV48" s="111"/>
       <c r="DW48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX48" s="111"/>
       <c r="DY48" s="111"/>
       <c r="DZ48" s="111"/>
       <c r="EA48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB48" s="111"/>
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>795</v>
+        <v>851</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
       <c r="EL48" s="111"/>
       <c r="EM48" s="111" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="EN48" s="111"/>
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20878,13 +20875,13 @@
       <c r="EW48" s="111"/>
       <c r="EX48" s="111"/>
       <c r="EY48" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ48" s="111"/>
       <c r="FA48" s="111"/>
       <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -20983,7 +20980,7 @@
       <c r="AJ49" s="89"/>
       <c r="AK49" s="89"/>
       <c r="AL49" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM49" s="162"/>
       <c r="AN49" s="162"/>
@@ -21025,112 +21022,112 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="CA49" s="111" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="CB49" s="111"/>
       <c r="CC49" s="111"/>
       <c r="CD49" s="111"/>
       <c r="CE49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF49" s="111"/>
       <c r="CG49" s="111"/>
       <c r="CH49" s="111"/>
       <c r="CI49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ49" s="111"/>
       <c r="CK49" s="111"/>
       <c r="CL49" s="111"/>
       <c r="CM49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN49" s="111"/>
       <c r="CO49" s="111"/>
       <c r="CP49" s="111"/>
       <c r="CQ49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR49" s="111"/>
       <c r="CS49" s="111"/>
       <c r="CT49" s="111"/>
       <c r="CU49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV49" s="111"/>
       <c r="CW49" s="111"/>
       <c r="CX49" s="111"/>
       <c r="CY49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ49" s="111"/>
       <c r="DA49" s="111"/>
       <c r="DB49" s="111"/>
       <c r="DC49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD49" s="111"/>
       <c r="DE49" s="111"/>
       <c r="DF49" s="111"/>
       <c r="DG49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH49" s="111"/>
       <c r="DI49" s="111"/>
       <c r="DJ49" s="111"/>
       <c r="DK49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL49" s="111"/>
       <c r="DM49" s="111"/>
       <c r="DN49" s="111"/>
       <c r="DO49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP49" s="111"/>
       <c r="DQ49" s="111"/>
       <c r="DR49" s="111"/>
       <c r="DS49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT49" s="111"/>
       <c r="DU49" s="111"/>
       <c r="DV49" s="111"/>
       <c r="DW49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX49" s="111"/>
       <c r="DY49" s="111"/>
       <c r="DZ49" s="111"/>
       <c r="EA49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB49" s="111"/>
       <c r="EC49" s="111"/>
       <c r="ED49" s="111"/>
       <c r="EE49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF49" s="111"/>
       <c r="EG49" s="111"/>
       <c r="EH49" s="111"/>
       <c r="EI49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ49" s="111"/>
       <c r="EK49" s="111"/>
       <c r="EL49" s="111"/>
       <c r="EM49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN49" s="111"/>
       <c r="EO49" s="111"/>
       <c r="EP49" s="111"/>
       <c r="EQ49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER49" s="111"/>
       <c r="ES49" s="111"/>
@@ -21140,13 +21137,13 @@
       <c r="EW49" s="111"/>
       <c r="EX49" s="207"/>
       <c r="EY49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ49" s="208"/>
       <c r="FA49" s="208"/>
       <c r="FB49" s="208"/>
       <c r="FC49" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD49" s="111"/>
       <c r="FE49" s="111"/>
@@ -21245,7 +21242,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21287,112 +21284,112 @@
       <c r="BX50" s="167"/>
       <c r="BY50" s="252"/>
       <c r="BZ50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CA50" s="208" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
       <c r="CH50" s="111"/>
       <c r="CI50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ50" s="111"/>
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
       <c r="CP50" s="111"/>
       <c r="CQ50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR50" s="111"/>
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
       <c r="DF50" s="111"/>
       <c r="DG50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH50" s="111"/>
       <c r="DI50" s="111"/>
       <c r="DJ50" s="111"/>
       <c r="DK50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL50" s="111"/>
       <c r="DM50" s="111"/>
       <c r="DN50" s="111"/>
       <c r="DO50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP50" s="111"/>
       <c r="DQ50" s="111"/>
       <c r="DR50" s="111"/>
       <c r="DS50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT50" s="111"/>
       <c r="DU50" s="111"/>
       <c r="DV50" s="111"/>
       <c r="DW50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX50" s="111"/>
       <c r="DY50" s="111"/>
       <c r="DZ50" s="111"/>
       <c r="EA50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB50" s="111"/>
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>808</v>
+        <v>852</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21402,13 +21399,13 @@
       <c r="EW50" s="111"/>
       <c r="EX50" s="207"/>
       <c r="EY50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ50" s="208"/>
       <c r="FA50" s="208"/>
       <c r="FB50" s="208"/>
       <c r="FC50" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD50" s="111"/>
       <c r="FE50" s="111"/>
@@ -21507,7 +21504,7 @@
       <c r="AJ51" s="89"/>
       <c r="AK51" s="89"/>
       <c r="AL51" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM51" s="162"/>
       <c r="AN51" s="162"/>
@@ -21549,112 +21546,112 @@
       <c r="BX51" s="167"/>
       <c r="BY51" s="252"/>
       <c r="BZ51" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA51" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA51" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB51" s="111"/>
       <c r="CC51" s="111"/>
       <c r="CD51" s="111"/>
       <c r="CE51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF51" s="111"/>
       <c r="CG51" s="111"/>
       <c r="CH51" s="111"/>
       <c r="CI51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ51" s="111"/>
       <c r="CK51" s="111"/>
       <c r="CL51" s="111"/>
       <c r="CM51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN51" s="111"/>
       <c r="CO51" s="111"/>
       <c r="CP51" s="111"/>
       <c r="CQ51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR51" s="111"/>
       <c r="CS51" s="111"/>
       <c r="CT51" s="111"/>
       <c r="CU51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV51" s="111"/>
       <c r="CW51" s="111"/>
       <c r="CX51" s="111"/>
       <c r="CY51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ51" s="111"/>
       <c r="DA51" s="111"/>
       <c r="DB51" s="111"/>
       <c r="DC51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD51" s="111"/>
       <c r="DE51" s="111"/>
       <c r="DF51" s="111"/>
       <c r="DG51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH51" s="111"/>
       <c r="DI51" s="111"/>
       <c r="DJ51" s="111"/>
       <c r="DK51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL51" s="111"/>
       <c r="DM51" s="111"/>
       <c r="DN51" s="111"/>
       <c r="DO51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP51" s="111"/>
       <c r="DQ51" s="111"/>
       <c r="DR51" s="111"/>
       <c r="DS51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT51" s="111"/>
       <c r="DU51" s="111"/>
       <c r="DV51" s="111"/>
       <c r="DW51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX51" s="111"/>
       <c r="DY51" s="111"/>
       <c r="DZ51" s="111"/>
       <c r="EA51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB51" s="111"/>
       <c r="EC51" s="111"/>
       <c r="ED51" s="111"/>
       <c r="EE51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF51" s="111"/>
       <c r="EG51" s="111"/>
       <c r="EH51" s="111"/>
       <c r="EI51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ51" s="111"/>
       <c r="EK51" s="111"/>
       <c r="EL51" s="111"/>
       <c r="EM51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN51" s="111"/>
       <c r="EO51" s="111"/>
       <c r="EP51" s="111"/>
       <c r="EQ51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER51" s="111"/>
       <c r="ES51" s="111"/>
@@ -21664,13 +21661,13 @@
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
       <c r="FB51" s="208"/>
       <c r="FC51" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD51" s="111"/>
       <c r="FE51" s="111"/>
@@ -21769,7 +21766,7 @@
       <c r="AJ52" s="89"/>
       <c r="AK52" s="89"/>
       <c r="AL52" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM52" s="162"/>
       <c r="AN52" s="162"/>
@@ -21811,112 +21808,112 @@
       <c r="BX52" s="167"/>
       <c r="BY52" s="252"/>
       <c r="BZ52" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA52" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA52" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB52" s="111"/>
       <c r="CC52" s="111"/>
       <c r="CD52" s="111"/>
       <c r="CE52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF52" s="111"/>
       <c r="CG52" s="111"/>
       <c r="CH52" s="111"/>
       <c r="CI52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ52" s="111"/>
       <c r="CK52" s="111"/>
       <c r="CL52" s="111"/>
       <c r="CM52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN52" s="111"/>
       <c r="CO52" s="111"/>
       <c r="CP52" s="111"/>
       <c r="CQ52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR52" s="111"/>
       <c r="CS52" s="111"/>
       <c r="CT52" s="111"/>
       <c r="CU52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV52" s="111"/>
       <c r="CW52" s="111"/>
       <c r="CX52" s="111"/>
       <c r="CY52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ52" s="111"/>
       <c r="DA52" s="111"/>
       <c r="DB52" s="111"/>
       <c r="DC52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD52" s="111"/>
       <c r="DE52" s="111"/>
       <c r="DF52" s="111"/>
       <c r="DG52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH52" s="111"/>
       <c r="DI52" s="111"/>
       <c r="DJ52" s="111"/>
       <c r="DK52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL52" s="111"/>
       <c r="DM52" s="111"/>
       <c r="DN52" s="111"/>
       <c r="DO52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP52" s="111"/>
       <c r="DQ52" s="111"/>
       <c r="DR52" s="111"/>
       <c r="DS52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT52" s="111"/>
       <c r="DU52" s="111"/>
       <c r="DV52" s="111"/>
       <c r="DW52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX52" s="111"/>
       <c r="DY52" s="111"/>
       <c r="DZ52" s="111"/>
       <c r="EA52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB52" s="111"/>
       <c r="EC52" s="111"/>
       <c r="ED52" s="111"/>
       <c r="EE52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF52" s="111"/>
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
       <c r="EL52" s="111"/>
       <c r="EM52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN52" s="111"/>
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -21926,13 +21923,13 @@
       <c r="EW52" s="111"/>
       <c r="EX52" s="207"/>
       <c r="EY52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ52" s="208"/>
       <c r="FA52" s="208"/>
       <c r="FB52" s="208"/>
       <c r="FC52" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD52" s="111"/>
       <c r="FE52" s="111"/>
@@ -22043,7 +22040,7 @@
         <v>283</v>
       </c>
       <c r="AL53" s="165" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22133,112 +22130,112 @@
         <v>283</v>
       </c>
       <c r="BZ53" s="111" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="CA53" s="111" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="CB53" s="111"/>
       <c r="CC53" s="111"/>
       <c r="CD53" s="111"/>
       <c r="CE53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF53" s="111"/>
       <c r="CG53" s="111"/>
       <c r="CH53" s="111"/>
       <c r="CI53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ53" s="111"/>
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
       <c r="CP53" s="111"/>
       <c r="CQ53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR53" s="111"/>
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
       <c r="CX53" s="111"/>
       <c r="CY53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ53" s="111"/>
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
       <c r="DF53" s="111"/>
       <c r="DG53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH53" s="111"/>
       <c r="DI53" s="111"/>
       <c r="DJ53" s="111"/>
       <c r="DK53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL53" s="111"/>
       <c r="DM53" s="111"/>
       <c r="DN53" s="111"/>
       <c r="DO53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP53" s="111"/>
       <c r="DQ53" s="111"/>
       <c r="DR53" s="111"/>
       <c r="DS53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT53" s="111"/>
       <c r="DU53" s="111"/>
       <c r="DV53" s="111"/>
       <c r="DW53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX53" s="111"/>
       <c r="DY53" s="111"/>
       <c r="DZ53" s="111"/>
       <c r="EA53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB53" s="111"/>
       <c r="EC53" s="111"/>
       <c r="ED53" s="111"/>
       <c r="EE53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF53" s="111"/>
       <c r="EG53" s="111"/>
       <c r="EH53" s="111"/>
       <c r="EI53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ53" s="111"/>
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
       <c r="EP53" s="111"/>
       <c r="EQ53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER53" s="111"/>
       <c r="ES53" s="111"/>
@@ -22248,13 +22245,13 @@
       <c r="EW53" s="111"/>
       <c r="EX53" s="207"/>
       <c r="EY53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ53" s="208"/>
       <c r="FA53" s="208"/>
       <c r="FB53" s="208"/>
       <c r="FC53" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD53" s="111"/>
       <c r="FE53" s="111"/>
@@ -22323,7 +22320,7 @@
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
       <c r="H54" s="110" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="I54" s="110" t="s">
         <v>545</v>
@@ -22357,7 +22354,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22399,46 +22396,46 @@
       <c r="BX54" s="167"/>
       <c r="BY54" s="252"/>
       <c r="BZ54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CA54" s="208" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="CB54" s="111"/>
       <c r="CC54" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD54" s="111" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="CE54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF54" s="111"/>
       <c r="CG54" s="111"/>
       <c r="CH54" s="111"/>
       <c r="CI54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ54" s="111"/>
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="CN54" s="111"/>
       <c r="CO54" s="111" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR54" s="111"/>
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="CV54" s="111"/>
       <c r="CW54" s="111" t="s">
@@ -22446,7 +22443,7 @@
       </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="CZ54" s="111" t="s">
         <v>547</v>
@@ -22456,7 +22453,7 @@
       </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="DD54" s="111" t="s">
         <v>546</v>
@@ -22464,47 +22461,47 @@
       <c r="DE54" s="111"/>
       <c r="DF54" s="111"/>
       <c r="DG54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH54" s="111"/>
       <c r="DI54" s="111"/>
       <c r="DJ54" s="111"/>
       <c r="DK54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL54" s="111"/>
       <c r="DM54" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN54" s="111" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="DO54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP54" s="111"/>
       <c r="DQ54" s="111"/>
       <c r="DR54" s="111"/>
       <c r="DS54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT54" s="111"/>
       <c r="DU54" s="111"/>
       <c r="DV54" s="111"/>
       <c r="DW54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX54" s="111"/>
       <c r="DY54" s="111"/>
       <c r="DZ54" s="111"/>
       <c r="EA54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB54" s="111"/>
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>824</v>
+        <v>853</v>
       </c>
       <c r="EF54" s="111"/>
       <c r="EG54" s="111" t="s">
@@ -22512,7 +22509,7 @@
       </c>
       <c r="EH54" s="111"/>
       <c r="EI54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ54" s="111"/>
       <c r="EK54" s="111" t="s">
@@ -22520,13 +22517,13 @@
       </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
       <c r="EP54" s="111"/>
       <c r="EQ54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER54" s="111"/>
       <c r="ES54" s="111" t="s">
@@ -22538,13 +22535,13 @@
       <c r="EW54" s="111"/>
       <c r="EX54" s="207"/>
       <c r="EY54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ54" s="208"/>
       <c r="FA54" s="208"/>
       <c r="FB54" s="208"/>
       <c r="FC54" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD54" s="111"/>
       <c r="FE54" s="111"/>
@@ -22613,7 +22610,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
       <c r="H55" s="110" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="I55" s="110" t="s">
         <v>545</v>
@@ -22647,11 +22644,11 @@
       <c r="AJ55" s="89"/>
       <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="AM55" s="162"/>
       <c r="AN55" s="162" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
@@ -22691,46 +22688,46 @@
       <c r="BX55" s="167"/>
       <c r="BY55" s="252"/>
       <c r="BZ55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CA55" s="208" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="CB55" s="111"/>
       <c r="CC55" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD55" s="111" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="CE55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF55" s="111"/>
       <c r="CG55" s="111"/>
       <c r="CH55" s="111"/>
       <c r="CI55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ55" s="111"/>
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="CN55" s="111"/>
       <c r="CO55" s="111" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR55" s="111"/>
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="CV55" s="111"/>
       <c r="CW55" s="111" t="s">
@@ -22738,13 +22735,13 @@
       </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
       <c r="DB55" s="111"/>
       <c r="DC55" s="111" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="DD55" s="111" t="s">
         <v>546</v>
@@ -22752,65 +22749,65 @@
       <c r="DE55" s="111"/>
       <c r="DF55" s="111"/>
       <c r="DG55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH55" s="111"/>
       <c r="DI55" s="111"/>
       <c r="DJ55" s="111"/>
       <c r="DK55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL55" s="111"/>
       <c r="DM55" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN55" s="111" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="DO55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP55" s="111"/>
       <c r="DQ55" s="111"/>
       <c r="DR55" s="111"/>
       <c r="DS55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT55" s="111"/>
       <c r="DU55" s="111"/>
       <c r="DV55" s="111"/>
       <c r="DW55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX55" s="111"/>
       <c r="DY55" s="111"/>
       <c r="DZ55" s="111"/>
       <c r="EA55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB55" s="111"/>
       <c r="EC55" s="111"/>
       <c r="ED55" s="111"/>
       <c r="EE55" s="111" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="EF55" s="111"/>
       <c r="EG55" s="111"/>
       <c r="EH55" s="111"/>
       <c r="EI55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ55" s="111"/>
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
       <c r="EP55" s="111"/>
       <c r="EQ55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER55" s="111"/>
       <c r="ES55" s="111"/>
@@ -22820,13 +22817,13 @@
       <c r="EW55" s="111"/>
       <c r="EX55" s="207"/>
       <c r="EY55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ55" s="208"/>
       <c r="FA55" s="208"/>
       <c r="FB55" s="208"/>
       <c r="FC55" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD55" s="111"/>
       <c r="FE55" s="111"/>
@@ -22925,7 +22922,7 @@
       <c r="AJ56" s="89"/>
       <c r="AK56" s="89"/>
       <c r="AL56" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM56" s="162"/>
       <c r="AN56" s="162"/>
@@ -22967,112 +22964,112 @@
       <c r="BX56" s="167"/>
       <c r="BY56" s="252"/>
       <c r="BZ56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CA56" s="208" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
       <c r="CH56" s="111"/>
       <c r="CI56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ56" s="111"/>
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
       <c r="CP56" s="111"/>
       <c r="CQ56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR56" s="111"/>
       <c r="CS56" s="111"/>
       <c r="CT56" s="111"/>
       <c r="CU56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV56" s="111"/>
       <c r="CW56" s="111"/>
       <c r="CX56" s="111"/>
       <c r="CY56" s="111" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="CZ56" s="111"/>
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
       <c r="DF56" s="111"/>
       <c r="DG56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH56" s="111"/>
       <c r="DI56" s="111"/>
       <c r="DJ56" s="111"/>
       <c r="DK56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL56" s="111"/>
       <c r="DM56" s="111"/>
       <c r="DN56" s="111"/>
       <c r="DO56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP56" s="111"/>
       <c r="DQ56" s="111"/>
       <c r="DR56" s="111"/>
       <c r="DS56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT56" s="111"/>
       <c r="DU56" s="111"/>
       <c r="DV56" s="111"/>
       <c r="DW56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX56" s="111"/>
       <c r="DY56" s="111"/>
       <c r="DZ56" s="111"/>
       <c r="EA56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB56" s="111"/>
       <c r="EC56" s="111"/>
       <c r="ED56" s="111"/>
       <c r="EE56" s="111" t="s">
-        <v>837</v>
+        <v>854</v>
       </c>
       <c r="EF56" s="111"/>
       <c r="EG56" s="111"/>
       <c r="EH56" s="111"/>
       <c r="EI56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ56" s="111"/>
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
       <c r="EP56" s="111"/>
       <c r="EQ56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER56" s="111"/>
       <c r="ES56" s="111"/>
@@ -23082,13 +23079,13 @@
       <c r="EW56" s="111"/>
       <c r="EX56" s="207"/>
       <c r="EY56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ56" s="208"/>
       <c r="FA56" s="208"/>
       <c r="FB56" s="208"/>
       <c r="FC56" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD56" s="111"/>
       <c r="FE56" s="111"/>
@@ -23187,7 +23184,7 @@
       <c r="AJ57" s="89"/>
       <c r="AK57" s="89"/>
       <c r="AL57" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM57" s="162"/>
       <c r="AN57" s="162"/>
@@ -23229,112 +23226,112 @@
       <c r="BX57" s="167"/>
       <c r="BY57" s="252"/>
       <c r="BZ57" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA57" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA57" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB57" s="111"/>
       <c r="CC57" s="111"/>
       <c r="CD57" s="111"/>
       <c r="CE57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF57" s="111"/>
       <c r="CG57" s="111"/>
       <c r="CH57" s="111"/>
       <c r="CI57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ57" s="111"/>
       <c r="CK57" s="111"/>
       <c r="CL57" s="111"/>
       <c r="CM57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN57" s="111"/>
       <c r="CO57" s="111"/>
       <c r="CP57" s="111"/>
       <c r="CQ57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR57" s="111"/>
       <c r="CS57" s="111"/>
       <c r="CT57" s="111"/>
       <c r="CU57" s="111" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="CV57" s="111"/>
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
       <c r="DB57" s="111"/>
       <c r="DC57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD57" s="111"/>
       <c r="DE57" s="111"/>
       <c r="DF57" s="111"/>
       <c r="DG57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH57" s="111"/>
       <c r="DI57" s="111"/>
       <c r="DJ57" s="111"/>
       <c r="DK57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL57" s="111"/>
       <c r="DM57" s="111"/>
       <c r="DN57" s="111"/>
       <c r="DO57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP57" s="111"/>
       <c r="DQ57" s="111"/>
       <c r="DR57" s="111"/>
       <c r="DS57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT57" s="111"/>
       <c r="DU57" s="111"/>
       <c r="DV57" s="111"/>
       <c r="DW57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX57" s="111"/>
       <c r="DY57" s="111"/>
       <c r="DZ57" s="111"/>
       <c r="EA57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB57" s="111"/>
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>840</v>
+        <v>856</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
       <c r="EH57" s="111"/>
       <c r="EI57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ57" s="111"/>
       <c r="EK57" s="111"/>
       <c r="EL57" s="111"/>
       <c r="EM57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN57" s="111"/>
       <c r="EO57" s="111"/>
       <c r="EP57" s="111"/>
       <c r="EQ57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER57" s="111"/>
       <c r="ES57" s="111"/>
@@ -23344,13 +23341,13 @@
       <c r="EW57" s="111"/>
       <c r="EX57" s="207"/>
       <c r="EY57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ57" s="208"/>
       <c r="FA57" s="208"/>
       <c r="FB57" s="208"/>
       <c r="FC57" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD57" s="111"/>
       <c r="FE57" s="111"/>
@@ -23449,7 +23446,7 @@
       <c r="AJ58" s="90"/>
       <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23491,112 +23488,112 @@
       <c r="BX58" s="167"/>
       <c r="BY58" s="252"/>
       <c r="BZ58" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA58" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA58" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB58" s="111"/>
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
       <c r="CH58" s="111"/>
       <c r="CI58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ58" s="111"/>
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
       <c r="CP58" s="111"/>
       <c r="CQ58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR58" s="111"/>
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
       <c r="DF58" s="111"/>
       <c r="DG58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH58" s="111"/>
       <c r="DI58" s="111"/>
       <c r="DJ58" s="111"/>
       <c r="DK58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL58" s="111"/>
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
       <c r="DR58" s="111"/>
       <c r="DS58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT58" s="111"/>
       <c r="DU58" s="111"/>
       <c r="DV58" s="111"/>
       <c r="DW58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX58" s="111"/>
       <c r="DY58" s="111"/>
       <c r="DZ58" s="111"/>
       <c r="EA58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB58" s="111"/>
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>847</v>
+        <v>855</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23606,13 +23603,13 @@
       <c r="EW58" s="111"/>
       <c r="EX58" s="207"/>
       <c r="EY58" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ58" s="208"/>
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
       <c r="FC58" s="208" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23711,7 +23708,7 @@
       <c r="AJ59" s="90"/>
       <c r="AK59" s="90"/>
       <c r="AL59" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM59" s="162"/>
       <c r="AN59" s="162"/>
@@ -23753,112 +23750,112 @@
       <c r="BX59" s="167"/>
       <c r="BY59" s="252"/>
       <c r="BZ59" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA59" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA59" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB59" s="111"/>
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
       <c r="CH59" s="111"/>
       <c r="CI59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ59" s="111"/>
       <c r="CK59" s="111"/>
       <c r="CL59" s="111"/>
       <c r="CM59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN59" s="111"/>
       <c r="CO59" s="111"/>
       <c r="CP59" s="111"/>
       <c r="CQ59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CR59" s="111"/>
       <c r="CS59" s="111"/>
       <c r="CT59" s="111"/>
       <c r="CU59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV59" s="111"/>
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
       <c r="DB59" s="111"/>
       <c r="DC59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD59" s="111"/>
       <c r="DE59" s="111"/>
       <c r="DF59" s="111"/>
       <c r="DG59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH59" s="111"/>
       <c r="DI59" s="111"/>
       <c r="DJ59" s="111"/>
       <c r="DK59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL59" s="111"/>
       <c r="DM59" s="111"/>
       <c r="DN59" s="111"/>
       <c r="DO59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP59" s="111"/>
       <c r="DQ59" s="111"/>
       <c r="DR59" s="111"/>
       <c r="DS59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT59" s="111"/>
       <c r="DU59" s="111"/>
       <c r="DV59" s="111"/>
       <c r="DW59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX59" s="111"/>
       <c r="DY59" s="111"/>
       <c r="DZ59" s="111"/>
       <c r="EA59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB59" s="111"/>
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>837</v>
+        <v>851</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
       <c r="EH59" s="111"/>
       <c r="EI59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ59" s="111"/>
       <c r="EK59" s="111"/>
       <c r="EL59" s="111"/>
       <c r="EM59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN59" s="111"/>
       <c r="EO59" s="111"/>
       <c r="EP59" s="111"/>
       <c r="EQ59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER59" s="111"/>
       <c r="ES59" s="111"/>
@@ -23868,13 +23865,13 @@
       <c r="EW59" s="111"/>
       <c r="EX59" s="207"/>
       <c r="EY59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ59" s="208"/>
       <c r="FA59" s="208"/>
       <c r="FB59" s="208"/>
       <c r="FC59" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="FD59" s="111"/>
       <c r="FE59" s="111"/>
@@ -23973,7 +23970,7 @@
       <c r="AJ60" s="90"/>
       <c r="AK60" s="90"/>
       <c r="AL60" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="AM60" s="162"/>
       <c r="AN60" s="162"/>
@@ -24015,112 +24012,112 @@
       <c r="BX60" s="167"/>
       <c r="BY60" s="252"/>
       <c r="BZ60" s="111" t="s">
+        <v>784</v>
+      </c>
+      <c r="CA60" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="CA60" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="CB60" s="111"/>
       <c r="CC60" s="111"/>
       <c r="CD60" s="111"/>
       <c r="CE60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CF60" s="111"/>
       <c r="CG60" s="111"/>
       <c r="CH60" s="111"/>
       <c r="CI60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CJ60" s="111"/>
       <c r="CK60" s="111"/>
       <c r="CL60" s="111"/>
       <c r="CM60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CN60" s="111"/>
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
       <c r="CT60" s="111"/>
       <c r="CU60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CV60" s="111"/>
       <c r="CW60" s="111"/>
       <c r="CX60" s="111"/>
       <c r="CY60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ60" s="111"/>
       <c r="DA60" s="111"/>
       <c r="DB60" s="111"/>
       <c r="DC60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DD60" s="111"/>
       <c r="DE60" s="111"/>
       <c r="DF60" s="111"/>
       <c r="DG60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DH60" s="111"/>
       <c r="DI60" s="111"/>
       <c r="DJ60" s="111"/>
       <c r="DK60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DL60" s="111"/>
       <c r="DM60" s="111"/>
       <c r="DN60" s="111"/>
       <c r="DO60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DP60" s="111"/>
       <c r="DQ60" s="111"/>
       <c r="DR60" s="111"/>
       <c r="DS60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DT60" s="111"/>
       <c r="DU60" s="111"/>
       <c r="DV60" s="111"/>
       <c r="DW60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="DX60" s="111"/>
       <c r="DY60" s="111"/>
       <c r="DZ60" s="111"/>
       <c r="EA60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EB60" s="111"/>
       <c r="EC60" s="111"/>
       <c r="ED60" s="111"/>
       <c r="EE60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EF60" s="111"/>
       <c r="EG60" s="111"/>
       <c r="EH60" s="111"/>
       <c r="EI60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EJ60" s="111"/>
       <c r="EK60" s="111"/>
       <c r="EL60" s="111"/>
       <c r="EM60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EN60" s="111"/>
       <c r="EO60" s="111"/>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="ER60" s="111"/>
       <c r="ES60" s="111"/>
@@ -24130,13 +24127,13 @@
       <c r="EW60" s="111"/>
       <c r="EX60" s="207"/>
       <c r="EY60" s="111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="EZ60" s="208"/>
       <c r="FA60" s="208"/>
       <c r="FB60" s="208"/>
       <c r="FC60" s="208" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="FD60" s="111"/>
       <c r="FE60" s="111"/>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Fix error in cmd_bio where units were not parsed
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="858">
   <si>
     <t>Name</t>
   </si>
@@ -2605,6 +2605,9 @@
   </si>
   <si>
     <t>[0.7; 1.99 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 1.5 ug/L]</t>
   </si>
 </sst>
 </file>
@@ -5555,10 +5558,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CI32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CQ32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EE55" sqref="EE55"/>
+      <selection pane="bottomRight" activeCell="DK47" sqref="DK47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -20555,7 +20558,7 @@
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>784</v>
+        <v>857</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Finalize propofol sedation update
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="860">
   <si>
     <t>Name</t>
   </si>
@@ -2226,12 +2226,6 @@
     <t>0.1 mL/min kg</t>
   </si>
   <si>
-    <t>13000 mL/min kg</t>
-  </si>
-  <si>
-    <t>40.0 mL/min kg</t>
-  </si>
-  <si>
     <t>Blood_ABNegative</t>
   </si>
   <si>
@@ -2589,25 +2583,37 @@
     <t>[0.5; 0.4 ug/L]</t>
   </si>
   <si>
-    <t>[-0.25; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.15; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.5; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.55; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.7; 1.99 ug/mL]</t>
-  </si>
-  <si>
     <t>[0; 1.5 ug/L]</t>
+  </si>
+  <si>
+    <t>3350 mL/min kg</t>
+  </si>
+  <si>
+    <t>28.0 mL/min kg</t>
+  </si>
+  <si>
+    <t>[1.0; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.75; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1.0; 1.2 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.25; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.15; 2.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.5; 2.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 1.5 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5558,10 +5564,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CQ32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DG33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DK47" sqref="DK47"/>
+      <selection pane="bottomRight" activeCell="EE55" sqref="EE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6528,7 +6534,7 @@
         <v>165</v>
       </c>
       <c r="BZ2" s="96" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="CA2" s="257" t="s">
         <v>190</v>
@@ -6879,64 +6885,64 @@
         <v>563</v>
       </c>
       <c r="GM2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="GN2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="GO2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="GP2" s="101" t="s">
+        <v>735</v>
+      </c>
+      <c r="GQ2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GN2" s="101" t="s">
+      <c r="GR2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GO2" s="101" t="s">
+      <c r="GS2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GP2" s="101" t="s">
+      <c r="GT2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GQ2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GR2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GS2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GT2" s="101" t="s">
-        <v>739</v>
-      </c>
       <c r="GU2" s="101" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="GV2" s="101" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="GW2" s="101" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="GX2" s="101" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="GY2" s="101" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="GZ2" s="101" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="HA2" s="101" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="HB2" s="101" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="HC2" s="101" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="HD2" s="101" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="HE2" s="101" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="HF2" s="101" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="3" spans="1:214" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -7993,31 +7999,31 @@
       <c r="GK5" s="178"/>
       <c r="GL5" s="178"/>
       <c r="GM5" s="245" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="GN5" s="246"/>
       <c r="GO5" s="246"/>
       <c r="GP5" s="246"/>
       <c r="GQ5" s="245" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="GR5" s="246"/>
       <c r="GS5" s="246"/>
       <c r="GT5" s="246"/>
       <c r="GU5" s="245" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="GV5" s="246"/>
       <c r="GW5" s="246"/>
       <c r="GX5" s="246"/>
       <c r="GY5" s="245" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="GZ5" s="246"/>
       <c r="HA5" s="246"/>
       <c r="HB5" s="246"/>
       <c r="HC5" s="245" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="HD5" s="221"/>
       <c r="HE5" s="221"/>
@@ -8116,7 +8122,7 @@
       <c r="BX6" s="167"/>
       <c r="BY6" s="252"/>
       <c r="BZ6" s="107" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="CA6" s="258" t="s">
         <v>124</v>
@@ -8249,19 +8255,19 @@
       <c r="GS6" s="246"/>
       <c r="GT6" s="246"/>
       <c r="GU6" s="249" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="GV6" s="246"/>
       <c r="GW6" s="246"/>
       <c r="GX6" s="246"/>
       <c r="GY6" s="249" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="GZ6" s="246"/>
       <c r="HA6" s="246"/>
       <c r="HB6" s="246"/>
       <c r="HC6" s="249" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="HD6" s="221"/>
       <c r="HE6" s="221"/>
@@ -9060,7 +9066,7 @@
       <c r="BX10" s="167"/>
       <c r="BY10" s="252"/>
       <c r="BZ10" s="107" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="CA10" s="258" t="s">
         <v>312</v>
@@ -9237,31 +9243,31 @@
       <c r="GK10" s="178"/>
       <c r="GL10" s="178"/>
       <c r="GM10" s="245" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="GN10" s="246"/>
       <c r="GO10" s="246"/>
       <c r="GP10" s="246"/>
       <c r="GQ10" s="245" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="GR10" s="246"/>
       <c r="GS10" s="246"/>
       <c r="GT10" s="246"/>
       <c r="GU10" s="245" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="GV10" s="246"/>
       <c r="GW10" s="246"/>
       <c r="GX10" s="246"/>
       <c r="GY10" s="245" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="GZ10" s="246"/>
       <c r="HA10" s="246"/>
       <c r="HB10" s="246"/>
       <c r="HC10" s="245" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="HD10" s="221"/>
       <c r="HE10" s="221"/>
@@ -12125,7 +12131,7 @@
       <c r="EC20" s="107"/>
       <c r="ED20" s="107"/>
       <c r="EE20" s="107" t="s">
-        <v>730</v>
+        <v>850</v>
       </c>
       <c r="EF20" s="107"/>
       <c r="EG20" s="107"/>
@@ -12312,7 +12318,7 @@
       <c r="BX21" s="167"/>
       <c r="BY21" s="252"/>
       <c r="BZ21" s="107" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="CA21" s="258" t="s">
         <v>528</v>
@@ -12572,7 +12578,7 @@
         <v>591</v>
       </c>
       <c r="AV22" s="162" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="AW22" s="162"/>
       <c r="AX22" s="167"/>
@@ -12699,7 +12705,7 @@
       <c r="EC22" s="107"/>
       <c r="ED22" s="107"/>
       <c r="EE22" s="107" t="s">
-        <v>731</v>
+        <v>851</v>
       </c>
       <c r="EF22" s="107"/>
       <c r="EG22" s="107"/>
@@ -13372,7 +13378,7 @@
       <c r="BX24" s="167"/>
       <c r="BY24" s="252"/>
       <c r="BZ24" s="107" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="CA24" s="258" t="str">
         <f>CA21</f>
@@ -15201,7 +15207,7 @@
     </row>
     <row r="30" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="79" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B30" s="222"/>
       <c r="C30" s="223" t="s">
@@ -15691,7 +15697,7 @@
     </row>
     <row r="31" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="80" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B31" s="99"/>
       <c r="C31" s="99"/>
@@ -15887,31 +15893,31 @@
       <c r="GK31" s="177"/>
       <c r="GL31" s="177"/>
       <c r="GM31" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GN31" s="245"/>
       <c r="GO31" s="245"/>
       <c r="GP31" s="245"/>
       <c r="GQ31" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GR31" s="245"/>
       <c r="GS31" s="245"/>
       <c r="GT31" s="245"/>
       <c r="GU31" s="245" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="GV31" s="245"/>
       <c r="GW31" s="245"/>
       <c r="GX31" s="245"/>
       <c r="GY31" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GZ31" s="245"/>
       <c r="HA31" s="245"/>
       <c r="HB31" s="245"/>
       <c r="HC31" s="245" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="HD31" s="220"/>
       <c r="HE31" s="220"/>
@@ -15919,7 +15925,7 @@
     </row>
     <row r="32" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="80" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B32" s="99"/>
       <c r="C32" s="99"/>
@@ -16115,31 +16121,31 @@
       <c r="GK32" s="177"/>
       <c r="GL32" s="177"/>
       <c r="GM32" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GN32" s="245"/>
       <c r="GO32" s="245"/>
       <c r="GP32" s="245"/>
       <c r="GQ32" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GR32" s="245"/>
       <c r="GS32" s="245"/>
       <c r="GT32" s="245"/>
       <c r="GU32" s="245" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="GV32" s="245"/>
       <c r="GW32" s="245"/>
       <c r="GX32" s="245"/>
       <c r="GY32" s="245" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="GZ32" s="245"/>
       <c r="HA32" s="245"/>
       <c r="HB32" s="245"/>
       <c r="HC32" s="245" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="HD32" s="220"/>
       <c r="HE32" s="220"/>
@@ -16765,7 +16771,7 @@
       <c r="DE34" s="107"/>
       <c r="DF34" s="107"/>
       <c r="DG34" s="107" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="DH34" s="107"/>
       <c r="DI34" s="107"/>
@@ -19738,7 +19744,7 @@
       <c r="EC44" s="111"/>
       <c r="ED44" s="111"/>
       <c r="EE44" s="111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="EF44" s="111"/>
       <c r="EG44" s="111"/>
@@ -20133,14 +20139,14 @@
       <c r="AJ46" s="89"/>
       <c r="AK46" s="89"/>
       <c r="AL46" s="165" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="AM46" s="162"/>
       <c r="AN46" s="162" t="s">
         <v>285</v>
       </c>
       <c r="AO46" s="162" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="AP46" s="162"/>
       <c r="AQ46" s="162"/>
@@ -20179,112 +20185,112 @@
       <c r="BX46" s="167"/>
       <c r="BY46" s="252"/>
       <c r="BZ46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA46" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB46" s="111"/>
       <c r="CC46" s="111"/>
       <c r="CD46" s="111"/>
       <c r="CE46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF46" s="111"/>
       <c r="CG46" s="111"/>
       <c r="CH46" s="111"/>
       <c r="CI46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ46" s="111"/>
       <c r="CK46" s="111"/>
       <c r="CL46" s="111"/>
       <c r="CM46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN46" s="111"/>
       <c r="CO46" s="111"/>
       <c r="CP46" s="111"/>
       <c r="CQ46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR46" s="111"/>
       <c r="CS46" s="111"/>
       <c r="CT46" s="111"/>
       <c r="CU46" s="111" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="CV46" s="111"/>
       <c r="CW46" s="111"/>
       <c r="CX46" s="111"/>
       <c r="CY46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ46" s="111"/>
       <c r="DA46" s="111"/>
       <c r="DB46" s="111"/>
       <c r="DC46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD46" s="111"/>
       <c r="DE46" s="111"/>
       <c r="DF46" s="111"/>
       <c r="DG46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH46" s="111"/>
       <c r="DI46" s="111"/>
       <c r="DJ46" s="111"/>
       <c r="DK46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL46" s="111"/>
       <c r="DM46" s="111"/>
       <c r="DN46" s="111"/>
       <c r="DO46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP46" s="111"/>
       <c r="DQ46" s="111"/>
       <c r="DR46" s="111"/>
       <c r="DS46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT46" s="111"/>
       <c r="DU46" s="111"/>
       <c r="DV46" s="111"/>
       <c r="DW46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX46" s="111"/>
       <c r="DY46" s="111"/>
       <c r="DZ46" s="111"/>
       <c r="EA46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB46" s="111"/>
       <c r="EC46" s="111"/>
       <c r="ED46" s="111"/>
       <c r="EE46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF46" s="111"/>
       <c r="EG46" s="111"/>
       <c r="EH46" s="111"/>
       <c r="EI46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ46" s="111"/>
       <c r="EK46" s="111"/>
       <c r="EL46" s="111"/>
       <c r="EM46" s="111" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="EN46" s="111"/>
       <c r="EO46" s="111"/>
       <c r="EP46" s="111"/>
       <c r="EQ46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER46" s="111"/>
       <c r="ES46" s="111"/>
@@ -20294,13 +20300,13 @@
       <c r="EW46" s="111"/>
       <c r="EX46" s="111"/>
       <c r="EY46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ46" s="111"/>
       <c r="FA46" s="111"/>
       <c r="FB46" s="111"/>
       <c r="FC46" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD46" s="111"/>
       <c r="FE46" s="111"/>
@@ -20411,7 +20417,7 @@
         <v>283</v>
       </c>
       <c r="AL47" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM47" s="162"/>
       <c r="AN47" s="162"/>
@@ -20501,112 +20507,112 @@
         <v>283</v>
       </c>
       <c r="BZ47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA47" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB47" s="111"/>
       <c r="CC47" s="111"/>
       <c r="CD47" s="111"/>
       <c r="CE47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF47" s="111"/>
       <c r="CG47" s="111"/>
       <c r="CH47" s="111"/>
       <c r="CI47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ47" s="111"/>
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
       <c r="CP47" s="111"/>
       <c r="CQ47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR47" s="111"/>
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
       <c r="CX47" s="111"/>
       <c r="CY47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ47" s="111"/>
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
       <c r="DF47" s="111"/>
       <c r="DG47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH47" s="111"/>
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>
       <c r="DN47" s="111"/>
       <c r="DO47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP47" s="111"/>
       <c r="DQ47" s="111"/>
       <c r="DR47" s="111"/>
       <c r="DS47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT47" s="111"/>
       <c r="DU47" s="111"/>
       <c r="DV47" s="111"/>
       <c r="DW47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX47" s="111"/>
       <c r="DY47" s="111"/>
       <c r="DZ47" s="111"/>
       <c r="EA47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB47" s="111"/>
       <c r="EC47" s="111"/>
       <c r="ED47" s="111"/>
       <c r="EE47" s="111" t="s">
-        <v>784</v>
+        <v>852</v>
       </c>
       <c r="EF47" s="111"/>
       <c r="EG47" s="111"/>
       <c r="EH47" s="111"/>
       <c r="EI47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ47" s="111"/>
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
       <c r="EP47" s="111"/>
       <c r="EQ47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER47" s="111"/>
       <c r="ES47" s="111"/>
@@ -20616,13 +20622,13 @@
       <c r="EW47" s="111"/>
       <c r="EX47" s="207"/>
       <c r="EY47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ47" s="208"/>
       <c r="FA47" s="208"/>
       <c r="FB47" s="208"/>
       <c r="FC47" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD47" s="111"/>
       <c r="FE47" s="111"/>
@@ -20721,7 +20727,7 @@
       <c r="AJ48" s="89"/>
       <c r="AK48" s="89"/>
       <c r="AL48" s="165" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="AM48" s="162"/>
       <c r="AN48" s="162"/>
@@ -20763,112 +20769,112 @@
       <c r="BX48" s="167"/>
       <c r="BY48" s="252"/>
       <c r="BZ48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA48" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB48" s="111"/>
       <c r="CC48" s="111"/>
       <c r="CD48" s="111"/>
       <c r="CE48" s="111" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="CF48" s="111"/>
       <c r="CG48" s="111"/>
       <c r="CH48" s="111"/>
       <c r="CI48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ48" s="111"/>
       <c r="CK48" s="111"/>
       <c r="CL48" s="111"/>
       <c r="CM48" s="111" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="CN48" s="111"/>
       <c r="CO48" s="111"/>
       <c r="CP48" s="111"/>
       <c r="CQ48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR48" s="111"/>
       <c r="CS48" s="111"/>
       <c r="CT48" s="111"/>
       <c r="CU48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV48" s="111"/>
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
       <c r="DF48" s="111"/>
       <c r="DG48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH48" s="111"/>
       <c r="DI48" s="111"/>
       <c r="DJ48" s="111"/>
       <c r="DK48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL48" s="111"/>
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
       <c r="DR48" s="111"/>
       <c r="DS48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT48" s="111"/>
       <c r="DU48" s="111"/>
       <c r="DV48" s="111"/>
       <c r="DW48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX48" s="111"/>
       <c r="DY48" s="111"/>
       <c r="DZ48" s="111"/>
       <c r="EA48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB48" s="111"/>
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
       <c r="EL48" s="111"/>
       <c r="EM48" s="111" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="EN48" s="111"/>
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20878,13 +20884,13 @@
       <c r="EW48" s="111"/>
       <c r="EX48" s="111"/>
       <c r="EY48" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ48" s="111"/>
       <c r="FA48" s="111"/>
       <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -20944,7 +20950,7 @@
     </row>
     <row r="49" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="62" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="110"/>
@@ -20983,7 +20989,7 @@
       <c r="AJ49" s="89"/>
       <c r="AK49" s="89"/>
       <c r="AL49" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM49" s="162"/>
       <c r="AN49" s="162"/>
@@ -21025,112 +21031,112 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="CA49" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB49" s="111"/>
       <c r="CC49" s="111"/>
       <c r="CD49" s="111"/>
       <c r="CE49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF49" s="111"/>
       <c r="CG49" s="111"/>
       <c r="CH49" s="111"/>
       <c r="CI49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ49" s="111"/>
       <c r="CK49" s="111"/>
       <c r="CL49" s="111"/>
       <c r="CM49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN49" s="111"/>
       <c r="CO49" s="111"/>
       <c r="CP49" s="111"/>
       <c r="CQ49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR49" s="111"/>
       <c r="CS49" s="111"/>
       <c r="CT49" s="111"/>
       <c r="CU49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV49" s="111"/>
       <c r="CW49" s="111"/>
       <c r="CX49" s="111"/>
       <c r="CY49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ49" s="111"/>
       <c r="DA49" s="111"/>
       <c r="DB49" s="111"/>
       <c r="DC49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD49" s="111"/>
       <c r="DE49" s="111"/>
       <c r="DF49" s="111"/>
       <c r="DG49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH49" s="111"/>
       <c r="DI49" s="111"/>
       <c r="DJ49" s="111"/>
       <c r="DK49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL49" s="111"/>
       <c r="DM49" s="111"/>
       <c r="DN49" s="111"/>
       <c r="DO49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP49" s="111"/>
       <c r="DQ49" s="111"/>
       <c r="DR49" s="111"/>
       <c r="DS49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT49" s="111"/>
       <c r="DU49" s="111"/>
       <c r="DV49" s="111"/>
       <c r="DW49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX49" s="111"/>
       <c r="DY49" s="111"/>
       <c r="DZ49" s="111"/>
       <c r="EA49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB49" s="111"/>
       <c r="EC49" s="111"/>
       <c r="ED49" s="111"/>
       <c r="EE49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF49" s="111"/>
       <c r="EG49" s="111"/>
       <c r="EH49" s="111"/>
       <c r="EI49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ49" s="111"/>
       <c r="EK49" s="111"/>
       <c r="EL49" s="111"/>
       <c r="EM49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN49" s="111"/>
       <c r="EO49" s="111"/>
       <c r="EP49" s="111"/>
       <c r="EQ49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER49" s="111"/>
       <c r="ES49" s="111"/>
@@ -21140,13 +21146,13 @@
       <c r="EW49" s="111"/>
       <c r="EX49" s="207"/>
       <c r="EY49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ49" s="208"/>
       <c r="FA49" s="208"/>
       <c r="FB49" s="208"/>
       <c r="FC49" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD49" s="111"/>
       <c r="FE49" s="111"/>
@@ -21245,7 +21251,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21287,112 +21293,112 @@
       <c r="BX50" s="167"/>
       <c r="BY50" s="252"/>
       <c r="BZ50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA50" s="208" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
       <c r="CH50" s="111"/>
       <c r="CI50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ50" s="111"/>
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
       <c r="CP50" s="111"/>
       <c r="CQ50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR50" s="111"/>
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
       <c r="DF50" s="111"/>
       <c r="DG50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH50" s="111"/>
       <c r="DI50" s="111"/>
       <c r="DJ50" s="111"/>
       <c r="DK50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL50" s="111"/>
       <c r="DM50" s="111"/>
       <c r="DN50" s="111"/>
       <c r="DO50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP50" s="111"/>
       <c r="DQ50" s="111"/>
       <c r="DR50" s="111"/>
       <c r="DS50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT50" s="111"/>
       <c r="DU50" s="111"/>
       <c r="DV50" s="111"/>
       <c r="DW50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX50" s="111"/>
       <c r="DY50" s="111"/>
       <c r="DZ50" s="111"/>
       <c r="EA50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB50" s="111"/>
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21402,13 +21408,13 @@
       <c r="EW50" s="111"/>
       <c r="EX50" s="207"/>
       <c r="EY50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ50" s="208"/>
       <c r="FA50" s="208"/>
       <c r="FB50" s="208"/>
       <c r="FC50" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD50" s="111"/>
       <c r="FE50" s="111"/>
@@ -21507,7 +21513,7 @@
       <c r="AJ51" s="89"/>
       <c r="AK51" s="89"/>
       <c r="AL51" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM51" s="162"/>
       <c r="AN51" s="162"/>
@@ -21549,112 +21555,112 @@
       <c r="BX51" s="167"/>
       <c r="BY51" s="252"/>
       <c r="BZ51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA51" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB51" s="111"/>
       <c r="CC51" s="111"/>
       <c r="CD51" s="111"/>
       <c r="CE51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF51" s="111"/>
       <c r="CG51" s="111"/>
       <c r="CH51" s="111"/>
       <c r="CI51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ51" s="111"/>
       <c r="CK51" s="111"/>
       <c r="CL51" s="111"/>
       <c r="CM51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN51" s="111"/>
       <c r="CO51" s="111"/>
       <c r="CP51" s="111"/>
       <c r="CQ51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR51" s="111"/>
       <c r="CS51" s="111"/>
       <c r="CT51" s="111"/>
       <c r="CU51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV51" s="111"/>
       <c r="CW51" s="111"/>
       <c r="CX51" s="111"/>
       <c r="CY51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ51" s="111"/>
       <c r="DA51" s="111"/>
       <c r="DB51" s="111"/>
       <c r="DC51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD51" s="111"/>
       <c r="DE51" s="111"/>
       <c r="DF51" s="111"/>
       <c r="DG51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH51" s="111"/>
       <c r="DI51" s="111"/>
       <c r="DJ51" s="111"/>
       <c r="DK51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL51" s="111"/>
       <c r="DM51" s="111"/>
       <c r="DN51" s="111"/>
       <c r="DO51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP51" s="111"/>
       <c r="DQ51" s="111"/>
       <c r="DR51" s="111"/>
       <c r="DS51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT51" s="111"/>
       <c r="DU51" s="111"/>
       <c r="DV51" s="111"/>
       <c r="DW51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX51" s="111"/>
       <c r="DY51" s="111"/>
       <c r="DZ51" s="111"/>
       <c r="EA51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB51" s="111"/>
       <c r="EC51" s="111"/>
       <c r="ED51" s="111"/>
       <c r="EE51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF51" s="111"/>
       <c r="EG51" s="111"/>
       <c r="EH51" s="111"/>
       <c r="EI51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ51" s="111"/>
       <c r="EK51" s="111"/>
       <c r="EL51" s="111"/>
       <c r="EM51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN51" s="111"/>
       <c r="EO51" s="111"/>
       <c r="EP51" s="111"/>
       <c r="EQ51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER51" s="111"/>
       <c r="ES51" s="111"/>
@@ -21664,13 +21670,13 @@
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
       <c r="FB51" s="208"/>
       <c r="FC51" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD51" s="111"/>
       <c r="FE51" s="111"/>
@@ -21769,7 +21775,7 @@
       <c r="AJ52" s="89"/>
       <c r="AK52" s="89"/>
       <c r="AL52" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM52" s="162"/>
       <c r="AN52" s="162"/>
@@ -21811,112 +21817,112 @@
       <c r="BX52" s="167"/>
       <c r="BY52" s="252"/>
       <c r="BZ52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA52" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB52" s="111"/>
       <c r="CC52" s="111"/>
       <c r="CD52" s="111"/>
       <c r="CE52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF52" s="111"/>
       <c r="CG52" s="111"/>
       <c r="CH52" s="111"/>
       <c r="CI52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ52" s="111"/>
       <c r="CK52" s="111"/>
       <c r="CL52" s="111"/>
       <c r="CM52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN52" s="111"/>
       <c r="CO52" s="111"/>
       <c r="CP52" s="111"/>
       <c r="CQ52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR52" s="111"/>
       <c r="CS52" s="111"/>
       <c r="CT52" s="111"/>
       <c r="CU52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV52" s="111"/>
       <c r="CW52" s="111"/>
       <c r="CX52" s="111"/>
       <c r="CY52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ52" s="111"/>
       <c r="DA52" s="111"/>
       <c r="DB52" s="111"/>
       <c r="DC52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD52" s="111"/>
       <c r="DE52" s="111"/>
       <c r="DF52" s="111"/>
       <c r="DG52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH52" s="111"/>
       <c r="DI52" s="111"/>
       <c r="DJ52" s="111"/>
       <c r="DK52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL52" s="111"/>
       <c r="DM52" s="111"/>
       <c r="DN52" s="111"/>
       <c r="DO52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP52" s="111"/>
       <c r="DQ52" s="111"/>
       <c r="DR52" s="111"/>
       <c r="DS52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT52" s="111"/>
       <c r="DU52" s="111"/>
       <c r="DV52" s="111"/>
       <c r="DW52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX52" s="111"/>
       <c r="DY52" s="111"/>
       <c r="DZ52" s="111"/>
       <c r="EA52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB52" s="111"/>
       <c r="EC52" s="111"/>
       <c r="ED52" s="111"/>
       <c r="EE52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF52" s="111"/>
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
       <c r="EL52" s="111"/>
       <c r="EM52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN52" s="111"/>
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -21926,13 +21932,13 @@
       <c r="EW52" s="111"/>
       <c r="EX52" s="207"/>
       <c r="EY52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ52" s="208"/>
       <c r="FA52" s="208"/>
       <c r="FB52" s="208"/>
       <c r="FC52" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD52" s="111"/>
       <c r="FE52" s="111"/>
@@ -21992,7 +21998,7 @@
     </row>
     <row r="53" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B53" s="110"/>
       <c r="C53" s="110"/>
@@ -22043,7 +22049,7 @@
         <v>283</v>
       </c>
       <c r="AL53" s="165" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22133,112 +22139,112 @@
         <v>283</v>
       </c>
       <c r="BZ53" s="111" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="CA53" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB53" s="111"/>
       <c r="CC53" s="111"/>
       <c r="CD53" s="111"/>
       <c r="CE53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF53" s="111"/>
       <c r="CG53" s="111"/>
       <c r="CH53" s="111"/>
       <c r="CI53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ53" s="111"/>
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
       <c r="CP53" s="111"/>
       <c r="CQ53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR53" s="111"/>
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
       <c r="CX53" s="111"/>
       <c r="CY53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ53" s="111"/>
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
       <c r="DF53" s="111"/>
       <c r="DG53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH53" s="111"/>
       <c r="DI53" s="111"/>
       <c r="DJ53" s="111"/>
       <c r="DK53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL53" s="111"/>
       <c r="DM53" s="111"/>
       <c r="DN53" s="111"/>
       <c r="DO53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP53" s="111"/>
       <c r="DQ53" s="111"/>
       <c r="DR53" s="111"/>
       <c r="DS53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT53" s="111"/>
       <c r="DU53" s="111"/>
       <c r="DV53" s="111"/>
       <c r="DW53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX53" s="111"/>
       <c r="DY53" s="111"/>
       <c r="DZ53" s="111"/>
       <c r="EA53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB53" s="111"/>
       <c r="EC53" s="111"/>
       <c r="ED53" s="111"/>
       <c r="EE53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF53" s="111"/>
       <c r="EG53" s="111"/>
       <c r="EH53" s="111"/>
       <c r="EI53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ53" s="111"/>
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
       <c r="EP53" s="111"/>
       <c r="EQ53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER53" s="111"/>
       <c r="ES53" s="111"/>
@@ -22248,13 +22254,13 @@
       <c r="EW53" s="111"/>
       <c r="EX53" s="207"/>
       <c r="EY53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ53" s="208"/>
       <c r="FA53" s="208"/>
       <c r="FB53" s="208"/>
       <c r="FC53" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD53" s="111"/>
       <c r="FE53" s="111"/>
@@ -22323,7 +22329,7 @@
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
       <c r="H54" s="110" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="I54" s="110" t="s">
         <v>545</v>
@@ -22357,7 +22363,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22399,46 +22405,46 @@
       <c r="BX54" s="167"/>
       <c r="BY54" s="252"/>
       <c r="BZ54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA54" s="208" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="CB54" s="111"/>
       <c r="CC54" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD54" s="111" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="CE54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF54" s="111"/>
       <c r="CG54" s="111"/>
       <c r="CH54" s="111"/>
       <c r="CI54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ54" s="111"/>
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="CN54" s="111"/>
       <c r="CO54" s="111" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR54" s="111"/>
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="CV54" s="111"/>
       <c r="CW54" s="111" t="s">
@@ -22446,7 +22452,7 @@
       </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="CZ54" s="111" t="s">
         <v>547</v>
@@ -22456,7 +22462,7 @@
       </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="DD54" s="111" t="s">
         <v>546</v>
@@ -22464,47 +22470,47 @@
       <c r="DE54" s="111"/>
       <c r="DF54" s="111"/>
       <c r="DG54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH54" s="111"/>
       <c r="DI54" s="111"/>
       <c r="DJ54" s="111"/>
       <c r="DK54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL54" s="111"/>
       <c r="DM54" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN54" s="111" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="DO54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP54" s="111"/>
       <c r="DQ54" s="111"/>
       <c r="DR54" s="111"/>
       <c r="DS54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT54" s="111"/>
       <c r="DU54" s="111"/>
       <c r="DV54" s="111"/>
       <c r="DW54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX54" s="111"/>
       <c r="DY54" s="111"/>
       <c r="DZ54" s="111"/>
       <c r="EA54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB54" s="111"/>
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="EF54" s="111"/>
       <c r="EG54" s="111" t="s">
@@ -22512,7 +22518,7 @@
       </c>
       <c r="EH54" s="111"/>
       <c r="EI54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ54" s="111"/>
       <c r="EK54" s="111" t="s">
@@ -22520,13 +22526,13 @@
       </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
       <c r="EP54" s="111"/>
       <c r="EQ54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER54" s="111"/>
       <c r="ES54" s="111" t="s">
@@ -22538,13 +22544,13 @@
       <c r="EW54" s="111"/>
       <c r="EX54" s="207"/>
       <c r="EY54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ54" s="208"/>
       <c r="FA54" s="208"/>
       <c r="FB54" s="208"/>
       <c r="FC54" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD54" s="111"/>
       <c r="FE54" s="111"/>
@@ -22613,7 +22619,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
       <c r="H55" s="110" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="I55" s="110" t="s">
         <v>545</v>
@@ -22647,11 +22653,11 @@
       <c r="AJ55" s="89"/>
       <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="AM55" s="162"/>
       <c r="AN55" s="162" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
@@ -22691,46 +22697,46 @@
       <c r="BX55" s="167"/>
       <c r="BY55" s="252"/>
       <c r="BZ55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA55" s="208" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="CB55" s="111"/>
       <c r="CC55" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD55" s="111" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="CE55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF55" s="111"/>
       <c r="CG55" s="111"/>
       <c r="CH55" s="111"/>
       <c r="CI55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ55" s="111"/>
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="CN55" s="111"/>
       <c r="CO55" s="111" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR55" s="111"/>
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="CV55" s="111"/>
       <c r="CW55" s="111" t="s">
@@ -22738,13 +22744,13 @@
       </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
       <c r="DB55" s="111"/>
       <c r="DC55" s="111" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="DD55" s="111" t="s">
         <v>546</v>
@@ -22752,65 +22758,65 @@
       <c r="DE55" s="111"/>
       <c r="DF55" s="111"/>
       <c r="DG55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH55" s="111"/>
       <c r="DI55" s="111"/>
       <c r="DJ55" s="111"/>
       <c r="DK55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL55" s="111"/>
       <c r="DM55" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN55" s="111" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="DO55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP55" s="111"/>
       <c r="DQ55" s="111"/>
       <c r="DR55" s="111"/>
       <c r="DS55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT55" s="111"/>
       <c r="DU55" s="111"/>
       <c r="DV55" s="111"/>
       <c r="DW55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX55" s="111"/>
       <c r="DY55" s="111"/>
       <c r="DZ55" s="111"/>
       <c r="EA55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB55" s="111"/>
       <c r="EC55" s="111"/>
       <c r="ED55" s="111"/>
       <c r="EE55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF55" s="111"/>
       <c r="EG55" s="111"/>
       <c r="EH55" s="111"/>
       <c r="EI55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ55" s="111"/>
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
       <c r="EP55" s="111"/>
       <c r="EQ55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER55" s="111"/>
       <c r="ES55" s="111"/>
@@ -22820,13 +22826,13 @@
       <c r="EW55" s="111"/>
       <c r="EX55" s="207"/>
       <c r="EY55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ55" s="208"/>
       <c r="FA55" s="208"/>
       <c r="FB55" s="208"/>
       <c r="FC55" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD55" s="111"/>
       <c r="FE55" s="111"/>
@@ -22925,7 +22931,7 @@
       <c r="AJ56" s="89"/>
       <c r="AK56" s="89"/>
       <c r="AL56" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM56" s="162"/>
       <c r="AN56" s="162"/>
@@ -22967,112 +22973,112 @@
       <c r="BX56" s="167"/>
       <c r="BY56" s="252"/>
       <c r="BZ56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA56" s="208" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
       <c r="CH56" s="111"/>
       <c r="CI56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ56" s="111"/>
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
       <c r="CP56" s="111"/>
       <c r="CQ56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR56" s="111"/>
       <c r="CS56" s="111"/>
       <c r="CT56" s="111"/>
       <c r="CU56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV56" s="111"/>
       <c r="CW56" s="111"/>
       <c r="CX56" s="111"/>
       <c r="CY56" s="111" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="CZ56" s="111"/>
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
       <c r="DF56" s="111"/>
       <c r="DG56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH56" s="111"/>
       <c r="DI56" s="111"/>
       <c r="DJ56" s="111"/>
       <c r="DK56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL56" s="111"/>
       <c r="DM56" s="111"/>
       <c r="DN56" s="111"/>
       <c r="DO56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP56" s="111"/>
       <c r="DQ56" s="111"/>
       <c r="DR56" s="111"/>
       <c r="DS56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT56" s="111"/>
       <c r="DU56" s="111"/>
       <c r="DV56" s="111"/>
       <c r="DW56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX56" s="111"/>
       <c r="DY56" s="111"/>
       <c r="DZ56" s="111"/>
       <c r="EA56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB56" s="111"/>
       <c r="EC56" s="111"/>
       <c r="ED56" s="111"/>
       <c r="EE56" s="111" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="EF56" s="111"/>
       <c r="EG56" s="111"/>
       <c r="EH56" s="111"/>
       <c r="EI56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ56" s="111"/>
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
       <c r="EP56" s="111"/>
       <c r="EQ56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER56" s="111"/>
       <c r="ES56" s="111"/>
@@ -23082,13 +23088,13 @@
       <c r="EW56" s="111"/>
       <c r="EX56" s="207"/>
       <c r="EY56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ56" s="208"/>
       <c r="FA56" s="208"/>
       <c r="FB56" s="208"/>
       <c r="FC56" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD56" s="111"/>
       <c r="FE56" s="111"/>
@@ -23187,7 +23193,7 @@
       <c r="AJ57" s="89"/>
       <c r="AK57" s="89"/>
       <c r="AL57" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM57" s="162"/>
       <c r="AN57" s="162"/>
@@ -23229,112 +23235,112 @@
       <c r="BX57" s="167"/>
       <c r="BY57" s="252"/>
       <c r="BZ57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA57" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB57" s="111"/>
       <c r="CC57" s="111"/>
       <c r="CD57" s="111"/>
       <c r="CE57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF57" s="111"/>
       <c r="CG57" s="111"/>
       <c r="CH57" s="111"/>
       <c r="CI57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ57" s="111"/>
       <c r="CK57" s="111"/>
       <c r="CL57" s="111"/>
       <c r="CM57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN57" s="111"/>
       <c r="CO57" s="111"/>
       <c r="CP57" s="111"/>
       <c r="CQ57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR57" s="111"/>
       <c r="CS57" s="111"/>
       <c r="CT57" s="111"/>
       <c r="CU57" s="111" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="CV57" s="111"/>
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
       <c r="DB57" s="111"/>
       <c r="DC57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD57" s="111"/>
       <c r="DE57" s="111"/>
       <c r="DF57" s="111"/>
       <c r="DG57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH57" s="111"/>
       <c r="DI57" s="111"/>
       <c r="DJ57" s="111"/>
       <c r="DK57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL57" s="111"/>
       <c r="DM57" s="111"/>
       <c r="DN57" s="111"/>
       <c r="DO57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP57" s="111"/>
       <c r="DQ57" s="111"/>
       <c r="DR57" s="111"/>
       <c r="DS57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT57" s="111"/>
       <c r="DU57" s="111"/>
       <c r="DV57" s="111"/>
       <c r="DW57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX57" s="111"/>
       <c r="DY57" s="111"/>
       <c r="DZ57" s="111"/>
       <c r="EA57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB57" s="111"/>
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
       <c r="EH57" s="111"/>
       <c r="EI57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ57" s="111"/>
       <c r="EK57" s="111"/>
       <c r="EL57" s="111"/>
       <c r="EM57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN57" s="111"/>
       <c r="EO57" s="111"/>
       <c r="EP57" s="111"/>
       <c r="EQ57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER57" s="111"/>
       <c r="ES57" s="111"/>
@@ -23344,13 +23350,13 @@
       <c r="EW57" s="111"/>
       <c r="EX57" s="207"/>
       <c r="EY57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ57" s="208"/>
       <c r="FA57" s="208"/>
       <c r="FB57" s="208"/>
       <c r="FC57" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD57" s="111"/>
       <c r="FE57" s="111"/>
@@ -23449,7 +23455,7 @@
       <c r="AJ58" s="90"/>
       <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23491,112 +23497,112 @@
       <c r="BX58" s="167"/>
       <c r="BY58" s="252"/>
       <c r="BZ58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA58" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB58" s="111"/>
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
       <c r="CH58" s="111"/>
       <c r="CI58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ58" s="111"/>
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
       <c r="CP58" s="111"/>
       <c r="CQ58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR58" s="111"/>
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
       <c r="DF58" s="111"/>
       <c r="DG58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH58" s="111"/>
       <c r="DI58" s="111"/>
       <c r="DJ58" s="111"/>
       <c r="DK58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL58" s="111"/>
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
       <c r="DR58" s="111"/>
       <c r="DS58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT58" s="111"/>
       <c r="DU58" s="111"/>
       <c r="DV58" s="111"/>
       <c r="DW58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX58" s="111"/>
       <c r="DY58" s="111"/>
       <c r="DZ58" s="111"/>
       <c r="EA58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB58" s="111"/>
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23606,13 +23612,13 @@
       <c r="EW58" s="111"/>
       <c r="EX58" s="207"/>
       <c r="EY58" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ58" s="208"/>
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
       <c r="FC58" s="208" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23711,7 +23717,7 @@
       <c r="AJ59" s="90"/>
       <c r="AK59" s="90"/>
       <c r="AL59" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM59" s="162"/>
       <c r="AN59" s="162"/>
@@ -23753,112 +23759,112 @@
       <c r="BX59" s="167"/>
       <c r="BY59" s="252"/>
       <c r="BZ59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA59" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB59" s="111"/>
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
       <c r="CH59" s="111"/>
       <c r="CI59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ59" s="111"/>
       <c r="CK59" s="111"/>
       <c r="CL59" s="111"/>
       <c r="CM59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN59" s="111"/>
       <c r="CO59" s="111"/>
       <c r="CP59" s="111"/>
       <c r="CQ59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CR59" s="111"/>
       <c r="CS59" s="111"/>
       <c r="CT59" s="111"/>
       <c r="CU59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV59" s="111"/>
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
       <c r="DB59" s="111"/>
       <c r="DC59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD59" s="111"/>
       <c r="DE59" s="111"/>
       <c r="DF59" s="111"/>
       <c r="DG59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH59" s="111"/>
       <c r="DI59" s="111"/>
       <c r="DJ59" s="111"/>
       <c r="DK59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL59" s="111"/>
       <c r="DM59" s="111"/>
       <c r="DN59" s="111"/>
       <c r="DO59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP59" s="111"/>
       <c r="DQ59" s="111"/>
       <c r="DR59" s="111"/>
       <c r="DS59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT59" s="111"/>
       <c r="DU59" s="111"/>
       <c r="DV59" s="111"/>
       <c r="DW59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX59" s="111"/>
       <c r="DY59" s="111"/>
       <c r="DZ59" s="111"/>
       <c r="EA59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB59" s="111"/>
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
       <c r="EH59" s="111"/>
       <c r="EI59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ59" s="111"/>
       <c r="EK59" s="111"/>
       <c r="EL59" s="111"/>
       <c r="EM59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN59" s="111"/>
       <c r="EO59" s="111"/>
       <c r="EP59" s="111"/>
       <c r="EQ59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER59" s="111"/>
       <c r="ES59" s="111"/>
@@ -23868,13 +23874,13 @@
       <c r="EW59" s="111"/>
       <c r="EX59" s="207"/>
       <c r="EY59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ59" s="208"/>
       <c r="FA59" s="208"/>
       <c r="FB59" s="208"/>
       <c r="FC59" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="FD59" s="111"/>
       <c r="FE59" s="111"/>
@@ -23973,7 +23979,7 @@
       <c r="AJ60" s="90"/>
       <c r="AK60" s="90"/>
       <c r="AL60" s="165" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AM60" s="162"/>
       <c r="AN60" s="162"/>
@@ -24015,112 +24021,112 @@
       <c r="BX60" s="167"/>
       <c r="BY60" s="252"/>
       <c r="BZ60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CA60" s="111" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="CB60" s="111"/>
       <c r="CC60" s="111"/>
       <c r="CD60" s="111"/>
       <c r="CE60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CF60" s="111"/>
       <c r="CG60" s="111"/>
       <c r="CH60" s="111"/>
       <c r="CI60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CJ60" s="111"/>
       <c r="CK60" s="111"/>
       <c r="CL60" s="111"/>
       <c r="CM60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CN60" s="111"/>
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
       <c r="CT60" s="111"/>
       <c r="CU60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CV60" s="111"/>
       <c r="CW60" s="111"/>
       <c r="CX60" s="111"/>
       <c r="CY60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="CZ60" s="111"/>
       <c r="DA60" s="111"/>
       <c r="DB60" s="111"/>
       <c r="DC60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DD60" s="111"/>
       <c r="DE60" s="111"/>
       <c r="DF60" s="111"/>
       <c r="DG60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DH60" s="111"/>
       <c r="DI60" s="111"/>
       <c r="DJ60" s="111"/>
       <c r="DK60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DL60" s="111"/>
       <c r="DM60" s="111"/>
       <c r="DN60" s="111"/>
       <c r="DO60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DP60" s="111"/>
       <c r="DQ60" s="111"/>
       <c r="DR60" s="111"/>
       <c r="DS60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DT60" s="111"/>
       <c r="DU60" s="111"/>
       <c r="DV60" s="111"/>
       <c r="DW60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="DX60" s="111"/>
       <c r="DY60" s="111"/>
       <c r="DZ60" s="111"/>
       <c r="EA60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EB60" s="111"/>
       <c r="EC60" s="111"/>
       <c r="ED60" s="111"/>
       <c r="EE60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EF60" s="111"/>
       <c r="EG60" s="111"/>
       <c r="EH60" s="111"/>
       <c r="EI60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EJ60" s="111"/>
       <c r="EK60" s="111"/>
       <c r="EL60" s="111"/>
       <c r="EM60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EN60" s="111"/>
       <c r="EO60" s="111"/>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="ER60" s="111"/>
       <c r="ES60" s="111"/>
@@ -24130,13 +24136,13 @@
       <c r="EW60" s="111"/>
       <c r="EX60" s="207"/>
       <c r="EY60" s="111" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="EZ60" s="208"/>
       <c r="FA60" s="208"/>
       <c r="FB60" s="208"/>
       <c r="FC60" s="208" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="FD60" s="111"/>
       <c r="FE60" s="111"/>
@@ -33626,7 +33632,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="214" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D3" s="189" t="s">
         <v>603</v>
@@ -33635,31 +33641,31 @@
         <v>663</v>
       </c>
       <c r="F3" s="214" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G3" s="214" t="s">
+        <v>742</v>
+      </c>
+      <c r="H3" s="214" t="s">
+        <v>743</v>
+      </c>
+      <c r="I3" s="214" t="s">
         <v>744</v>
       </c>
-      <c r="H3" s="214" t="s">
+      <c r="J3" s="214" t="s">
         <v>745</v>
       </c>
-      <c r="I3" s="214" t="s">
+      <c r="K3" s="214" t="s">
         <v>746</v>
       </c>
-      <c r="J3" s="214" t="s">
+      <c r="L3" s="214" t="s">
         <v>747</v>
       </c>
-      <c r="K3" s="214" t="s">
+      <c r="M3" s="214" t="s">
         <v>748</v>
       </c>
-      <c r="L3" s="214" t="s">
+      <c r="N3" s="214" t="s">
         <v>749</v>
-      </c>
-      <c r="M3" s="214" t="s">
-        <v>750</v>
-      </c>
-      <c r="N3" s="214" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -33671,62 +33677,62 @@
       <c r="D4" s="216"/>
       <c r="E4" s="216"/>
       <c r="F4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="H4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="I4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="K4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="L4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="M4" s="216" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="N4" s="216"/>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="215" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B5" s="216"/>
       <c r="C5" s="216"/>
       <c r="D5" s="216"/>
       <c r="E5" s="216"/>
       <c r="F5" s="248" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="G5" s="248" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="H5" s="248" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="I5" s="248" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="J5" s="248" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="K5" s="248" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="L5" s="248" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="M5" s="248" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="N5" s="216"/>
     </row>
@@ -35319,28 +35325,28 @@
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
       <c r="F46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="J46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="K46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="L46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="M46" s="72" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="N46" s="72"/>
     </row>
@@ -35353,28 +35359,28 @@
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
       <c r="F47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="I47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="L47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="M47" s="72" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="N47" s="72"/>
     </row>
@@ -35429,28 +35435,28 @@
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
       <c r="F49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="H49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="I49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="J49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="K49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="N49" s="72"/>
     </row>
@@ -35463,28 +35469,28 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="L50" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="N50" s="72"/>
     </row>
@@ -35539,28 +35545,28 @@
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
       <c r="F52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="H52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="I52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="J52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="K52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="L52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="M52" s="72" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="N52" s="72"/>
     </row>
@@ -35573,28 +35579,28 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="H53" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="I53" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="J53" s="72" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="K53" s="72" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="L53" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="M53" s="72" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="N53" s="72"/>
     </row>
@@ -35649,28 +35655,28 @@
       <c r="D55" s="72"/>
       <c r="E55" s="72"/>
       <c r="F55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="I55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="J55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="K55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="L55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="M55" s="72" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="N55" s="72"/>
     </row>
@@ -35683,28 +35689,28 @@
       <c r="D56" s="72"/>
       <c r="E56" s="72"/>
       <c r="F56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="H56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="J56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="L56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M56" s="72" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="N56" s="72"/>
     </row>
@@ -35759,28 +35765,28 @@
       <c r="D58" s="72"/>
       <c r="E58" s="72"/>
       <c r="F58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="H58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="I58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="J58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="L58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M58" s="72" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="N58" s="72"/>
     </row>
@@ -35793,28 +35799,28 @@
       <c r="D59" s="72"/>
       <c r="E59" s="72"/>
       <c r="F59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="K59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="L59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="M59" s="72" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="N59" s="72"/>
     </row>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Update Midazolam sedation methodology and scenarios
Re-tune MDZ pharamcodynamics so that sedation occurs at lower doses and
anesthesia induction at higher doses.  Create two new scenarios to
demonstrate new behavior.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="862">
   <si>
     <t>Name</t>
   </si>
@@ -2403,9 +2403,6 @@
     <t>[-0.05; 4 ug/L]</t>
   </si>
   <si>
-    <t>[-0.25; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.15; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2442,9 +2439,6 @@
     <t>[0.2; 0.4319 ug/mL]</t>
   </si>
   <si>
-    <t>[0.3; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.06; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2523,18 +2517,12 @@
     <t>[-0.95; 4 ug/L]</t>
   </si>
   <si>
-    <t>[-1; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-1; 0.075 ug/mL]</t>
   </si>
   <si>
     <t>[-0.5; 0.5 ug/mL]</t>
   </si>
   <si>
-    <t>[1; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.5; 0.9 ug/L]</t>
   </si>
   <si>
@@ -2547,9 +2535,6 @@
     <t>[0.25; 0.4319 ug/mL]</t>
   </si>
   <si>
-    <t>[-0.5; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.1; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2614,6 +2599,27 @@
   </si>
   <si>
     <t>[-0.5; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.75; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.25; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.6; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.4; 0.3 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.25 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.6; 0.3 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5564,10 +5570,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="DG33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="BV36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EE55" sqref="EE55"/>
+      <selection pane="bottomRight" activeCell="CY4" sqref="CY4:CY60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -12131,7 +12137,7 @@
       <c r="EC20" s="107"/>
       <c r="ED20" s="107"/>
       <c r="EE20" s="107" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="EF20" s="107"/>
       <c r="EG20" s="107"/>
@@ -12705,7 +12711,7 @@
       <c r="EC22" s="107"/>
       <c r="ED22" s="107"/>
       <c r="EE22" s="107" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="EF22" s="107"/>
       <c r="EG22" s="107"/>
@@ -20528,7 +20534,7 @@
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
@@ -20540,19 +20546,19 @@
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
       <c r="CX47" s="111"/>
       <c r="CY47" s="111" t="s">
-        <v>782</v>
+        <v>855</v>
       </c>
       <c r="CZ47" s="111"/>
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
@@ -20564,7 +20570,7 @@
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>
@@ -20594,7 +20600,7 @@
       <c r="EC47" s="111"/>
       <c r="ED47" s="111"/>
       <c r="EE47" s="111" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="EF47" s="111"/>
       <c r="EG47" s="111"/>
@@ -20606,7 +20612,7 @@
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
@@ -20808,13 +20814,13 @@
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>789</v>
+        <v>856</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
@@ -20832,7 +20838,7 @@
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
@@ -20856,25 +20862,25 @@
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
       <c r="EL48" s="111"/>
       <c r="EM48" s="111" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="EN48" s="111"/>
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20890,7 +20896,7 @@
       <c r="FA48" s="111"/>
       <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -21031,7 +21037,7 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="CA49" s="111" t="s">
         <v>783</v>
@@ -21251,7 +21257,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21296,13 +21302,13 @@
         <v>782</v>
       </c>
       <c r="CA50" s="208" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
@@ -21314,7 +21320,7 @@
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
@@ -21326,19 +21332,19 @@
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>802</v>
+        <v>857</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
@@ -21380,25 +21386,25 @@
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21670,7 +21676,7 @@
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
@@ -21910,7 +21916,7 @@
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
@@ -21922,7 +21928,7 @@
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -22049,7 +22055,7 @@
         <v>283</v>
       </c>
       <c r="AL53" s="165" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22139,7 +22145,7 @@
         <v>283</v>
       </c>
       <c r="BZ53" s="111" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="CA53" s="111" t="s">
         <v>783</v>
@@ -22160,7 +22166,7 @@
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
@@ -22172,7 +22178,7 @@
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
@@ -22184,7 +22190,7 @@
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
@@ -22238,7 +22244,7 @@
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
@@ -22329,7 +22335,7 @@
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
       <c r="H54" s="110" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="I54" s="110" t="s">
         <v>545</v>
@@ -22363,7 +22369,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22408,14 +22414,14 @@
         <v>782</v>
       </c>
       <c r="CA54" s="208" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="CB54" s="111"/>
       <c r="CC54" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD54" s="111" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="CE54" s="111" t="s">
         <v>782</v>
@@ -22430,11 +22436,11 @@
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="CN54" s="111"/>
       <c r="CO54" s="111" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
@@ -22444,7 +22450,7 @@
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="CV54" s="111"/>
       <c r="CW54" s="111" t="s">
@@ -22452,7 +22458,7 @@
       </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="CZ54" s="111" t="s">
         <v>547</v>
@@ -22462,7 +22468,7 @@
       </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="DD54" s="111" t="s">
         <v>546</v>
@@ -22483,7 +22489,7 @@
         <v>549</v>
       </c>
       <c r="DN54" s="111" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="DO54" s="111" t="s">
         <v>782</v>
@@ -22510,7 +22516,7 @@
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="EF54" s="111"/>
       <c r="EG54" s="111" t="s">
@@ -22526,7 +22532,7 @@
       </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
@@ -22619,7 +22625,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
       <c r="H55" s="110" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="I55" s="110" t="s">
         <v>545</v>
@@ -22653,11 +22659,11 @@
       <c r="AJ55" s="89"/>
       <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="AM55" s="162"/>
       <c r="AN55" s="162" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
@@ -22700,14 +22706,14 @@
         <v>782</v>
       </c>
       <c r="CA55" s="208" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="CB55" s="111"/>
       <c r="CC55" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD55" s="111" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="CE55" s="111" t="s">
         <v>782</v>
@@ -22722,11 +22728,11 @@
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="CN55" s="111"/>
       <c r="CO55" s="111" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
@@ -22736,7 +22742,7 @@
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="CV55" s="111"/>
       <c r="CW55" s="111" t="s">
@@ -22744,7 +22750,7 @@
       </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
@@ -22771,7 +22777,7 @@
         <v>549</v>
       </c>
       <c r="DN55" s="111" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="DO55" s="111" t="s">
         <v>782</v>
@@ -22810,7 +22816,7 @@
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
@@ -22976,13 +22982,13 @@
         <v>782</v>
       </c>
       <c r="CA56" s="208" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
@@ -22994,7 +23000,7 @@
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
@@ -23012,13 +23018,13 @@
       <c r="CW56" s="111"/>
       <c r="CX56" s="111"/>
       <c r="CY56" s="111" t="s">
-        <v>829</v>
+        <v>858</v>
       </c>
       <c r="CZ56" s="111"/>
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
@@ -23060,7 +23066,7 @@
       <c r="EC56" s="111"/>
       <c r="ED56" s="111"/>
       <c r="EE56" s="111" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="EF56" s="111"/>
       <c r="EG56" s="111"/>
@@ -23072,7 +23078,7 @@
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
@@ -23274,7 +23280,7 @@
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>832</v>
+        <v>859</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
@@ -23322,7 +23328,7 @@
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
@@ -23455,7 +23461,7 @@
       <c r="AJ58" s="90"/>
       <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23506,7 +23512,7 @@
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
@@ -23518,7 +23524,7 @@
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
@@ -23530,19 +23536,19 @@
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>837</v>
+        <v>860</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
@@ -23560,7 +23566,7 @@
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
@@ -23584,25 +23590,25 @@
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23618,7 +23624,7 @@
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
       <c r="FC58" s="208" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23768,7 +23774,7 @@
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
@@ -23798,7 +23804,7 @@
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>829</v>
+        <v>861</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
@@ -23846,7 +23852,7 @@
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
@@ -24048,7 +24054,7 @@
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
@@ -24142,7 +24148,7 @@
       <c r="FA60" s="208"/>
       <c r="FB60" s="208"/>
       <c r="FC60" s="208" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="FD60" s="111"/>
       <c r="FE60" s="111"/>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Update Ketamine substance and scenarios
Create scenatios for ketamine sedation, ketamine anesthesia induction,
and ketamine pain relief.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -2115,9 +2115,6 @@
     <t>0.7 mL/min kg</t>
   </si>
   <si>
-    <t>2.0 1/min</t>
-  </si>
-  <si>
     <t>0.0314 g/L</t>
   </si>
   <si>
@@ -2202,18 +2199,12 @@
     <t>37.0 mL/min kg</t>
   </si>
   <si>
-    <t>195 mL/min kg</t>
-  </si>
-  <si>
     <t>420 mL/min kg</t>
   </si>
   <si>
     <t>27.5 mL/min kg</t>
   </si>
   <si>
-    <t>16 mL/min kg</t>
-  </si>
-  <si>
     <t>4.0 mL/min kg</t>
   </si>
   <si>
@@ -2388,9 +2379,6 @@
     <t>[0; 0.0 ug/L]</t>
   </si>
   <si>
-    <t>[1; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.8; 0.5 ug/mL]</t>
   </si>
   <si>
@@ -2436,9 +2424,6 @@
     <t>[-0.01; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.2; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.06; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2475,9 +2460,6 @@
     <t>https://www.ncbi.nlm.nih.gov/pubmed/2875674; http://anesthesiology.pubs.asahq.org/article.aspx?articleid=1936490</t>
   </si>
   <si>
-    <t>[-0.5; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.5; 0.0588 ug/mL]</t>
   </si>
   <si>
@@ -2502,9 +2484,6 @@
     <t>[-0.33; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[0; 0.0588 ug/mL]</t>
   </si>
   <si>
@@ -2532,9 +2511,6 @@
     <t>[-0.1; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.25; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.1; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2550,9 +2526,6 @@
     <t>[1.0; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.75; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.85; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2620,6 +2593,33 @@
   </si>
   <si>
     <t>[-0.6; 0.3 ug/mL]</t>
+  </si>
+  <si>
+    <t>277 mL/min kg</t>
+  </si>
+  <si>
+    <t>20 mL/min kg</t>
+  </si>
+  <si>
+    <t>3.0 1/min</t>
+  </si>
+  <si>
+    <t>[1; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.1; 0.75 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.25; 0.75 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.6; 0.2 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.4; 0.75 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5573,7 +5573,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="BV36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CY4" sqref="CY4:CY60"/>
+      <selection pane="bottomRight" activeCell="CU4" sqref="CU4:CU60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6540,7 +6540,7 @@
         <v>165</v>
       </c>
       <c r="BZ2" s="96" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="CA2" s="257" t="s">
         <v>190</v>
@@ -6567,16 +6567,16 @@
         <v>50</v>
       </c>
       <c r="CI2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CJ2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CK2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CL2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CM2" s="96" t="s">
         <v>51</v>
@@ -6639,16 +6639,16 @@
         <v>47</v>
       </c>
       <c r="DG2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DH2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DI2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DJ2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DK2" s="96" t="s">
         <v>48</v>
@@ -6771,16 +6771,16 @@
         <v>648</v>
       </c>
       <c r="EY2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="EZ2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FA2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FB2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FC2" s="96" t="s">
         <v>637</v>
@@ -6891,64 +6891,64 @@
         <v>563</v>
       </c>
       <c r="GM2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GN2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GO2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GP2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GQ2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GR2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GS2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GT2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GU2" s="101" t="s">
+        <v>737</v>
+      </c>
+      <c r="GV2" s="101" t="s">
+        <v>737</v>
+      </c>
+      <c r="GW2" s="101" t="s">
+        <v>737</v>
+      </c>
+      <c r="GX2" s="101" t="s">
+        <v>737</v>
+      </c>
+      <c r="GY2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="GZ2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HA2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HB2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HC2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="GN2" s="101" t="s">
+      <c r="HD2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="GO2" s="101" t="s">
+      <c r="HE2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="GP2" s="101" t="s">
+      <c r="HF2" s="101" t="s">
         <v>735</v>
-      </c>
-      <c r="GQ2" s="101" t="s">
-        <v>737</v>
-      </c>
-      <c r="GR2" s="101" t="s">
-        <v>737</v>
-      </c>
-      <c r="GS2" s="101" t="s">
-        <v>737</v>
-      </c>
-      <c r="GT2" s="101" t="s">
-        <v>737</v>
-      </c>
-      <c r="GU2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="GV2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="GW2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="GX2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="GY2" s="101" t="s">
-        <v>733</v>
-      </c>
-      <c r="GZ2" s="101" t="s">
-        <v>733</v>
-      </c>
-      <c r="HA2" s="101" t="s">
-        <v>733</v>
-      </c>
-      <c r="HB2" s="101" t="s">
-        <v>733</v>
-      </c>
-      <c r="HC2" s="101" t="s">
-        <v>738</v>
-      </c>
-      <c r="HD2" s="101" t="s">
-        <v>738</v>
-      </c>
-      <c r="HE2" s="101" t="s">
-        <v>738</v>
-      </c>
-      <c r="HF2" s="101" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="3" spans="1:214" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -8005,31 +8005,31 @@
       <c r="GK5" s="178"/>
       <c r="GL5" s="178"/>
       <c r="GM5" s="245" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="GN5" s="246"/>
       <c r="GO5" s="246"/>
       <c r="GP5" s="246"/>
       <c r="GQ5" s="245" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="GR5" s="246"/>
       <c r="GS5" s="246"/>
       <c r="GT5" s="246"/>
       <c r="GU5" s="245" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="GV5" s="246"/>
       <c r="GW5" s="246"/>
       <c r="GX5" s="246"/>
       <c r="GY5" s="245" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="GZ5" s="246"/>
       <c r="HA5" s="246"/>
       <c r="HB5" s="246"/>
       <c r="HC5" s="245" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="HD5" s="221"/>
       <c r="HE5" s="221"/>
@@ -8128,7 +8128,7 @@
       <c r="BX6" s="167"/>
       <c r="BY6" s="252"/>
       <c r="BZ6" s="107" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="CA6" s="258" t="s">
         <v>124</v>
@@ -8261,19 +8261,19 @@
       <c r="GS6" s="246"/>
       <c r="GT6" s="246"/>
       <c r="GU6" s="249" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="GV6" s="246"/>
       <c r="GW6" s="246"/>
       <c r="GX6" s="246"/>
       <c r="GY6" s="249" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="GZ6" s="246"/>
       <c r="HA6" s="246"/>
       <c r="HB6" s="246"/>
       <c r="HC6" s="249" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="HD6" s="221"/>
       <c r="HE6" s="221"/>
@@ -9072,7 +9072,7 @@
       <c r="BX10" s="167"/>
       <c r="BY10" s="252"/>
       <c r="BZ10" s="107" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="CA10" s="258" t="s">
         <v>312</v>
@@ -9087,7 +9087,7 @@
       <c r="CG10" s="107"/>
       <c r="CH10" s="107"/>
       <c r="CI10" s="107" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="CJ10" s="107"/>
       <c r="CK10" s="107"/>
@@ -9123,7 +9123,7 @@
       <c r="DE10" s="107"/>
       <c r="DF10" s="107"/>
       <c r="DG10" s="107" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="DH10" s="107"/>
       <c r="DI10" s="107"/>
@@ -9193,7 +9193,7 @@
       </c>
       <c r="EX10" s="107"/>
       <c r="EY10" s="107" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="EZ10" s="107"/>
       <c r="FA10" s="107"/>
@@ -9249,31 +9249,31 @@
       <c r="GK10" s="178"/>
       <c r="GL10" s="178"/>
       <c r="GM10" s="245" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="GN10" s="246"/>
       <c r="GO10" s="246"/>
       <c r="GP10" s="246"/>
       <c r="GQ10" s="245" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="GR10" s="246"/>
       <c r="GS10" s="246"/>
       <c r="GT10" s="246"/>
       <c r="GU10" s="245" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="GV10" s="246"/>
       <c r="GW10" s="246"/>
       <c r="GX10" s="246"/>
       <c r="GY10" s="245" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="GZ10" s="246"/>
       <c r="HA10" s="246"/>
       <c r="HB10" s="246"/>
       <c r="HC10" s="245" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="HD10" s="221"/>
       <c r="HE10" s="221"/>
@@ -11801,7 +11801,7 @@
       <c r="CS19" s="107"/>
       <c r="CT19" s="107"/>
       <c r="CU19" s="107">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="CV19" s="107"/>
       <c r="CW19" s="107"/>
@@ -12071,7 +12071,7 @@
       <c r="CK20" s="107"/>
       <c r="CL20" s="107"/>
       <c r="CM20" s="107" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="CN20" s="107"/>
       <c r="CO20" s="107"/>
@@ -12083,13 +12083,13 @@
       <c r="CS20" s="107"/>
       <c r="CT20" s="107"/>
       <c r="CU20" s="107" t="s">
-        <v>722</v>
+        <v>853</v>
       </c>
       <c r="CV20" s="107"/>
       <c r="CW20" s="107"/>
       <c r="CX20" s="107"/>
       <c r="CY20" s="107" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="CZ20" s="107"/>
       <c r="DA20" s="107"/>
@@ -12101,13 +12101,13 @@
       <c r="DE20" s="107"/>
       <c r="DF20" s="107"/>
       <c r="DG20" s="107" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="DH20" s="107"/>
       <c r="DI20" s="107"/>
       <c r="DJ20" s="107"/>
       <c r="DK20" s="107" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="DL20" s="107"/>
       <c r="DM20" s="107"/>
@@ -12137,13 +12137,13 @@
       <c r="EC20" s="107"/>
       <c r="ED20" s="107"/>
       <c r="EE20" s="107" t="s">
-        <v>845</v>
+        <v>836</v>
       </c>
       <c r="EF20" s="107"/>
       <c r="EG20" s="107"/>
       <c r="EH20" s="107"/>
       <c r="EI20" s="107" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="EJ20" s="107"/>
       <c r="EK20" s="107"/>
@@ -12161,7 +12161,7 @@
       <c r="ES20" s="107"/>
       <c r="ET20" s="107"/>
       <c r="EU20" s="107" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="EV20" s="107"/>
       <c r="EW20" s="107"/>
@@ -12173,7 +12173,7 @@
       <c r="FA20" s="107"/>
       <c r="FB20" s="107"/>
       <c r="FC20" s="107" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="FD20" s="107"/>
       <c r="FE20" s="107"/>
@@ -12324,7 +12324,7 @@
       <c r="BX21" s="167"/>
       <c r="BY21" s="252"/>
       <c r="BZ21" s="107" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="CA21" s="258" t="s">
         <v>528</v>
@@ -12363,7 +12363,7 @@
       <c r="CW21" s="107"/>
       <c r="CX21" s="107"/>
       <c r="CY21" s="107" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="CZ21" s="107"/>
       <c r="DA21" s="107"/>
@@ -12375,7 +12375,7 @@
       <c r="DE21" s="107"/>
       <c r="DF21" s="107"/>
       <c r="DG21" s="107" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="DH21" s="107"/>
       <c r="DI21" s="107"/>
@@ -12449,7 +12449,7 @@
         <v>656</v>
       </c>
       <c r="EY21" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ21" s="107"/>
       <c r="FA21" s="107"/>
@@ -12584,7 +12584,7 @@
         <v>591</v>
       </c>
       <c r="AV22" s="162" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="AW22" s="162"/>
       <c r="AX22" s="167"/>
@@ -12633,13 +12633,13 @@
       <c r="CG22" s="107"/>
       <c r="CH22" s="107"/>
       <c r="CI22" s="107" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="CJ22" s="107"/>
       <c r="CK22" s="107"/>
       <c r="CL22" s="107"/>
       <c r="CM22" s="107" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="CN22" s="107"/>
       <c r="CO22" s="107"/>
@@ -12651,7 +12651,7 @@
       <c r="CS22" s="107"/>
       <c r="CT22" s="107"/>
       <c r="CU22" s="107" t="s">
-        <v>725</v>
+        <v>854</v>
       </c>
       <c r="CV22" s="107"/>
       <c r="CW22" s="107"/>
@@ -12669,19 +12669,19 @@
       <c r="DE22" s="107"/>
       <c r="DF22" s="107"/>
       <c r="DG22" s="107" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="DH22" s="107"/>
       <c r="DI22" s="107"/>
       <c r="DJ22" s="107"/>
       <c r="DK22" s="107" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="DL22" s="107"/>
       <c r="DM22" s="107"/>
       <c r="DN22" s="107"/>
       <c r="DO22" s="107" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="DP22" s="107"/>
       <c r="DQ22" s="107" t="s">
@@ -12711,13 +12711,13 @@
       <c r="EC22" s="107"/>
       <c r="ED22" s="107"/>
       <c r="EE22" s="107" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="EF22" s="107"/>
       <c r="EG22" s="107"/>
       <c r="EH22" s="107"/>
       <c r="EI22" s="107" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="EJ22" s="107"/>
       <c r="EK22" s="107"/>
@@ -12729,7 +12729,7 @@
       <c r="EO22" s="107"/>
       <c r="EP22" s="107"/>
       <c r="EQ22" s="107" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="ER22" s="107"/>
       <c r="ES22" s="107"/>
@@ -12745,13 +12745,13 @@
         <v>656</v>
       </c>
       <c r="EY22" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ22" s="107"/>
       <c r="FA22" s="107"/>
       <c r="FB22" s="107"/>
       <c r="FC22" s="107" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="FD22" s="107"/>
       <c r="FE22" s="107"/>
@@ -13384,7 +13384,7 @@
       <c r="BX24" s="167"/>
       <c r="BY24" s="252"/>
       <c r="BZ24" s="107" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="CA24" s="258" t="str">
         <f>CA21</f>
@@ -13619,7 +13619,7 @@
         <v>656</v>
       </c>
       <c r="EY24" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ24" s="107"/>
       <c r="FA24" s="107"/>
@@ -15213,7 +15213,7 @@
     </row>
     <row r="30" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="79" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="B30" s="222"/>
       <c r="C30" s="223" t="s">
@@ -15703,7 +15703,7 @@
     </row>
     <row r="31" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="80" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="B31" s="99"/>
       <c r="C31" s="99"/>
@@ -15899,31 +15899,31 @@
       <c r="GK31" s="177"/>
       <c r="GL31" s="177"/>
       <c r="GM31" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GN31" s="245"/>
       <c r="GO31" s="245"/>
       <c r="GP31" s="245"/>
       <c r="GQ31" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GR31" s="245"/>
       <c r="GS31" s="245"/>
       <c r="GT31" s="245"/>
       <c r="GU31" s="245" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="GV31" s="245"/>
       <c r="GW31" s="245"/>
       <c r="GX31" s="245"/>
       <c r="GY31" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GZ31" s="245"/>
       <c r="HA31" s="245"/>
       <c r="HB31" s="245"/>
       <c r="HC31" s="245" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="HD31" s="220"/>
       <c r="HE31" s="220"/>
@@ -15931,7 +15931,7 @@
     </row>
     <row r="32" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="80" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B32" s="99"/>
       <c r="C32" s="99"/>
@@ -16127,31 +16127,31 @@
       <c r="GK32" s="177"/>
       <c r="GL32" s="177"/>
       <c r="GM32" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GN32" s="245"/>
       <c r="GO32" s="245"/>
       <c r="GP32" s="245"/>
       <c r="GQ32" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GR32" s="245"/>
       <c r="GS32" s="245"/>
       <c r="GT32" s="245"/>
       <c r="GU32" s="245" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="GV32" s="245"/>
       <c r="GW32" s="245"/>
       <c r="GX32" s="245"/>
       <c r="GY32" s="245" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="GZ32" s="245"/>
       <c r="HA32" s="245"/>
       <c r="HB32" s="245"/>
       <c r="HC32" s="245" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="HD32" s="220"/>
       <c r="HE32" s="220"/>
@@ -16777,7 +16777,7 @@
       <c r="DE34" s="107"/>
       <c r="DF34" s="107"/>
       <c r="DG34" s="107" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="DH34" s="107"/>
       <c r="DI34" s="107"/>
@@ -17103,7 +17103,7 @@
       <c r="EW35" s="107"/>
       <c r="EX35" s="107"/>
       <c r="EY35" s="107" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="EZ35" s="107"/>
       <c r="FA35" s="107"/>
@@ -17571,7 +17571,7 @@
         <v>0</v>
       </c>
       <c r="CU37" s="107">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="CV37" s="107">
         <f t="shared" si="3"/>
@@ -17924,7 +17924,7 @@
       <c r="DE38" s="107"/>
       <c r="DF38" s="107"/>
       <c r="DG38" s="107" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="DH38" s="107"/>
       <c r="DI38" s="107"/>
@@ -19422,7 +19422,7 @@
       <c r="CK43" s="111"/>
       <c r="CL43" s="111"/>
       <c r="CM43" s="111" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="CN43" s="111"/>
       <c r="CO43" s="111"/>
@@ -19434,7 +19434,7 @@
       <c r="CS43" s="111"/>
       <c r="CT43" s="111"/>
       <c r="CU43" s="111" t="s">
-        <v>693</v>
+        <v>855</v>
       </c>
       <c r="CV43" s="111"/>
       <c r="CW43" s="111"/>
@@ -19516,7 +19516,7 @@
       <c r="EW43" s="185"/>
       <c r="EX43" s="185"/>
       <c r="EY43" s="209" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="EZ43" s="185"/>
       <c r="FA43" s="185"/>
@@ -19844,7 +19844,7 @@
     </row>
     <row r="45" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="157" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B45" s="110"/>
       <c r="C45" s="110"/>
@@ -19883,7 +19883,7 @@
       <c r="AJ45" s="92"/>
       <c r="AK45" s="92"/>
       <c r="AL45" s="165" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AM45" s="162"/>
       <c r="AN45" s="162"/>
@@ -19925,112 +19925,112 @@
       <c r="BX45" s="166"/>
       <c r="BY45" s="250"/>
       <c r="BZ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CA45" s="208" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CB45" s="111"/>
       <c r="CC45" s="111"/>
       <c r="CD45" s="111"/>
       <c r="CE45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CF45" s="111"/>
       <c r="CG45" s="111"/>
       <c r="CH45" s="111"/>
       <c r="CI45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="CJ45" s="111"/>
       <c r="CK45" s="111"/>
       <c r="CL45" s="111"/>
       <c r="CM45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CN45" s="111"/>
       <c r="CO45" s="111"/>
       <c r="CP45" s="111"/>
       <c r="CQ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CR45" s="111"/>
       <c r="CS45" s="111"/>
       <c r="CT45" s="111"/>
       <c r="CU45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CV45" s="111"/>
       <c r="CW45" s="111"/>
       <c r="CX45" s="111"/>
       <c r="CY45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CZ45" s="111"/>
       <c r="DA45" s="111"/>
       <c r="DB45" s="111"/>
       <c r="DC45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DD45" s="111"/>
       <c r="DE45" s="111"/>
       <c r="DF45" s="111"/>
       <c r="DG45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="DH45" s="111"/>
       <c r="DI45" s="111"/>
       <c r="DJ45" s="111"/>
       <c r="DK45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DL45" s="111"/>
       <c r="DM45" s="111"/>
       <c r="DN45" s="111"/>
       <c r="DO45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DP45" s="111"/>
       <c r="DQ45" s="111"/>
       <c r="DR45" s="111"/>
       <c r="DS45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="DT45" s="111"/>
       <c r="DU45" s="111"/>
       <c r="DV45" s="111"/>
       <c r="DW45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DX45" s="111"/>
       <c r="DY45" s="111"/>
       <c r="DZ45" s="111"/>
       <c r="EA45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EB45" s="111"/>
       <c r="EC45" s="111"/>
       <c r="ED45" s="111"/>
       <c r="EE45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EF45" s="111"/>
       <c r="EG45" s="111"/>
       <c r="EH45" s="111"/>
       <c r="EI45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EJ45" s="111"/>
       <c r="EK45" s="111"/>
       <c r="EL45" s="111"/>
       <c r="EM45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EN45" s="111"/>
       <c r="EO45" s="111"/>
       <c r="EP45" s="111"/>
       <c r="EQ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="ER45" s="185"/>
       <c r="ES45" s="185"/>
@@ -20040,13 +20040,13 @@
       <c r="EW45" s="185"/>
       <c r="EX45" s="185"/>
       <c r="EY45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EZ45" s="185"/>
       <c r="FA45" s="185"/>
       <c r="FB45" s="185"/>
       <c r="FC45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="FD45" s="185"/>
       <c r="FE45" s="185"/>
@@ -20145,14 +20145,14 @@
       <c r="AJ46" s="89"/>
       <c r="AK46" s="89"/>
       <c r="AL46" s="165" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="AM46" s="162"/>
       <c r="AN46" s="162" t="s">
         <v>285</v>
       </c>
       <c r="AO46" s="162" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="AP46" s="162"/>
       <c r="AQ46" s="162"/>
@@ -20191,112 +20191,112 @@
       <c r="BX46" s="167"/>
       <c r="BY46" s="252"/>
       <c r="BZ46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA46" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB46" s="111"/>
       <c r="CC46" s="111"/>
       <c r="CD46" s="111"/>
       <c r="CE46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF46" s="111"/>
       <c r="CG46" s="111"/>
       <c r="CH46" s="111"/>
       <c r="CI46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ46" s="111"/>
       <c r="CK46" s="111"/>
       <c r="CL46" s="111"/>
       <c r="CM46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN46" s="111"/>
       <c r="CO46" s="111"/>
       <c r="CP46" s="111"/>
       <c r="CQ46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR46" s="111"/>
       <c r="CS46" s="111"/>
       <c r="CT46" s="111"/>
       <c r="CU46" s="111" t="s">
-        <v>784</v>
+        <v>856</v>
       </c>
       <c r="CV46" s="111"/>
       <c r="CW46" s="111"/>
       <c r="CX46" s="111"/>
       <c r="CY46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ46" s="111"/>
       <c r="DA46" s="111"/>
       <c r="DB46" s="111"/>
       <c r="DC46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD46" s="111"/>
       <c r="DE46" s="111"/>
       <c r="DF46" s="111"/>
       <c r="DG46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH46" s="111"/>
       <c r="DI46" s="111"/>
       <c r="DJ46" s="111"/>
       <c r="DK46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL46" s="111"/>
       <c r="DM46" s="111"/>
       <c r="DN46" s="111"/>
       <c r="DO46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP46" s="111"/>
       <c r="DQ46" s="111"/>
       <c r="DR46" s="111"/>
       <c r="DS46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT46" s="111"/>
       <c r="DU46" s="111"/>
       <c r="DV46" s="111"/>
       <c r="DW46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX46" s="111"/>
       <c r="DY46" s="111"/>
       <c r="DZ46" s="111"/>
       <c r="EA46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB46" s="111"/>
       <c r="EC46" s="111"/>
       <c r="ED46" s="111"/>
       <c r="EE46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF46" s="111"/>
       <c r="EG46" s="111"/>
       <c r="EH46" s="111"/>
       <c r="EI46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ46" s="111"/>
       <c r="EK46" s="111"/>
       <c r="EL46" s="111"/>
       <c r="EM46" s="111" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="EN46" s="111"/>
       <c r="EO46" s="111"/>
       <c r="EP46" s="111"/>
       <c r="EQ46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER46" s="111"/>
       <c r="ES46" s="111"/>
@@ -20306,13 +20306,13 @@
       <c r="EW46" s="111"/>
       <c r="EX46" s="111"/>
       <c r="EY46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ46" s="111"/>
       <c r="FA46" s="111"/>
       <c r="FB46" s="111"/>
       <c r="FC46" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD46" s="111"/>
       <c r="FE46" s="111"/>
@@ -20423,7 +20423,7 @@
         <v>283</v>
       </c>
       <c r="AL47" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM47" s="162"/>
       <c r="AN47" s="162"/>
@@ -20513,112 +20513,112 @@
         <v>283</v>
       </c>
       <c r="BZ47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA47" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB47" s="111"/>
       <c r="CC47" s="111"/>
       <c r="CD47" s="111"/>
       <c r="CE47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF47" s="111"/>
       <c r="CG47" s="111"/>
       <c r="CH47" s="111"/>
       <c r="CI47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ47" s="111"/>
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
       <c r="CP47" s="111"/>
       <c r="CQ47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR47" s="111"/>
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>838</v>
+        <v>779</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
       <c r="CX47" s="111"/>
       <c r="CY47" s="111" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="CZ47" s="111"/>
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
       <c r="DF47" s="111"/>
       <c r="DG47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH47" s="111"/>
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>
       <c r="DN47" s="111"/>
       <c r="DO47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP47" s="111"/>
       <c r="DQ47" s="111"/>
       <c r="DR47" s="111"/>
       <c r="DS47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT47" s="111"/>
       <c r="DU47" s="111"/>
       <c r="DV47" s="111"/>
       <c r="DW47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX47" s="111"/>
       <c r="DY47" s="111"/>
       <c r="DZ47" s="111"/>
       <c r="EA47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB47" s="111"/>
       <c r="EC47" s="111"/>
       <c r="ED47" s="111"/>
       <c r="EE47" s="111" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
       <c r="EF47" s="111"/>
       <c r="EG47" s="111"/>
       <c r="EH47" s="111"/>
       <c r="EI47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ47" s="111"/>
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
       <c r="EP47" s="111"/>
       <c r="EQ47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER47" s="111"/>
       <c r="ES47" s="111"/>
@@ -20628,13 +20628,13 @@
       <c r="EW47" s="111"/>
       <c r="EX47" s="207"/>
       <c r="EY47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ47" s="208"/>
       <c r="FA47" s="208"/>
       <c r="FB47" s="208"/>
       <c r="FC47" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD47" s="111"/>
       <c r="FE47" s="111"/>
@@ -20733,7 +20733,7 @@
       <c r="AJ48" s="89"/>
       <c r="AK48" s="89"/>
       <c r="AL48" s="165" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="AM48" s="162"/>
       <c r="AN48" s="162"/>
@@ -20775,112 +20775,112 @@
       <c r="BX48" s="167"/>
       <c r="BY48" s="252"/>
       <c r="BZ48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA48" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB48" s="111"/>
       <c r="CC48" s="111"/>
       <c r="CD48" s="111"/>
       <c r="CE48" s="111" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="CF48" s="111"/>
       <c r="CG48" s="111"/>
       <c r="CH48" s="111"/>
       <c r="CI48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ48" s="111"/>
       <c r="CK48" s="111"/>
       <c r="CL48" s="111"/>
       <c r="CM48" s="111" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="CN48" s="111"/>
       <c r="CO48" s="111"/>
       <c r="CP48" s="111"/>
       <c r="CQ48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR48" s="111"/>
       <c r="CS48" s="111"/>
       <c r="CT48" s="111"/>
       <c r="CU48" s="111" t="s">
-        <v>782</v>
+        <v>857</v>
       </c>
       <c r="CV48" s="111"/>
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
       <c r="DF48" s="111"/>
       <c r="DG48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH48" s="111"/>
       <c r="DI48" s="111"/>
       <c r="DJ48" s="111"/>
       <c r="DK48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL48" s="111"/>
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
       <c r="DR48" s="111"/>
       <c r="DS48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT48" s="111"/>
       <c r="DU48" s="111"/>
       <c r="DV48" s="111"/>
       <c r="DW48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX48" s="111"/>
       <c r="DY48" s="111"/>
       <c r="DZ48" s="111"/>
       <c r="EA48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB48" s="111"/>
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
       <c r="EL48" s="111"/>
       <c r="EM48" s="111" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="EN48" s="111"/>
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20890,13 +20890,13 @@
       <c r="EW48" s="111"/>
       <c r="EX48" s="111"/>
       <c r="EY48" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ48" s="111"/>
       <c r="FA48" s="111"/>
       <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -20956,7 +20956,7 @@
     </row>
     <row r="49" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="62" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="110"/>
@@ -20995,7 +20995,7 @@
       <c r="AJ49" s="89"/>
       <c r="AK49" s="89"/>
       <c r="AL49" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM49" s="162"/>
       <c r="AN49" s="162"/>
@@ -21037,112 +21037,112 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="CA49" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB49" s="111"/>
       <c r="CC49" s="111"/>
       <c r="CD49" s="111"/>
       <c r="CE49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF49" s="111"/>
       <c r="CG49" s="111"/>
       <c r="CH49" s="111"/>
       <c r="CI49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ49" s="111"/>
       <c r="CK49" s="111"/>
       <c r="CL49" s="111"/>
       <c r="CM49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN49" s="111"/>
       <c r="CO49" s="111"/>
       <c r="CP49" s="111"/>
       <c r="CQ49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR49" s="111"/>
       <c r="CS49" s="111"/>
       <c r="CT49" s="111"/>
       <c r="CU49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CV49" s="111"/>
       <c r="CW49" s="111"/>
       <c r="CX49" s="111"/>
       <c r="CY49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ49" s="111"/>
       <c r="DA49" s="111"/>
       <c r="DB49" s="111"/>
       <c r="DC49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD49" s="111"/>
       <c r="DE49" s="111"/>
       <c r="DF49" s="111"/>
       <c r="DG49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH49" s="111"/>
       <c r="DI49" s="111"/>
       <c r="DJ49" s="111"/>
       <c r="DK49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL49" s="111"/>
       <c r="DM49" s="111"/>
       <c r="DN49" s="111"/>
       <c r="DO49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP49" s="111"/>
       <c r="DQ49" s="111"/>
       <c r="DR49" s="111"/>
       <c r="DS49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT49" s="111"/>
       <c r="DU49" s="111"/>
       <c r="DV49" s="111"/>
       <c r="DW49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX49" s="111"/>
       <c r="DY49" s="111"/>
       <c r="DZ49" s="111"/>
       <c r="EA49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB49" s="111"/>
       <c r="EC49" s="111"/>
       <c r="ED49" s="111"/>
       <c r="EE49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF49" s="111"/>
       <c r="EG49" s="111"/>
       <c r="EH49" s="111"/>
       <c r="EI49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ49" s="111"/>
       <c r="EK49" s="111"/>
       <c r="EL49" s="111"/>
       <c r="EM49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN49" s="111"/>
       <c r="EO49" s="111"/>
       <c r="EP49" s="111"/>
       <c r="EQ49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER49" s="111"/>
       <c r="ES49" s="111"/>
@@ -21152,13 +21152,13 @@
       <c r="EW49" s="111"/>
       <c r="EX49" s="207"/>
       <c r="EY49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ49" s="208"/>
       <c r="FA49" s="208"/>
       <c r="FB49" s="208"/>
       <c r="FC49" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD49" s="111"/>
       <c r="FE49" s="111"/>
@@ -21257,7 +21257,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21299,112 +21299,112 @@
       <c r="BX50" s="167"/>
       <c r="BY50" s="252"/>
       <c r="BZ50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA50" s="208" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
       <c r="CH50" s="111"/>
       <c r="CI50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ50" s="111"/>
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
       <c r="CP50" s="111"/>
       <c r="CQ50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR50" s="111"/>
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>800</v>
+        <v>858</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>857</v>
+        <v>848</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
       <c r="DF50" s="111"/>
       <c r="DG50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH50" s="111"/>
       <c r="DI50" s="111"/>
       <c r="DJ50" s="111"/>
       <c r="DK50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL50" s="111"/>
       <c r="DM50" s="111"/>
       <c r="DN50" s="111"/>
       <c r="DO50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP50" s="111"/>
       <c r="DQ50" s="111"/>
       <c r="DR50" s="111"/>
       <c r="DS50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT50" s="111"/>
       <c r="DU50" s="111"/>
       <c r="DV50" s="111"/>
       <c r="DW50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX50" s="111"/>
       <c r="DY50" s="111"/>
       <c r="DZ50" s="111"/>
       <c r="EA50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB50" s="111"/>
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21414,13 +21414,13 @@
       <c r="EW50" s="111"/>
       <c r="EX50" s="207"/>
       <c r="EY50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ50" s="208"/>
       <c r="FA50" s="208"/>
       <c r="FB50" s="208"/>
       <c r="FC50" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD50" s="111"/>
       <c r="FE50" s="111"/>
@@ -21480,7 +21480,7 @@
     </row>
     <row r="51" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="62" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B51" s="110"/>
       <c r="C51" s="110"/>
@@ -21519,7 +21519,7 @@
       <c r="AJ51" s="89"/>
       <c r="AK51" s="89"/>
       <c r="AL51" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM51" s="162"/>
       <c r="AN51" s="162"/>
@@ -21561,112 +21561,112 @@
       <c r="BX51" s="167"/>
       <c r="BY51" s="252"/>
       <c r="BZ51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA51" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB51" s="111"/>
       <c r="CC51" s="111"/>
       <c r="CD51" s="111"/>
       <c r="CE51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF51" s="111"/>
       <c r="CG51" s="111"/>
       <c r="CH51" s="111"/>
       <c r="CI51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ51" s="111"/>
       <c r="CK51" s="111"/>
       <c r="CL51" s="111"/>
       <c r="CM51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN51" s="111"/>
       <c r="CO51" s="111"/>
       <c r="CP51" s="111"/>
       <c r="CQ51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR51" s="111"/>
       <c r="CS51" s="111"/>
       <c r="CT51" s="111"/>
       <c r="CU51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CV51" s="111"/>
       <c r="CW51" s="111"/>
       <c r="CX51" s="111"/>
       <c r="CY51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ51" s="111"/>
       <c r="DA51" s="111"/>
       <c r="DB51" s="111"/>
       <c r="DC51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD51" s="111"/>
       <c r="DE51" s="111"/>
       <c r="DF51" s="111"/>
       <c r="DG51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH51" s="111"/>
       <c r="DI51" s="111"/>
       <c r="DJ51" s="111"/>
       <c r="DK51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL51" s="111"/>
       <c r="DM51" s="111"/>
       <c r="DN51" s="111"/>
       <c r="DO51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP51" s="111"/>
       <c r="DQ51" s="111"/>
       <c r="DR51" s="111"/>
       <c r="DS51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT51" s="111"/>
       <c r="DU51" s="111"/>
       <c r="DV51" s="111"/>
       <c r="DW51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX51" s="111"/>
       <c r="DY51" s="111"/>
       <c r="DZ51" s="111"/>
       <c r="EA51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB51" s="111"/>
       <c r="EC51" s="111"/>
       <c r="ED51" s="111"/>
       <c r="EE51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF51" s="111"/>
       <c r="EG51" s="111"/>
       <c r="EH51" s="111"/>
       <c r="EI51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ51" s="111"/>
       <c r="EK51" s="111"/>
       <c r="EL51" s="111"/>
       <c r="EM51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN51" s="111"/>
       <c r="EO51" s="111"/>
       <c r="EP51" s="111"/>
       <c r="EQ51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER51" s="111"/>
       <c r="ES51" s="111"/>
@@ -21676,13 +21676,13 @@
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
       <c r="FB51" s="208"/>
       <c r="FC51" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD51" s="111"/>
       <c r="FE51" s="111"/>
@@ -21781,7 +21781,7 @@
       <c r="AJ52" s="89"/>
       <c r="AK52" s="89"/>
       <c r="AL52" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM52" s="162"/>
       <c r="AN52" s="162"/>
@@ -21823,112 +21823,112 @@
       <c r="BX52" s="167"/>
       <c r="BY52" s="252"/>
       <c r="BZ52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA52" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB52" s="111"/>
       <c r="CC52" s="111"/>
       <c r="CD52" s="111"/>
       <c r="CE52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF52" s="111"/>
       <c r="CG52" s="111"/>
       <c r="CH52" s="111"/>
       <c r="CI52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ52" s="111"/>
       <c r="CK52" s="111"/>
       <c r="CL52" s="111"/>
       <c r="CM52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN52" s="111"/>
       <c r="CO52" s="111"/>
       <c r="CP52" s="111"/>
       <c r="CQ52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR52" s="111"/>
       <c r="CS52" s="111"/>
       <c r="CT52" s="111"/>
       <c r="CU52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CV52" s="111"/>
       <c r="CW52" s="111"/>
       <c r="CX52" s="111"/>
       <c r="CY52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ52" s="111"/>
       <c r="DA52" s="111"/>
       <c r="DB52" s="111"/>
       <c r="DC52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD52" s="111"/>
       <c r="DE52" s="111"/>
       <c r="DF52" s="111"/>
       <c r="DG52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH52" s="111"/>
       <c r="DI52" s="111"/>
       <c r="DJ52" s="111"/>
       <c r="DK52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL52" s="111"/>
       <c r="DM52" s="111"/>
       <c r="DN52" s="111"/>
       <c r="DO52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP52" s="111"/>
       <c r="DQ52" s="111"/>
       <c r="DR52" s="111"/>
       <c r="DS52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT52" s="111"/>
       <c r="DU52" s="111"/>
       <c r="DV52" s="111"/>
       <c r="DW52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX52" s="111"/>
       <c r="DY52" s="111"/>
       <c r="DZ52" s="111"/>
       <c r="EA52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB52" s="111"/>
       <c r="EC52" s="111"/>
       <c r="ED52" s="111"/>
       <c r="EE52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF52" s="111"/>
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
       <c r="EL52" s="111"/>
       <c r="EM52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN52" s="111"/>
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -21938,13 +21938,13 @@
       <c r="EW52" s="111"/>
       <c r="EX52" s="207"/>
       <c r="EY52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ52" s="208"/>
       <c r="FA52" s="208"/>
       <c r="FB52" s="208"/>
       <c r="FC52" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD52" s="111"/>
       <c r="FE52" s="111"/>
@@ -22004,7 +22004,7 @@
     </row>
     <row r="53" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="B53" s="110"/>
       <c r="C53" s="110"/>
@@ -22055,7 +22055,7 @@
         <v>283</v>
       </c>
       <c r="AL53" s="165" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22145,112 +22145,112 @@
         <v>283</v>
       </c>
       <c r="BZ53" s="111" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
       <c r="CA53" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB53" s="111"/>
       <c r="CC53" s="111"/>
       <c r="CD53" s="111"/>
       <c r="CE53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF53" s="111"/>
       <c r="CG53" s="111"/>
       <c r="CH53" s="111"/>
       <c r="CI53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ53" s="111"/>
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
       <c r="CP53" s="111"/>
       <c r="CQ53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR53" s="111"/>
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>838</v>
+        <v>859</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
       <c r="CX53" s="111"/>
       <c r="CY53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ53" s="111"/>
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
       <c r="DF53" s="111"/>
       <c r="DG53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH53" s="111"/>
       <c r="DI53" s="111"/>
       <c r="DJ53" s="111"/>
       <c r="DK53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL53" s="111"/>
       <c r="DM53" s="111"/>
       <c r="DN53" s="111"/>
       <c r="DO53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP53" s="111"/>
       <c r="DQ53" s="111"/>
       <c r="DR53" s="111"/>
       <c r="DS53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT53" s="111"/>
       <c r="DU53" s="111"/>
       <c r="DV53" s="111"/>
       <c r="DW53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX53" s="111"/>
       <c r="DY53" s="111"/>
       <c r="DZ53" s="111"/>
       <c r="EA53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB53" s="111"/>
       <c r="EC53" s="111"/>
       <c r="ED53" s="111"/>
       <c r="EE53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF53" s="111"/>
       <c r="EG53" s="111"/>
       <c r="EH53" s="111"/>
       <c r="EI53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ53" s="111"/>
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
       <c r="EP53" s="111"/>
       <c r="EQ53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER53" s="111"/>
       <c r="ES53" s="111"/>
@@ -22260,13 +22260,13 @@
       <c r="EW53" s="111"/>
       <c r="EX53" s="207"/>
       <c r="EY53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ53" s="208"/>
       <c r="FA53" s="208"/>
       <c r="FB53" s="208"/>
       <c r="FC53" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD53" s="111"/>
       <c r="FE53" s="111"/>
@@ -22335,7 +22335,7 @@
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
       <c r="H54" s="110" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="I54" s="110" t="s">
         <v>545</v>
@@ -22369,7 +22369,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22411,46 +22411,46 @@
       <c r="BX54" s="167"/>
       <c r="BY54" s="252"/>
       <c r="BZ54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA54" s="208" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="CB54" s="111"/>
       <c r="CC54" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD54" s="111" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="CE54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF54" s="111"/>
       <c r="CG54" s="111"/>
       <c r="CH54" s="111"/>
       <c r="CI54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ54" s="111"/>
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="CN54" s="111"/>
       <c r="CO54" s="111" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR54" s="111"/>
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>813</v>
+        <v>851</v>
       </c>
       <c r="CV54" s="111"/>
       <c r="CW54" s="111" t="s">
@@ -22458,7 +22458,7 @@
       </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="CZ54" s="111" t="s">
         <v>547</v>
@@ -22468,7 +22468,7 @@
       </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="DD54" s="111" t="s">
         <v>546</v>
@@ -22476,47 +22476,47 @@
       <c r="DE54" s="111"/>
       <c r="DF54" s="111"/>
       <c r="DG54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH54" s="111"/>
       <c r="DI54" s="111"/>
       <c r="DJ54" s="111"/>
       <c r="DK54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL54" s="111"/>
       <c r="DM54" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN54" s="111" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="DO54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP54" s="111"/>
       <c r="DQ54" s="111"/>
       <c r="DR54" s="111"/>
       <c r="DS54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT54" s="111"/>
       <c r="DU54" s="111"/>
       <c r="DV54" s="111"/>
       <c r="DW54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX54" s="111"/>
       <c r="DY54" s="111"/>
       <c r="DZ54" s="111"/>
       <c r="EA54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB54" s="111"/>
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="EF54" s="111"/>
       <c r="EG54" s="111" t="s">
@@ -22524,7 +22524,7 @@
       </c>
       <c r="EH54" s="111"/>
       <c r="EI54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ54" s="111"/>
       <c r="EK54" s="111" t="s">
@@ -22532,13 +22532,13 @@
       </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
       <c r="EP54" s="111"/>
       <c r="EQ54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER54" s="111"/>
       <c r="ES54" s="111" t="s">
@@ -22550,13 +22550,13 @@
       <c r="EW54" s="111"/>
       <c r="EX54" s="207"/>
       <c r="EY54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ54" s="208"/>
       <c r="FA54" s="208"/>
       <c r="FB54" s="208"/>
       <c r="FC54" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD54" s="111"/>
       <c r="FE54" s="111"/>
@@ -22625,7 +22625,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
       <c r="H55" s="110" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="I55" s="110" t="s">
         <v>545</v>
@@ -22659,11 +22659,11 @@
       <c r="AJ55" s="89"/>
       <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="AM55" s="162"/>
       <c r="AN55" s="162" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
@@ -22703,46 +22703,46 @@
       <c r="BX55" s="167"/>
       <c r="BY55" s="252"/>
       <c r="BZ55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA55" s="208" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="CB55" s="111"/>
       <c r="CC55" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD55" s="111" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="CE55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF55" s="111"/>
       <c r="CG55" s="111"/>
       <c r="CH55" s="111"/>
       <c r="CI55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ55" s="111"/>
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="CN55" s="111"/>
       <c r="CO55" s="111" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR55" s="111"/>
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>822</v>
+        <v>860</v>
       </c>
       <c r="CV55" s="111"/>
       <c r="CW55" s="111" t="s">
@@ -22750,13 +22750,13 @@
       </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
       <c r="DB55" s="111"/>
       <c r="DC55" s="111" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="DD55" s="111" t="s">
         <v>546</v>
@@ -22764,65 +22764,65 @@
       <c r="DE55" s="111"/>
       <c r="DF55" s="111"/>
       <c r="DG55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH55" s="111"/>
       <c r="DI55" s="111"/>
       <c r="DJ55" s="111"/>
       <c r="DK55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL55" s="111"/>
       <c r="DM55" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN55" s="111" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="DO55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP55" s="111"/>
       <c r="DQ55" s="111"/>
       <c r="DR55" s="111"/>
       <c r="DS55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT55" s="111"/>
       <c r="DU55" s="111"/>
       <c r="DV55" s="111"/>
       <c r="DW55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX55" s="111"/>
       <c r="DY55" s="111"/>
       <c r="DZ55" s="111"/>
       <c r="EA55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB55" s="111"/>
       <c r="EC55" s="111"/>
       <c r="ED55" s="111"/>
       <c r="EE55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF55" s="111"/>
       <c r="EG55" s="111"/>
       <c r="EH55" s="111"/>
       <c r="EI55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ55" s="111"/>
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
       <c r="EP55" s="111"/>
       <c r="EQ55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER55" s="111"/>
       <c r="ES55" s="111"/>
@@ -22832,13 +22832,13 @@
       <c r="EW55" s="111"/>
       <c r="EX55" s="207"/>
       <c r="EY55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ55" s="208"/>
       <c r="FA55" s="208"/>
       <c r="FB55" s="208"/>
       <c r="FC55" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD55" s="111"/>
       <c r="FE55" s="111"/>
@@ -22937,7 +22937,7 @@
       <c r="AJ56" s="89"/>
       <c r="AK56" s="89"/>
       <c r="AL56" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM56" s="162"/>
       <c r="AN56" s="162"/>
@@ -22979,112 +22979,112 @@
       <c r="BX56" s="167"/>
       <c r="BY56" s="252"/>
       <c r="BZ56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA56" s="208" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
       <c r="CH56" s="111"/>
       <c r="CI56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ56" s="111"/>
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
       <c r="CP56" s="111"/>
       <c r="CQ56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR56" s="111"/>
       <c r="CS56" s="111"/>
       <c r="CT56" s="111"/>
       <c r="CU56" s="111" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="CV56" s="111"/>
       <c r="CW56" s="111"/>
       <c r="CX56" s="111"/>
       <c r="CY56" s="111" t="s">
-        <v>858</v>
+        <v>849</v>
       </c>
       <c r="CZ56" s="111"/>
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
       <c r="DF56" s="111"/>
       <c r="DG56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH56" s="111"/>
       <c r="DI56" s="111"/>
       <c r="DJ56" s="111"/>
       <c r="DK56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL56" s="111"/>
       <c r="DM56" s="111"/>
       <c r="DN56" s="111"/>
       <c r="DO56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP56" s="111"/>
       <c r="DQ56" s="111"/>
       <c r="DR56" s="111"/>
       <c r="DS56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT56" s="111"/>
       <c r="DU56" s="111"/>
       <c r="DV56" s="111"/>
       <c r="DW56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX56" s="111"/>
       <c r="DY56" s="111"/>
       <c r="DZ56" s="111"/>
       <c r="EA56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB56" s="111"/>
       <c r="EC56" s="111"/>
       <c r="ED56" s="111"/>
       <c r="EE56" s="111" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
       <c r="EF56" s="111"/>
       <c r="EG56" s="111"/>
       <c r="EH56" s="111"/>
       <c r="EI56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ56" s="111"/>
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
       <c r="EP56" s="111"/>
       <c r="EQ56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER56" s="111"/>
       <c r="ES56" s="111"/>
@@ -23094,13 +23094,13 @@
       <c r="EW56" s="111"/>
       <c r="EX56" s="207"/>
       <c r="EY56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ56" s="208"/>
       <c r="FA56" s="208"/>
       <c r="FB56" s="208"/>
       <c r="FC56" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD56" s="111"/>
       <c r="FE56" s="111"/>
@@ -23199,7 +23199,7 @@
       <c r="AJ57" s="89"/>
       <c r="AK57" s="89"/>
       <c r="AL57" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM57" s="162"/>
       <c r="AN57" s="162"/>
@@ -23241,112 +23241,112 @@
       <c r="BX57" s="167"/>
       <c r="BY57" s="252"/>
       <c r="BZ57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA57" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB57" s="111"/>
       <c r="CC57" s="111"/>
       <c r="CD57" s="111"/>
       <c r="CE57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF57" s="111"/>
       <c r="CG57" s="111"/>
       <c r="CH57" s="111"/>
       <c r="CI57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ57" s="111"/>
       <c r="CK57" s="111"/>
       <c r="CL57" s="111"/>
       <c r="CM57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN57" s="111"/>
       <c r="CO57" s="111"/>
       <c r="CP57" s="111"/>
       <c r="CQ57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR57" s="111"/>
       <c r="CS57" s="111"/>
       <c r="CT57" s="111"/>
       <c r="CU57" s="111" t="s">
-        <v>784</v>
+        <v>856</v>
       </c>
       <c r="CV57" s="111"/>
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
       <c r="DB57" s="111"/>
       <c r="DC57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD57" s="111"/>
       <c r="DE57" s="111"/>
       <c r="DF57" s="111"/>
       <c r="DG57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH57" s="111"/>
       <c r="DI57" s="111"/>
       <c r="DJ57" s="111"/>
       <c r="DK57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL57" s="111"/>
       <c r="DM57" s="111"/>
       <c r="DN57" s="111"/>
       <c r="DO57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP57" s="111"/>
       <c r="DQ57" s="111"/>
       <c r="DR57" s="111"/>
       <c r="DS57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT57" s="111"/>
       <c r="DU57" s="111"/>
       <c r="DV57" s="111"/>
       <c r="DW57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX57" s="111"/>
       <c r="DY57" s="111"/>
       <c r="DZ57" s="111"/>
       <c r="EA57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB57" s="111"/>
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
       <c r="EH57" s="111"/>
       <c r="EI57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ57" s="111"/>
       <c r="EK57" s="111"/>
       <c r="EL57" s="111"/>
       <c r="EM57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN57" s="111"/>
       <c r="EO57" s="111"/>
       <c r="EP57" s="111"/>
       <c r="EQ57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER57" s="111"/>
       <c r="ES57" s="111"/>
@@ -23356,13 +23356,13 @@
       <c r="EW57" s="111"/>
       <c r="EX57" s="207"/>
       <c r="EY57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ57" s="208"/>
       <c r="FA57" s="208"/>
       <c r="FB57" s="208"/>
       <c r="FC57" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD57" s="111"/>
       <c r="FE57" s="111"/>
@@ -23461,7 +23461,7 @@
       <c r="AJ58" s="90"/>
       <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23503,112 +23503,112 @@
       <c r="BX58" s="167"/>
       <c r="BY58" s="252"/>
       <c r="BZ58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA58" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB58" s="111"/>
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
       <c r="CH58" s="111"/>
       <c r="CI58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ58" s="111"/>
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
       <c r="CP58" s="111"/>
       <c r="CQ58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR58" s="111"/>
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>832</v>
+        <v>861</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
       <c r="DF58" s="111"/>
       <c r="DG58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH58" s="111"/>
       <c r="DI58" s="111"/>
       <c r="DJ58" s="111"/>
       <c r="DK58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL58" s="111"/>
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
       <c r="DR58" s="111"/>
       <c r="DS58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT58" s="111"/>
       <c r="DU58" s="111"/>
       <c r="DV58" s="111"/>
       <c r="DW58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX58" s="111"/>
       <c r="DY58" s="111"/>
       <c r="DZ58" s="111"/>
       <c r="EA58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB58" s="111"/>
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23618,13 +23618,13 @@
       <c r="EW58" s="111"/>
       <c r="EX58" s="207"/>
       <c r="EY58" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ58" s="208"/>
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
       <c r="FC58" s="208" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23723,7 +23723,7 @@
       <c r="AJ59" s="90"/>
       <c r="AK59" s="90"/>
       <c r="AL59" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM59" s="162"/>
       <c r="AN59" s="162"/>
@@ -23765,112 +23765,112 @@
       <c r="BX59" s="167"/>
       <c r="BY59" s="252"/>
       <c r="BZ59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA59" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB59" s="111"/>
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
       <c r="CH59" s="111"/>
       <c r="CI59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ59" s="111"/>
       <c r="CK59" s="111"/>
       <c r="CL59" s="111"/>
       <c r="CM59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN59" s="111"/>
       <c r="CO59" s="111"/>
       <c r="CP59" s="111"/>
       <c r="CQ59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CR59" s="111"/>
       <c r="CS59" s="111"/>
       <c r="CT59" s="111"/>
       <c r="CU59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CV59" s="111"/>
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>861</v>
+        <v>852</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
       <c r="DB59" s="111"/>
       <c r="DC59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD59" s="111"/>
       <c r="DE59" s="111"/>
       <c r="DF59" s="111"/>
       <c r="DG59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH59" s="111"/>
       <c r="DI59" s="111"/>
       <c r="DJ59" s="111"/>
       <c r="DK59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL59" s="111"/>
       <c r="DM59" s="111"/>
       <c r="DN59" s="111"/>
       <c r="DO59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP59" s="111"/>
       <c r="DQ59" s="111"/>
       <c r="DR59" s="111"/>
       <c r="DS59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT59" s="111"/>
       <c r="DU59" s="111"/>
       <c r="DV59" s="111"/>
       <c r="DW59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX59" s="111"/>
       <c r="DY59" s="111"/>
       <c r="DZ59" s="111"/>
       <c r="EA59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB59" s="111"/>
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
       <c r="EH59" s="111"/>
       <c r="EI59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ59" s="111"/>
       <c r="EK59" s="111"/>
       <c r="EL59" s="111"/>
       <c r="EM59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN59" s="111"/>
       <c r="EO59" s="111"/>
       <c r="EP59" s="111"/>
       <c r="EQ59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER59" s="111"/>
       <c r="ES59" s="111"/>
@@ -23880,13 +23880,13 @@
       <c r="EW59" s="111"/>
       <c r="EX59" s="207"/>
       <c r="EY59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ59" s="208"/>
       <c r="FA59" s="208"/>
       <c r="FB59" s="208"/>
       <c r="FC59" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="FD59" s="111"/>
       <c r="FE59" s="111"/>
@@ -23985,7 +23985,7 @@
       <c r="AJ60" s="90"/>
       <c r="AK60" s="90"/>
       <c r="AL60" s="165" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="AM60" s="162"/>
       <c r="AN60" s="162"/>
@@ -24027,112 +24027,112 @@
       <c r="BX60" s="167"/>
       <c r="BY60" s="252"/>
       <c r="BZ60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CA60" s="111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="CB60" s="111"/>
       <c r="CC60" s="111"/>
       <c r="CD60" s="111"/>
       <c r="CE60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CF60" s="111"/>
       <c r="CG60" s="111"/>
       <c r="CH60" s="111"/>
       <c r="CI60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CJ60" s="111"/>
       <c r="CK60" s="111"/>
       <c r="CL60" s="111"/>
       <c r="CM60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CN60" s="111"/>
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
       <c r="CT60" s="111"/>
       <c r="CU60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CV60" s="111"/>
       <c r="CW60" s="111"/>
       <c r="CX60" s="111"/>
       <c r="CY60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="CZ60" s="111"/>
       <c r="DA60" s="111"/>
       <c r="DB60" s="111"/>
       <c r="DC60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DD60" s="111"/>
       <c r="DE60" s="111"/>
       <c r="DF60" s="111"/>
       <c r="DG60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DH60" s="111"/>
       <c r="DI60" s="111"/>
       <c r="DJ60" s="111"/>
       <c r="DK60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DL60" s="111"/>
       <c r="DM60" s="111"/>
       <c r="DN60" s="111"/>
       <c r="DO60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DP60" s="111"/>
       <c r="DQ60" s="111"/>
       <c r="DR60" s="111"/>
       <c r="DS60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DT60" s="111"/>
       <c r="DU60" s="111"/>
       <c r="DV60" s="111"/>
       <c r="DW60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="DX60" s="111"/>
       <c r="DY60" s="111"/>
       <c r="DZ60" s="111"/>
       <c r="EA60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EB60" s="111"/>
       <c r="EC60" s="111"/>
       <c r="ED60" s="111"/>
       <c r="EE60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EF60" s="111"/>
       <c r="EG60" s="111"/>
       <c r="EH60" s="111"/>
       <c r="EI60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EJ60" s="111"/>
       <c r="EK60" s="111"/>
       <c r="EL60" s="111"/>
       <c r="EM60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EN60" s="111"/>
       <c r="EO60" s="111"/>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="ER60" s="111"/>
       <c r="ES60" s="111"/>
@@ -24142,13 +24142,13 @@
       <c r="EW60" s="111"/>
       <c r="EX60" s="207"/>
       <c r="EY60" s="111" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="EZ60" s="208"/>
       <c r="FA60" s="208"/>
       <c r="FB60" s="208"/>
       <c r="FC60" s="208" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="FD60" s="111"/>
       <c r="FE60" s="111"/>
@@ -33638,7 +33638,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="214" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D3" s="189" t="s">
         <v>603</v>
@@ -33647,31 +33647,31 @@
         <v>663</v>
       </c>
       <c r="F3" s="214" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="G3" s="214" t="s">
+        <v>739</v>
+      </c>
+      <c r="H3" s="214" t="s">
+        <v>740</v>
+      </c>
+      <c r="I3" s="214" t="s">
+        <v>741</v>
+      </c>
+      <c r="J3" s="214" t="s">
         <v>742</v>
       </c>
-      <c r="H3" s="214" t="s">
+      <c r="K3" s="214" t="s">
         <v>743</v>
       </c>
-      <c r="I3" s="214" t="s">
+      <c r="L3" s="214" t="s">
         <v>744</v>
       </c>
-      <c r="J3" s="214" t="s">
+      <c r="M3" s="214" t="s">
         <v>745</v>
       </c>
-      <c r="K3" s="214" t="s">
+      <c r="N3" s="214" t="s">
         <v>746</v>
-      </c>
-      <c r="L3" s="214" t="s">
-        <v>747</v>
-      </c>
-      <c r="M3" s="214" t="s">
-        <v>748</v>
-      </c>
-      <c r="N3" s="214" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -33683,62 +33683,62 @@
       <c r="D4" s="216"/>
       <c r="E4" s="216"/>
       <c r="F4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="H4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="I4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="J4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="K4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="L4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="M4" s="216" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="N4" s="216"/>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="215" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="B5" s="216"/>
       <c r="C5" s="216"/>
       <c r="D5" s="216"/>
       <c r="E5" s="216"/>
       <c r="F5" s="248" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="G5" s="248" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="H5" s="248" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="I5" s="248" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="J5" s="248" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="K5" s="248" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="L5" s="248" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="M5" s="248" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="N5" s="216"/>
     </row>
@@ -34087,10 +34087,10 @@
         <v>53</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D14" s="72" t="s">
         <v>606</v>
@@ -34099,28 +34099,28 @@
         <v>666</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="L14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="M14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N14" s="72" t="s">
         <v>226</v>
@@ -34213,38 +34213,38 @@
         <v>53</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D17" s="72" t="s">
         <v>607</v>
       </c>
       <c r="E17" s="72"/>
       <c r="F17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="L17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="M17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N17" s="72" t="s">
         <v>227</v>
@@ -34455,7 +34455,7 @@
       <c r="B23" s="72"/>
       <c r="C23" s="72"/>
       <c r="D23" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E23" s="72"/>
       <c r="F23" s="72" t="s">
@@ -34573,7 +34573,7 @@
       <c r="B26" s="72"/>
       <c r="C26" s="72"/>
       <c r="D26" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E26" s="72"/>
       <c r="F26" s="72" t="s">
@@ -35331,28 +35331,28 @@
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
       <c r="F46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="I46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="J46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="K46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="L46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="M46" s="72" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="N46" s="72"/>
     </row>
@@ -35365,28 +35365,28 @@
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
       <c r="F47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="I47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="K47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="L47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="M47" s="72" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="N47" s="72"/>
     </row>
@@ -35441,28 +35441,28 @@
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
       <c r="F49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="G49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="H49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="I49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="J49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="K49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="L49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="N49" s="72"/>
     </row>
@@ -35475,28 +35475,28 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="L50" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="N50" s="72"/>
     </row>
@@ -35551,28 +35551,28 @@
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
       <c r="F52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="H52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="I52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="J52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="K52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="L52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="M52" s="72" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="N52" s="72"/>
     </row>
@@ -35585,28 +35585,28 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="H53" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="I53" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="J53" s="72" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="K53" s="72" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="L53" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M53" s="72" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="N53" s="72"/>
     </row>
@@ -35661,28 +35661,28 @@
       <c r="D55" s="72"/>
       <c r="E55" s="72"/>
       <c r="F55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="I55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="J55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="K55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="L55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="M55" s="72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="N55" s="72"/>
     </row>
@@ -35695,28 +35695,28 @@
       <c r="D56" s="72"/>
       <c r="E56" s="72"/>
       <c r="F56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="G56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="H56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="I56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="J56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="K56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="L56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="M56" s="72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="N56" s="72"/>
     </row>
@@ -35771,28 +35771,28 @@
       <c r="D58" s="72"/>
       <c r="E58" s="72"/>
       <c r="F58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="G58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="H58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="I58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="J58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="K58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="L58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="M58" s="72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="N58" s="72"/>
     </row>
@@ -35805,28 +35805,28 @@
       <c r="D59" s="72"/>
       <c r="E59" s="72"/>
       <c r="F59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="G59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="I59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="J59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="K59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="L59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="M59" s="72" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="N59" s="72"/>
     </row>

</xml_diff>